<commit_message>
Buy influence: Further minor updates to events and localisation
</commit_message>
<xml_diff>
--- a/buy_influence/CodeGen.xlsx
+++ b/buy_influence/CodeGen.xlsx
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>Theme</t>
   </si>
@@ -186,7 +186,13 @@
     <t>purchase response</t>
   </si>
   <si>
-    <t>Double-quote:</t>
+    <t>modifier name localisation</t>
+  </si>
+  <si>
+    <t>modifier desc localisation</t>
+  </si>
+  <si>
+    <t>Dbl-quote:</t>
   </si>
 </sst>
 </file>
@@ -234,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -767,11 +773,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -931,17 +948,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -985,6 +992,52 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1288,10 +1341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AM20"/>
+  <dimension ref="B1:AY20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
@@ -1300,17 +1353,22 @@
     <col min="2" max="3" width="9.06640625" style="27"/>
     <col min="4" max="5" width="10" style="27" customWidth="1"/>
     <col min="6" max="10" width="9.06640625" style="27"/>
-    <col min="11" max="16" width="9.06640625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="18" width="9.06640625" style="1"/>
-    <col min="19" max="23" width="9.06640625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="27" width="9.06640625" style="1"/>
-    <col min="28" max="32" width="9.06640625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="9.06640625" style="1"/>
-    <col min="34" max="38" width="9.06640625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="39" max="16384" width="9.06640625" style="1"/>
+    <col min="11" max="16" width="9.06640625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="9.06640625" style="1" collapsed="1"/>
+    <col min="18" max="18" width="9.06640625" style="1"/>
+    <col min="19" max="23" width="9.06640625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="9.06640625" style="1" collapsed="1"/>
+    <col min="25" max="27" width="9.06640625" style="1"/>
+    <col min="28" max="32" width="9.06640625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="9.06640625" style="1" collapsed="1"/>
+    <col min="34" max="38" width="9.06640625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="39" width="9.06640625" style="1" collapsed="1"/>
+    <col min="40" max="44" width="0" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="9.06640625" style="1" collapsed="1"/>
+    <col min="46" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:39" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:51" x14ac:dyDescent="0.45">
       <c r="B1" s="45" t="s">
         <v>19</v>
       </c>
@@ -1354,7 +1412,7 @@
 		}</v>
       </c>
     </row>
-    <row r="2" spans="2:39" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:51" x14ac:dyDescent="0.45">
       <c r="B2" s="47" t="s">
         <v>20</v>
       </c>
@@ -1365,7 +1423,7 @@
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
     </row>
-    <row r="3" spans="2:39" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:51" x14ac:dyDescent="0.45">
       <c r="B3" s="47" t="s">
         <v>23</v>
       </c>
@@ -1380,9 +1438,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:39" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:51" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="49" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C4" s="50" t="str">
         <f>CHAR(34)</f>
@@ -1433,118 +1491,146 @@
 		}</v>
       </c>
     </row>
-    <row r="5" spans="2:39" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="6" spans="2:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="75" t="s">
+    <row r="5" spans="2:51" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="6" spans="2:51" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="75" t="s">
+      <c r="C6" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="75" t="s">
+      <c r="D6" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="75" t="s">
+      <c r="E6" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="79" t="s">
+      <c r="F6" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="75" t="s">
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="78" t="s">
+      <c r="K6" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
-      <c r="N6" s="79"/>
-      <c r="O6" s="79"/>
-      <c r="P6" s="80"/>
-      <c r="Q6" s="75" t="s">
+      <c r="L6" s="75"/>
+      <c r="M6" s="75"/>
+      <c r="N6" s="75"/>
+      <c r="O6" s="75"/>
+      <c r="P6" s="76"/>
+      <c r="Q6" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="R6" s="75" t="s">
+      <c r="R6" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="S6" s="78" t="s">
+      <c r="S6" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="T6" s="79"/>
-      <c r="U6" s="79"/>
-      <c r="V6" s="79"/>
-      <c r="W6" s="79"/>
-      <c r="X6" s="80"/>
-      <c r="Y6" s="78" t="s">
+      <c r="T6" s="75"/>
+      <c r="U6" s="75"/>
+      <c r="V6" s="75"/>
+      <c r="W6" s="75"/>
+      <c r="X6" s="76"/>
+      <c r="Y6" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="Z6" s="79"/>
-      <c r="AA6" s="80"/>
-      <c r="AB6" s="84" t="s">
+      <c r="Z6" s="75"/>
+      <c r="AA6" s="76"/>
+      <c r="AB6" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="AC6" s="85"/>
-      <c r="AD6" s="85"/>
-      <c r="AE6" s="85"/>
-      <c r="AF6" s="85"/>
-      <c r="AG6" s="86"/>
-      <c r="AH6" s="78" t="s">
+      <c r="AC6" s="81"/>
+      <c r="AD6" s="81"/>
+      <c r="AE6" s="81"/>
+      <c r="AF6" s="81"/>
+      <c r="AG6" s="82"/>
+      <c r="AH6" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="AI6" s="79"/>
-      <c r="AJ6" s="79"/>
-      <c r="AK6" s="79"/>
-      <c r="AL6" s="79"/>
-      <c r="AM6" s="80"/>
+      <c r="AI6" s="75"/>
+      <c r="AJ6" s="75"/>
+      <c r="AK6" s="75"/>
+      <c r="AL6" s="75"/>
+      <c r="AM6" s="75"/>
+      <c r="AN6" s="95" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO6" s="96"/>
+      <c r="AP6" s="96"/>
+      <c r="AQ6" s="96"/>
+      <c r="AR6" s="96"/>
+      <c r="AS6" s="102"/>
+      <c r="AT6" s="95" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU6" s="96"/>
+      <c r="AV6" s="96"/>
+      <c r="AW6" s="96"/>
+      <c r="AX6" s="96"/>
+      <c r="AY6" s="97"/>
     </row>
-    <row r="7" spans="2:39" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="76"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="91"/>
-      <c r="M7" s="91"/>
-      <c r="N7" s="91"/>
-      <c r="O7" s="91"/>
-      <c r="P7" s="92"/>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="76"/>
-      <c r="S7" s="81"/>
-      <c r="T7" s="82"/>
-      <c r="U7" s="82"/>
-      <c r="V7" s="82"/>
-      <c r="W7" s="82"/>
-      <c r="X7" s="83"/>
-      <c r="Y7" s="81"/>
-      <c r="Z7" s="82"/>
-      <c r="AA7" s="83"/>
-      <c r="AB7" s="87"/>
-      <c r="AC7" s="88"/>
-      <c r="AD7" s="88"/>
-      <c r="AE7" s="88"/>
-      <c r="AF7" s="88"/>
-      <c r="AG7" s="89"/>
-      <c r="AH7" s="81"/>
-      <c r="AI7" s="82"/>
-      <c r="AJ7" s="82"/>
-      <c r="AK7" s="82"/>
-      <c r="AL7" s="82"/>
-      <c r="AM7" s="83"/>
+    <row r="7" spans="2:51" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="90"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="79"/>
+      <c r="J7" s="90"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="88"/>
+      <c r="Q7" s="90"/>
+      <c r="R7" s="90"/>
+      <c r="S7" s="77"/>
+      <c r="T7" s="78"/>
+      <c r="U7" s="78"/>
+      <c r="V7" s="78"/>
+      <c r="W7" s="78"/>
+      <c r="X7" s="79"/>
+      <c r="Y7" s="77"/>
+      <c r="Z7" s="78"/>
+      <c r="AA7" s="79"/>
+      <c r="AB7" s="83"/>
+      <c r="AC7" s="84"/>
+      <c r="AD7" s="84"/>
+      <c r="AE7" s="84"/>
+      <c r="AF7" s="84"/>
+      <c r="AG7" s="85"/>
+      <c r="AH7" s="77"/>
+      <c r="AI7" s="78"/>
+      <c r="AJ7" s="78"/>
+      <c r="AK7" s="78"/>
+      <c r="AL7" s="78"/>
+      <c r="AM7" s="78"/>
+      <c r="AN7" s="98"/>
+      <c r="AO7" s="93"/>
+      <c r="AP7" s="93"/>
+      <c r="AQ7" s="93"/>
+      <c r="AR7" s="93"/>
+      <c r="AS7" s="103"/>
+      <c r="AT7" s="98"/>
+      <c r="AU7" s="93"/>
+      <c r="AV7" s="93"/>
+      <c r="AW7" s="93"/>
+      <c r="AX7" s="93"/>
+      <c r="AY7" s="99"/>
     </row>
-    <row r="8" spans="2:39" s="3" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
+    <row r="8" spans="2:51" s="3" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="91"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
       <c r="F8" s="31" t="s">
         <v>4</v>
       </c>
@@ -1557,7 +1643,7 @@
       <c r="I8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="77"/>
+      <c r="J8" s="91"/>
       <c r="K8" s="9" t="s">
         <v>29</v>
       </c>
@@ -1576,8 +1662,8 @@
       <c r="P8" s="7">
         <v>5</v>
       </c>
-      <c r="Q8" s="77"/>
-      <c r="R8" s="77"/>
+      <c r="Q8" s="91"/>
+      <c r="R8" s="91"/>
       <c r="S8" s="9">
         <f>L8</f>
         <v>1</v>
@@ -1643,11 +1729,47 @@
       <c r="AL8" s="4">
         <v>5</v>
       </c>
-      <c r="AM8" s="5" t="s">
+      <c r="AM8" s="10" t="s">
         <v>21</v>
       </c>
+      <c r="AN8" s="100">
+        <v>1</v>
+      </c>
+      <c r="AO8" s="94">
+        <v>2</v>
+      </c>
+      <c r="AP8" s="94">
+        <v>3</v>
+      </c>
+      <c r="AQ8" s="94">
+        <v>4</v>
+      </c>
+      <c r="AR8" s="94">
+        <v>5</v>
+      </c>
+      <c r="AS8" s="104" t="s">
+        <v>21</v>
+      </c>
+      <c r="AT8" s="100">
+        <v>1</v>
+      </c>
+      <c r="AU8" s="94">
+        <v>2</v>
+      </c>
+      <c r="AV8" s="94">
+        <v>3</v>
+      </c>
+      <c r="AW8" s="94">
+        <v>4</v>
+      </c>
+      <c r="AX8" s="94">
+        <v>5</v>
+      </c>
+      <c r="AY8" s="101" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="9" spans="2:39" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:51" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B9" s="51" t="s">
         <v>1</v>
       </c>
@@ -1708,7 +1830,7 @@
 			has_modifier = buy_influence_0point5_e_5</v>
       </c>
       <c r="R9" s="24" t="str">
-        <f xml:space="preserve">
+        <f t="shared" ref="R9:R19" si="2" xml:space="preserve">
 newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$L9
 &amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$M9
 &amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$N9
@@ -1722,7 +1844,7 @@
 		remove_modifier = buy_influence_0point5_e_5</v>
       </c>
       <c r="S9" s="64" t="str">
-        <f>newline&amp;newline&amp;L9&amp;" = {"
+        <f t="shared" ref="S9:S19" si="3">newline&amp;newline&amp;L9&amp;" = {"
 &amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
 &amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D9
 &amp;IF($F9&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F9*$J9*L$8,"")
@@ -1738,7 +1860,7 @@
 }</v>
       </c>
       <c r="T9" s="65" t="str">
-        <f>newline&amp;newline&amp;M9&amp;" = {"
+        <f t="shared" ref="T9:T19" si="4">newline&amp;newline&amp;M9&amp;" = {"
 &amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
 &amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D9
 &amp;IF($F9&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F9*$J9*M$8,"")
@@ -1754,7 +1876,7 @@
 }</v>
       </c>
       <c r="U9" s="65" t="str">
-        <f>newline&amp;newline&amp;N9&amp;" = {"
+        <f t="shared" ref="U9:U19" si="5">newline&amp;newline&amp;N9&amp;" = {"
 &amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
 &amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D9
 &amp;IF($F9&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F9*$J9*N$8,"")
@@ -1770,7 +1892,7 @@
 }</v>
       </c>
       <c r="V9" s="65" t="str">
-        <f>newline&amp;newline&amp;O9&amp;" = {"
+        <f t="shared" ref="V9:V19" si="6">newline&amp;newline&amp;O9&amp;" = {"
 &amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
 &amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D9
 &amp;IF($F9&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F9*$J9*O$8,"")
@@ -1786,7 +1908,7 @@
 }</v>
       </c>
       <c r="W9" s="67" t="str">
-        <f>newline&amp;newline&amp;P9&amp;" = {"
+        <f t="shared" ref="W9:W19" si="7">newline&amp;newline&amp;P9&amp;" = {"
 &amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
 &amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D9
 &amp;IF($F9&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F9*$J9*P$8,"")
@@ -1843,7 +1965,7 @@
         <v>buy_influence_0point5_e_response</v>
       </c>
       <c r="AB9" s="64" t="str">
-        <f t="shared" ref="AB9:AB19" si="2">tab &amp; "option = {" &amp; newline &amp;
+        <f t="shared" ref="AB9:AB19" si="8">tab &amp; "option = {" &amp; newline &amp;
 tab &amp; tab &amp; "name = " &amp; $Y9 &amp; newline &amp;
 AB$1 &amp; newline &amp;
 SUBSTITUTE(event_option_add_static_modifier_raw,event_option_add_static_modifier_subst_text,L9) &amp; newline &amp;
@@ -1878,7 +2000,7 @@
 </v>
       </c>
       <c r="AC9" s="65" t="str">
-        <f t="shared" ref="AC9:AC19" si="3">tab &amp; "option = {" &amp; newline &amp;
+        <f t="shared" ref="AC9:AC19" si="9">tab &amp; "option = {" &amp; newline &amp;
 tab &amp; tab &amp; "name = " &amp; $Y9 &amp; newline &amp;
 AC$1 &amp; newline &amp;
 SUBSTITUTE(event_option_add_static_modifier_raw,event_option_add_static_modifier_subst_text,M9) &amp; newline &amp;
@@ -1914,7 +2036,7 @@
 </v>
       </c>
       <c r="AD9" s="65" t="str">
-        <f t="shared" ref="AD9:AD19" si="4">tab &amp; "option = {" &amp; newline &amp;
+        <f t="shared" ref="AD9:AD19" si="10">tab &amp; "option = {" &amp; newline &amp;
 tab &amp; tab &amp; "name = " &amp; $Y9 &amp; newline &amp;
 AD$1 &amp; newline &amp;
 SUBSTITUTE(event_option_add_static_modifier_raw,event_option_add_static_modifier_subst_text,N9) &amp; newline &amp;
@@ -1950,7 +2072,7 @@
 </v>
       </c>
       <c r="AE9" s="65" t="str">
-        <f t="shared" ref="AE9:AE19" si="5">tab &amp; "option = {" &amp; newline &amp;
+        <f t="shared" ref="AE9:AE19" si="11">tab &amp; "option = {" &amp; newline &amp;
 tab &amp; tab &amp; "name = " &amp; $Y9 &amp; newline &amp;
 AE$1 &amp; newline &amp;
 SUBSTITUTE(event_option_add_static_modifier_raw,event_option_add_static_modifier_subst_text,O9) &amp; newline &amp;
@@ -1986,7 +2108,7 @@
 </v>
       </c>
       <c r="AF9" s="65" t="str">
-        <f t="shared" ref="AF9:AF19" si="6">tab &amp; "option = {" &amp; newline &amp;
+        <f t="shared" ref="AF9:AF19" si="12">tab &amp; "option = {" &amp; newline &amp;
 tab &amp; tab &amp; "name = " &amp; $Y9 &amp; newline &amp;
 AF$1 &amp; newline &amp;
 SUBSTITUTE(event_option_add_static_modifier_raw,event_option_add_static_modifier_subst_text,P9) &amp; newline &amp;
@@ -2153,32 +2275,32 @@
 </v>
       </c>
       <c r="AH9" s="12" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; L9 &amp; " = { text = " &amp; $AA9 &amp; " }"</f>
+        <f t="shared" ref="AH9:AH19" si="13">newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; L9 &amp; " = { text = " &amp; $AA9 &amp; " }"</f>
         <v xml:space="preserve">
 				buy_influence_0point5_e_1 = { text = buy_influence_0point5_e_response }</v>
       </c>
       <c r="AI9" s="72" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; M9 &amp; " = { text = " &amp; $AA9 &amp; " }"</f>
+        <f t="shared" ref="AI9:AI19" si="14">newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; M9 &amp; " = { text = " &amp; $AA9 &amp; " }"</f>
         <v xml:space="preserve">
 				buy_influence_0point5_e_2 = { text = buy_influence_0point5_e_response }</v>
       </c>
       <c r="AJ9" s="72" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; N9 &amp; " = { text = " &amp; $AA9 &amp; " }"</f>
+        <f t="shared" ref="AJ9:AJ19" si="15">newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; N9 &amp; " = { text = " &amp; $AA9 &amp; " }"</f>
         <v xml:space="preserve">
 				buy_influence_0point5_e_3 = { text = buy_influence_0point5_e_response }</v>
       </c>
       <c r="AK9" s="72" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; O9 &amp; " = { text = " &amp; $AA9 &amp; " }"</f>
+        <f t="shared" ref="AK9:AK19" si="16">newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; O9 &amp; " = { text = " &amp; $AA9 &amp; " }"</f>
         <v xml:space="preserve">
 				buy_influence_0point5_e_4 = { text = buy_influence_0point5_e_response }</v>
       </c>
       <c r="AL9" s="72" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; P9 &amp; " = { text = " &amp; $AA9 &amp; " }"</f>
+        <f t="shared" ref="AL9:AL19" si="17">newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; P9 &amp; " = { text = " &amp; $AA9 &amp; " }"</f>
         <v xml:space="preserve">
 				buy_influence_0point5_e_5 = { text = buy_influence_0point5_e_response }</v>
       </c>
-      <c r="AM9" s="73" t="str">
-        <f t="shared" ref="AM9:AM19" si="7">CONCATENATE(AH9,AI9,AJ9,AK9,AL9)</f>
+      <c r="AM9" s="92" t="str">
+        <f t="shared" ref="AM9:AM19" si="18">CONCATENATE(AH9,AI9,AJ9,AK9,AL9)</f>
         <v xml:space="preserve">
 				buy_influence_0point5_e_1 = { text = buy_influence_0point5_e_response }
 				buy_influence_0point5_e_2 = { text = buy_influence_0point5_e_response }
@@ -2186,8 +2308,76 @@
 				buy_influence_0point5_e_4 = { text = buy_influence_0point5_e_response }
 				buy_influence_0point5_e_5 = { text = buy_influence_0point5_e_response }</v>
       </c>
+      <c r="AN9" s="14" t="str">
+        <f>newline &amp; space &amp; L9 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y9 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_1_name:0 "$buy_influence_0point5_e_name$"</v>
+      </c>
+      <c r="AO9" s="15" t="str">
+        <f>newline &amp; space &amp; M9 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y9 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_2_name:0 "$buy_influence_0point5_e_name$"</v>
+      </c>
+      <c r="AP9" s="15" t="str">
+        <f>newline &amp; space &amp; N9 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y9 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_3_name:0 "$buy_influence_0point5_e_name$"</v>
+      </c>
+      <c r="AQ9" s="15" t="str">
+        <f>newline &amp; space &amp; O9 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y9 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_4_name:0 "$buy_influence_0point5_e_name$"</v>
+      </c>
+      <c r="AR9" s="15" t="str">
+        <f>newline &amp; space &amp; P9 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y9 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_5_name:0 "$buy_influence_0point5_e_name$"</v>
+      </c>
+      <c r="AS9" s="18" t="str">
+        <f t="shared" ref="AS9:AS19" si="19">CONCATENATE(AN9,AO9,AP9,AQ9,AR9)</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_1_name:0 "$buy_influence_0point5_e_name$"
+ buy_influence_0point5_e_2_name:0 "$buy_influence_0point5_e_name$"
+ buy_influence_0point5_e_3_name:0 "$buy_influence_0point5_e_name$"
+ buy_influence_0point5_e_4_name:0 "$buy_influence_0point5_e_name$"
+ buy_influence_0point5_e_5_name:0 "$buy_influence_0point5_e_name$"</v>
+      </c>
+      <c r="AT9" s="14" t="str">
+        <f>newline &amp; space &amp; L9 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z9 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_1_desc:0 "$buy_influence_0point5_e_desc$"</v>
+      </c>
+      <c r="AU9" s="15" t="str">
+        <f>newline &amp; space &amp; M9 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z9 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_2_desc:0 "$buy_influence_0point5_e_desc$"</v>
+      </c>
+      <c r="AV9" s="15" t="str">
+        <f>newline &amp; space &amp; N9 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z9 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_3_desc:0 "$buy_influence_0point5_e_desc$"</v>
+      </c>
+      <c r="AW9" s="15" t="str">
+        <f>newline &amp; space &amp; O9 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z9 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_4_desc:0 "$buy_influence_0point5_e_desc$"</v>
+      </c>
+      <c r="AX9" s="15" t="str">
+        <f>newline &amp; space &amp; P9 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z9 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_5_desc:0 "$buy_influence_0point5_e_desc$"</v>
+      </c>
+      <c r="AY9" s="16" t="str">
+        <f t="shared" ref="AY9:AY19" si="20">CONCATENATE(AT9,AU9,AV9,AW9,AX9)</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_1_desc:0 "$buy_influence_0point5_e_desc$"
+ buy_influence_0point5_e_2_desc:0 "$buy_influence_0point5_e_desc$"
+ buy_influence_0point5_e_3_desc:0 "$buy_influence_0point5_e_desc$"
+ buy_influence_0point5_e_4_desc:0 "$buy_influence_0point5_e_desc$"
+ buy_influence_0point5_e_5_desc:0 "$buy_influence_0point5_e_desc$"</v>
+      </c>
     </row>
-    <row r="10" spans="2:39" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:51" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B10" s="55" t="s">
         <v>1</v>
       </c>
@@ -2198,7 +2388,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="43">
-        <f t="shared" ref="E10:E19" si="8">MIN(25,10*D10)</f>
+        <f t="shared" ref="E10:E19" si="21">MIN(25,10*D10)</f>
         <v>10</v>
       </c>
       <c r="F10" s="57">
@@ -2211,11 +2401,11 @@
         <v>1</v>
       </c>
       <c r="K10" s="14" t="str">
-        <f t="shared" ref="K10:K19" si="9">"buy_influence_"&amp;ROUNDDOWN($D10,0)&amp;"point"&amp;(ROUNDDOWN($D10*10,0)-(ROUNDDOWN($D10,0)*10))&amp;"_"&amp;$C10</f>
+        <f t="shared" ref="K10:K19" si="22">"buy_influence_"&amp;ROUNDDOWN($D10,0)&amp;"point"&amp;(ROUNDDOWN($D10*10,0)-(ROUNDDOWN($D10,0)*10))&amp;"_"&amp;$C10</f>
         <v>buy_influence_1point0_e</v>
       </c>
       <c r="L10" s="36" t="str">
-        <f t="shared" ref="L10:L19" si="10">$K10&amp;"_"&amp;L$8</f>
+        <f t="shared" ref="L10:L19" si="23">$K10&amp;"_"&amp;L$8</f>
         <v>buy_influence_1point0_e_1</v>
       </c>
       <c r="M10" s="37" t="str">
@@ -2244,12 +2434,7 @@
 			has_modifier = buy_influence_1point0_e_5</v>
       </c>
       <c r="R10" s="25" t="str">
-        <f xml:space="preserve">
-newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$L10
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$M10
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$N10
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$O10
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$P10</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">
 		remove_modifier = buy_influence_1point0_e_1
 		remove_modifier = buy_influence_1point0_e_2
@@ -2258,14 +2443,7 @@
 		remove_modifier = buy_influence_1point0_e_5</v>
       </c>
       <c r="S10" s="14" t="str">
-        <f>newline&amp;newline&amp;L10&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D10
-&amp;IF($F10&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F10*$J10*L$8,"")
-&amp;IF($G10&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G10*$J10*L$8,"")
-&amp;IF($H10&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H10*$J10*L$8,"")
-&amp;IF($I10&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I10*$J10*L$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">
 buy_influence_1point0_e_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -2274,14 +2452,7 @@
 }</v>
       </c>
       <c r="T10" s="15" t="str">
-        <f>newline&amp;newline&amp;M10&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D10
-&amp;IF($F10&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F10*$J10*M$8,"")
-&amp;IF($G10&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G10*$J10*M$8,"")
-&amp;IF($H10&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H10*$J10*M$8,"")
-&amp;IF($I10&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I10*$J10*M$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">
 buy_influence_1point0_e_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -2290,14 +2461,7 @@
 }</v>
       </c>
       <c r="U10" s="15" t="str">
-        <f>newline&amp;newline&amp;N10&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D10
-&amp;IF($F10&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F10*$J10*N$8,"")
-&amp;IF($G10&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G10*$J10*N$8,"")
-&amp;IF($H10&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H10*$J10*N$8,"")
-&amp;IF($I10&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I10*$J10*N$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">
 buy_influence_1point0_e_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -2306,14 +2470,7 @@
 }</v>
       </c>
       <c r="V10" s="15" t="str">
-        <f>newline&amp;newline&amp;O10&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D10
-&amp;IF($F10&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F10*$J10*O$8,"")
-&amp;IF($G10&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G10*$J10*O$8,"")
-&amp;IF($H10&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H10*$J10*O$8,"")
-&amp;IF($I10&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I10*$J10*O$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">
 buy_influence_1point0_e_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -2322,14 +2479,7 @@
 }</v>
       </c>
       <c r="W10" s="18" t="str">
-        <f>newline&amp;newline&amp;P10&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D10
-&amp;IF($F10&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F10*$J10*P$8,"")
-&amp;IF($G10&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G10*$J10*P$8,"")
-&amp;IF($H10&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H10*$J10*P$8,"")
-&amp;IF($I10&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I10*$J10*P$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">
 buy_influence_1point0_e_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -2338,7 +2488,7 @@
 }</v>
       </c>
       <c r="X10" s="16" t="str">
-        <f t="shared" ref="X10:X19" si="11">CONCATENATE(S10,T10,U10,V10,W10)</f>
+        <f t="shared" ref="X10:X19" si="24">CONCATENATE(S10,T10,U10,V10,W10)</f>
         <v xml:space="preserve">
 buy_influence_1point0_e_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -2367,19 +2517,19 @@
 }</v>
       </c>
       <c r="Y10" s="25" t="str">
-        <f t="shared" ref="Y10:Y19" si="12">$K10&amp;"_name"</f>
+        <f t="shared" ref="Y10:Y19" si="25">$K10&amp;"_name"</f>
         <v>buy_influence_1point0_e_name</v>
       </c>
       <c r="Z10" s="15" t="str">
-        <f t="shared" ref="Z10:Z19" si="13">$K10&amp;"_desc"</f>
+        <f t="shared" ref="Z10:Z19" si="26">$K10&amp;"_desc"</f>
         <v>buy_influence_1point0_e_desc</v>
       </c>
       <c r="AA10" s="70" t="str">
-        <f t="shared" ref="AA10:AA19" si="14">$K10&amp;"_response"</f>
+        <f t="shared" ref="AA10:AA19" si="27">$K10&amp;"_response"</f>
         <v>buy_influence_1point0_e_response</v>
       </c>
       <c r="AB10" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_e_name
 		trigger = {
@@ -2408,7 +2558,7 @@
 </v>
       </c>
       <c r="AC10" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_e_name
 		trigger = {
@@ -2438,7 +2588,7 @@
 </v>
       </c>
       <c r="AD10" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_e_name
 		trigger = {
@@ -2468,7 +2618,7 @@
 </v>
       </c>
       <c r="AE10" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_e_name
 		trigger = {
@@ -2498,7 +2648,7 @@
 </v>
       </c>
       <c r="AF10" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_e_name
 		trigger = {
@@ -2527,7 +2677,7 @@
 </v>
       </c>
       <c r="AG10" s="16" t="str">
-        <f t="shared" ref="AG10:AG19" si="15">CONCATENATE(AB10,AC10,AD10,AE10,AF10)</f>
+        <f t="shared" ref="AG10:AG19" si="28">CONCATENATE(AB10,AC10,AD10,AE10,AF10)</f>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_e_name
 		trigger = {
@@ -2659,32 +2809,32 @@
 </v>
       </c>
       <c r="AH10" s="14" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; L10 &amp; " = { text = " &amp; $AA10 &amp; " }"</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">
 				buy_influence_1point0_e_1 = { text = buy_influence_1point0_e_response }</v>
       </c>
       <c r="AI10" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; M10 &amp; " = { text = " &amp; $AA10 &amp; " }"</f>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">
 				buy_influence_1point0_e_2 = { text = buy_influence_1point0_e_response }</v>
       </c>
       <c r="AJ10" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; N10 &amp; " = { text = " &amp; $AA10 &amp; " }"</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">
 				buy_influence_1point0_e_3 = { text = buy_influence_1point0_e_response }</v>
       </c>
       <c r="AK10" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; O10 &amp; " = { text = " &amp; $AA10 &amp; " }"</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">
 				buy_influence_1point0_e_4 = { text = buy_influence_1point0_e_response }</v>
       </c>
       <c r="AL10" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; P10 &amp; " = { text = " &amp; $AA10 &amp; " }"</f>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">
 				buy_influence_1point0_e_5 = { text = buy_influence_1point0_e_response }</v>
       </c>
-      <c r="AM10" s="16" t="str">
-        <f t="shared" si="7"/>
+      <c r="AM10" s="18" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_1point0_e_1 = { text = buy_influence_1point0_e_response }
 				buy_influence_1point0_e_2 = { text = buy_influence_1point0_e_response }
@@ -2692,8 +2842,76 @@
 				buy_influence_1point0_e_4 = { text = buy_influence_1point0_e_response }
 				buy_influence_1point0_e_5 = { text = buy_influence_1point0_e_response }</v>
       </c>
+      <c r="AN10" s="14" t="str">
+        <f>newline &amp; space &amp; L10 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y10 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_1_name:0 "$buy_influence_1point0_e_name$"</v>
+      </c>
+      <c r="AO10" s="15" t="str">
+        <f>newline &amp; space &amp; M10 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y10 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_2_name:0 "$buy_influence_1point0_e_name$"</v>
+      </c>
+      <c r="AP10" s="15" t="str">
+        <f>newline &amp; space &amp; N10 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y10 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_3_name:0 "$buy_influence_1point0_e_name$"</v>
+      </c>
+      <c r="AQ10" s="15" t="str">
+        <f>newline &amp; space &amp; O10 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y10 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_4_name:0 "$buy_influence_1point0_e_name$"</v>
+      </c>
+      <c r="AR10" s="15" t="str">
+        <f>newline &amp; space &amp; P10 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y10 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_5_name:0 "$buy_influence_1point0_e_name$"</v>
+      </c>
+      <c r="AS10" s="18" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_1_name:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_e_2_name:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_e_3_name:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_e_4_name:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_e_5_name:0 "$buy_influence_1point0_e_name$"</v>
+      </c>
+      <c r="AT10" s="14" t="str">
+        <f>newline &amp; space &amp; L10 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z10 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_1_desc:0 "$buy_influence_1point0_e_desc$"</v>
+      </c>
+      <c r="AU10" s="15" t="str">
+        <f>newline &amp; space &amp; M10 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z10 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_2_desc:0 "$buy_influence_1point0_e_desc$"</v>
+      </c>
+      <c r="AV10" s="15" t="str">
+        <f>newline &amp; space &amp; N10 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z10 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_3_desc:0 "$buy_influence_1point0_e_desc$"</v>
+      </c>
+      <c r="AW10" s="15" t="str">
+        <f>newline &amp; space &amp; O10 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z10 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_4_desc:0 "$buy_influence_1point0_e_desc$"</v>
+      </c>
+      <c r="AX10" s="15" t="str">
+        <f>newline &amp; space &amp; P10 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z10 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_5_desc:0 "$buy_influence_1point0_e_desc$"</v>
+      </c>
+      <c r="AY10" s="16" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_1_desc:0 "$buy_influence_1point0_e_desc$"
+ buy_influence_1point0_e_2_desc:0 "$buy_influence_1point0_e_desc$"
+ buy_influence_1point0_e_3_desc:0 "$buy_influence_1point0_e_desc$"
+ buy_influence_1point0_e_4_desc:0 "$buy_influence_1point0_e_desc$"
+ buy_influence_1point0_e_5_desc:0 "$buy_influence_1point0_e_desc$"</v>
+      </c>
     </row>
-    <row r="11" spans="2:39" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:51" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B11" s="55" t="s">
         <v>8</v>
       </c>
@@ -2704,7 +2922,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="F11" s="57">
@@ -2719,11 +2937,11 @@
         <v>1</v>
       </c>
       <c r="K11" s="14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>buy_influence_1point0_em</v>
       </c>
       <c r="L11" s="36" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>buy_influence_1point0_em_1</v>
       </c>
       <c r="M11" s="37" t="str">
@@ -2752,12 +2970,7 @@
 			has_modifier = buy_influence_1point0_em_5</v>
       </c>
       <c r="R11" s="25" t="str">
-        <f xml:space="preserve">
-newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$L11
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$M11
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$N11
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$O11
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$P11</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">
 		remove_modifier = buy_influence_1point0_em_1
 		remove_modifier = buy_influence_1point0_em_2
@@ -2766,14 +2979,7 @@
 		remove_modifier = buy_influence_1point0_em_5</v>
       </c>
       <c r="S11" s="14" t="str">
-        <f>newline&amp;newline&amp;L11&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D11
-&amp;IF($F11&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F11*$J11*L$8,"")
-&amp;IF($G11&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G11*$J11*L$8,"")
-&amp;IF($H11&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H11*$J11*L$8,"")
-&amp;IF($I11&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I11*$J11*L$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">
 buy_influence_1point0_em_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -2783,14 +2989,7 @@
 }</v>
       </c>
       <c r="T11" s="15" t="str">
-        <f>newline&amp;newline&amp;M11&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D11
-&amp;IF($F11&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F11*$J11*M$8,"")
-&amp;IF($G11&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G11*$J11*M$8,"")
-&amp;IF($H11&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H11*$J11*M$8,"")
-&amp;IF($I11&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I11*$J11*M$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">
 buy_influence_1point0_em_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -2800,14 +2999,7 @@
 }</v>
       </c>
       <c r="U11" s="15" t="str">
-        <f>newline&amp;newline&amp;N11&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D11
-&amp;IF($F11&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F11*$J11*N$8,"")
-&amp;IF($G11&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G11*$J11*N$8,"")
-&amp;IF($H11&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H11*$J11*N$8,"")
-&amp;IF($I11&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I11*$J11*N$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">
 buy_influence_1point0_em_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -2817,14 +3009,7 @@
 }</v>
       </c>
       <c r="V11" s="15" t="str">
-        <f>newline&amp;newline&amp;O11&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D11
-&amp;IF($F11&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F11*$J11*O$8,"")
-&amp;IF($G11&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G11*$J11*O$8,"")
-&amp;IF($H11&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H11*$J11*O$8,"")
-&amp;IF($I11&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I11*$J11*O$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">
 buy_influence_1point0_em_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -2834,14 +3019,7 @@
 }</v>
       </c>
       <c r="W11" s="18" t="str">
-        <f>newline&amp;newline&amp;P11&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D11
-&amp;IF($F11&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F11*$J11*P$8,"")
-&amp;IF($G11&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G11*$J11*P$8,"")
-&amp;IF($H11&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H11*$J11*P$8,"")
-&amp;IF($I11&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I11*$J11*P$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">
 buy_influence_1point0_em_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -2851,7 +3029,7 @@
 }</v>
       </c>
       <c r="X11" s="16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
 buy_influence_1point0_em_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -2885,19 +3063,19 @@
 }</v>
       </c>
       <c r="Y11" s="25" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>buy_influence_1point0_em_name</v>
       </c>
       <c r="Z11" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>buy_influence_1point0_em_desc</v>
       </c>
       <c r="AA11" s="70" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_1point0_em_response</v>
       </c>
       <c r="AB11" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_em_name
 		trigger = {
@@ -2926,7 +3104,7 @@
 </v>
       </c>
       <c r="AC11" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_em_name
 		trigger = {
@@ -2956,7 +3134,7 @@
 </v>
       </c>
       <c r="AD11" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_em_name
 		trigger = {
@@ -2986,7 +3164,7 @@
 </v>
       </c>
       <c r="AE11" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_em_name
 		trigger = {
@@ -3016,7 +3194,7 @@
 </v>
       </c>
       <c r="AF11" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_em_name
 		trigger = {
@@ -3045,7 +3223,7 @@
 </v>
       </c>
       <c r="AG11" s="16" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_em_name
 		trigger = {
@@ -3177,32 +3355,32 @@
 </v>
       </c>
       <c r="AH11" s="14" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; L11 &amp; " = { text = " &amp; $AA11 &amp; " }"</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">
 				buy_influence_1point0_em_1 = { text = buy_influence_1point0_em_response }</v>
       </c>
       <c r="AI11" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; M11 &amp; " = { text = " &amp; $AA11 &amp; " }"</f>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">
 				buy_influence_1point0_em_2 = { text = buy_influence_1point0_em_response }</v>
       </c>
       <c r="AJ11" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; N11 &amp; " = { text = " &amp; $AA11 &amp; " }"</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">
 				buy_influence_1point0_em_3 = { text = buy_influence_1point0_em_response }</v>
       </c>
       <c r="AK11" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; O11 &amp; " = { text = " &amp; $AA11 &amp; " }"</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">
 				buy_influence_1point0_em_4 = { text = buy_influence_1point0_em_response }</v>
       </c>
       <c r="AL11" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; P11 &amp; " = { text = " &amp; $AA11 &amp; " }"</f>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">
 				buy_influence_1point0_em_5 = { text = buy_influence_1point0_em_response }</v>
       </c>
-      <c r="AM11" s="16" t="str">
-        <f t="shared" si="7"/>
+      <c r="AM11" s="18" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_1point0_em_1 = { text = buy_influence_1point0_em_response }
 				buy_influence_1point0_em_2 = { text = buy_influence_1point0_em_response }
@@ -3210,8 +3388,76 @@
 				buy_influence_1point0_em_4 = { text = buy_influence_1point0_em_response }
 				buy_influence_1point0_em_5 = { text = buy_influence_1point0_em_response }</v>
       </c>
+      <c r="AN11" s="14" t="str">
+        <f>newline &amp; space &amp; L11 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y11 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_1_name:0 "$buy_influence_1point0_em_name$"</v>
+      </c>
+      <c r="AO11" s="15" t="str">
+        <f>newline &amp; space &amp; M11 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y11 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_2_name:0 "$buy_influence_1point0_em_name$"</v>
+      </c>
+      <c r="AP11" s="15" t="str">
+        <f>newline &amp; space &amp; N11 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y11 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_3_name:0 "$buy_influence_1point0_em_name$"</v>
+      </c>
+      <c r="AQ11" s="15" t="str">
+        <f>newline &amp; space &amp; O11 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y11 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_4_name:0 "$buy_influence_1point0_em_name$"</v>
+      </c>
+      <c r="AR11" s="15" t="str">
+        <f>newline &amp; space &amp; P11 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y11 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_5_name:0 "$buy_influence_1point0_em_name$"</v>
+      </c>
+      <c r="AS11" s="18" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_1_name:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point0_em_2_name:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point0_em_3_name:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point0_em_4_name:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point0_em_5_name:0 "$buy_influence_1point0_em_name$"</v>
+      </c>
+      <c r="AT11" s="14" t="str">
+        <f>newline &amp; space &amp; L11 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z11 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_1_desc:0 "$buy_influence_1point0_em_desc$"</v>
+      </c>
+      <c r="AU11" s="15" t="str">
+        <f>newline &amp; space &amp; M11 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z11 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_2_desc:0 "$buy_influence_1point0_em_desc$"</v>
+      </c>
+      <c r="AV11" s="15" t="str">
+        <f>newline &amp; space &amp; N11 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z11 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_3_desc:0 "$buy_influence_1point0_em_desc$"</v>
+      </c>
+      <c r="AW11" s="15" t="str">
+        <f>newline &amp; space &amp; O11 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z11 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_4_desc:0 "$buy_influence_1point0_em_desc$"</v>
+      </c>
+      <c r="AX11" s="15" t="str">
+        <f>newline &amp; space &amp; P11 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z11 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_5_desc:0 "$buy_influence_1point0_em_desc$"</v>
+      </c>
+      <c r="AY11" s="16" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_1_desc:0 "$buy_influence_1point0_em_desc$"
+ buy_influence_1point0_em_2_desc:0 "$buy_influence_1point0_em_desc$"
+ buy_influence_1point0_em_3_desc:0 "$buy_influence_1point0_em_desc$"
+ buy_influence_1point0_em_4_desc:0 "$buy_influence_1point0_em_desc$"
+ buy_influence_1point0_em_5_desc:0 "$buy_influence_1point0_em_desc$"</v>
+      </c>
     </row>
-    <row r="12" spans="2:39" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:51" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B12" s="55" t="s">
         <v>8</v>
       </c>
@@ -3222,7 +3468,7 @@
         <v>1.5</v>
       </c>
       <c r="E12" s="43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>15</v>
       </c>
       <c r="F12" s="57">
@@ -3237,11 +3483,11 @@
         <v>1</v>
       </c>
       <c r="K12" s="14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>buy_influence_1point5_em</v>
       </c>
       <c r="L12" s="36" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>buy_influence_1point5_em_1</v>
       </c>
       <c r="M12" s="37" t="str">
@@ -3270,12 +3516,7 @@
 			has_modifier = buy_influence_1point5_em_5</v>
       </c>
       <c r="R12" s="25" t="str">
-        <f xml:space="preserve">
-newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$L12
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$M12
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$N12
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$O12
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$P12</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">
 		remove_modifier = buy_influence_1point5_em_1
 		remove_modifier = buy_influence_1point5_em_2
@@ -3284,14 +3525,7 @@
 		remove_modifier = buy_influence_1point5_em_5</v>
       </c>
       <c r="S12" s="14" t="str">
-        <f>newline&amp;newline&amp;L12&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D12
-&amp;IF($F12&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F12*$J12*L$8,"")
-&amp;IF($G12&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G12*$J12*L$8,"")
-&amp;IF($H12&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H12*$J12*L$8,"")
-&amp;IF($I12&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I12*$J12*L$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">
 buy_influence_1point5_em_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -3301,14 +3535,7 @@
 }</v>
       </c>
       <c r="T12" s="15" t="str">
-        <f>newline&amp;newline&amp;M12&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D12
-&amp;IF($F12&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F12*$J12*M$8,"")
-&amp;IF($G12&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G12*$J12*M$8,"")
-&amp;IF($H12&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H12*$J12*M$8,"")
-&amp;IF($I12&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I12*$J12*M$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">
 buy_influence_1point5_em_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -3318,14 +3545,7 @@
 }</v>
       </c>
       <c r="U12" s="15" t="str">
-        <f>newline&amp;newline&amp;N12&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D12
-&amp;IF($F12&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F12*$J12*N$8,"")
-&amp;IF($G12&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G12*$J12*N$8,"")
-&amp;IF($H12&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H12*$J12*N$8,"")
-&amp;IF($I12&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I12*$J12*N$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">
 buy_influence_1point5_em_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -3335,14 +3555,7 @@
 }</v>
       </c>
       <c r="V12" s="15" t="str">
-        <f>newline&amp;newline&amp;O12&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D12
-&amp;IF($F12&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F12*$J12*O$8,"")
-&amp;IF($G12&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G12*$J12*O$8,"")
-&amp;IF($H12&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H12*$J12*O$8,"")
-&amp;IF($I12&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I12*$J12*O$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">
 buy_influence_1point5_em_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -3352,14 +3565,7 @@
 }</v>
       </c>
       <c r="W12" s="18" t="str">
-        <f>newline&amp;newline&amp;P12&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D12
-&amp;IF($F12&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F12*$J12*P$8,"")
-&amp;IF($G12&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G12*$J12*P$8,"")
-&amp;IF($H12&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H12*$J12*P$8,"")
-&amp;IF($I12&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I12*$J12*P$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">
 buy_influence_1point5_em_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -3369,7 +3575,7 @@
 }</v>
       </c>
       <c r="X12" s="16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
 buy_influence_1point5_em_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -3403,19 +3609,19 @@
 }</v>
       </c>
       <c r="Y12" s="25" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>buy_influence_1point5_em_name</v>
       </c>
       <c r="Z12" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>buy_influence_1point5_em_desc</v>
       </c>
       <c r="AA12" s="70" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_1point5_em_response</v>
       </c>
       <c r="AB12" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point5_em_name
 		trigger = {
@@ -3444,7 +3650,7 @@
 </v>
       </c>
       <c r="AC12" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point5_em_name
 		trigger = {
@@ -3474,7 +3680,7 @@
 </v>
       </c>
       <c r="AD12" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point5_em_name
 		trigger = {
@@ -3504,7 +3710,7 @@
 </v>
       </c>
       <c r="AE12" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point5_em_name
 		trigger = {
@@ -3534,7 +3740,7 @@
 </v>
       </c>
       <c r="AF12" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point5_em_name
 		trigger = {
@@ -3563,7 +3769,7 @@
 </v>
       </c>
       <c r="AG12" s="16" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point5_em_name
 		trigger = {
@@ -3695,32 +3901,32 @@
 </v>
       </c>
       <c r="AH12" s="14" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; L12 &amp; " = { text = " &amp; $AA12 &amp; " }"</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">
 				buy_influence_1point5_em_1 = { text = buy_influence_1point5_em_response }</v>
       </c>
       <c r="AI12" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; M12 &amp; " = { text = " &amp; $AA12 &amp; " }"</f>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">
 				buy_influence_1point5_em_2 = { text = buy_influence_1point5_em_response }</v>
       </c>
       <c r="AJ12" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; N12 &amp; " = { text = " &amp; $AA12 &amp; " }"</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">
 				buy_influence_1point5_em_3 = { text = buy_influence_1point5_em_response }</v>
       </c>
       <c r="AK12" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; O12 &amp; " = { text = " &amp; $AA12 &amp; " }"</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">
 				buy_influence_1point5_em_4 = { text = buy_influence_1point5_em_response }</v>
       </c>
       <c r="AL12" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; P12 &amp; " = { text = " &amp; $AA12 &amp; " }"</f>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">
 				buy_influence_1point5_em_5 = { text = buy_influence_1point5_em_response }</v>
       </c>
-      <c r="AM12" s="16" t="str">
-        <f t="shared" si="7"/>
+      <c r="AM12" s="18" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_1point5_em_1 = { text = buy_influence_1point5_em_response }
 				buy_influence_1point5_em_2 = { text = buy_influence_1point5_em_response }
@@ -3728,8 +3934,76 @@
 				buy_influence_1point5_em_4 = { text = buy_influence_1point5_em_response }
 				buy_influence_1point5_em_5 = { text = buy_influence_1point5_em_response }</v>
       </c>
+      <c r="AN12" s="14" t="str">
+        <f>newline &amp; space &amp; L12 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y12 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_1_name:0 "$buy_influence_1point5_em_name$"</v>
+      </c>
+      <c r="AO12" s="15" t="str">
+        <f>newline &amp; space &amp; M12 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y12 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_2_name:0 "$buy_influence_1point5_em_name$"</v>
+      </c>
+      <c r="AP12" s="15" t="str">
+        <f>newline &amp; space &amp; N12 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y12 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_3_name:0 "$buy_influence_1point5_em_name$"</v>
+      </c>
+      <c r="AQ12" s="15" t="str">
+        <f>newline &amp; space &amp; O12 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y12 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_4_name:0 "$buy_influence_1point5_em_name$"</v>
+      </c>
+      <c r="AR12" s="15" t="str">
+        <f>newline &amp; space &amp; P12 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y12 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_5_name:0 "$buy_influence_1point5_em_name$"</v>
+      </c>
+      <c r="AS12" s="18" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_1_name:0 "$buy_influence_1point5_em_name$"
+ buy_influence_1point5_em_2_name:0 "$buy_influence_1point5_em_name$"
+ buy_influence_1point5_em_3_name:0 "$buy_influence_1point5_em_name$"
+ buy_influence_1point5_em_4_name:0 "$buy_influence_1point5_em_name$"
+ buy_influence_1point5_em_5_name:0 "$buy_influence_1point5_em_name$"</v>
+      </c>
+      <c r="AT12" s="14" t="str">
+        <f>newline &amp; space &amp; L12 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z12 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_1_desc:0 "$buy_influence_1point5_em_desc$"</v>
+      </c>
+      <c r="AU12" s="15" t="str">
+        <f>newline &amp; space &amp; M12 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z12 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_2_desc:0 "$buy_influence_1point5_em_desc$"</v>
+      </c>
+      <c r="AV12" s="15" t="str">
+        <f>newline &amp; space &amp; N12 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z12 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_3_desc:0 "$buy_influence_1point5_em_desc$"</v>
+      </c>
+      <c r="AW12" s="15" t="str">
+        <f>newline &amp; space &amp; O12 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z12 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_4_desc:0 "$buy_influence_1point5_em_desc$"</v>
+      </c>
+      <c r="AX12" s="15" t="str">
+        <f>newline &amp; space &amp; P12 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z12 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_5_desc:0 "$buy_influence_1point5_em_desc$"</v>
+      </c>
+      <c r="AY12" s="16" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_1_desc:0 "$buy_influence_1point5_em_desc$"
+ buy_influence_1point5_em_2_desc:0 "$buy_influence_1point5_em_desc$"
+ buy_influence_1point5_em_3_desc:0 "$buy_influence_1point5_em_desc$"
+ buy_influence_1point5_em_4_desc:0 "$buy_influence_1point5_em_desc$"
+ buy_influence_1point5_em_5_desc:0 "$buy_influence_1point5_em_desc$"</v>
+      </c>
     </row>
-    <row r="13" spans="2:39" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:51" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B13" s="55" t="s">
         <v>8</v>
       </c>
@@ -3740,7 +4014,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>20</v>
       </c>
       <c r="F13" s="57">
@@ -3755,11 +4029,11 @@
         <v>1</v>
       </c>
       <c r="K13" s="14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>buy_influence_2point0_em</v>
       </c>
       <c r="L13" s="36" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>buy_influence_2point0_em_1</v>
       </c>
       <c r="M13" s="37" t="str">
@@ -3788,12 +4062,7 @@
 			has_modifier = buy_influence_2point0_em_5</v>
       </c>
       <c r="R13" s="25" t="str">
-        <f xml:space="preserve">
-newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$L13
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$M13
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$N13
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$O13
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$P13</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">
 		remove_modifier = buy_influence_2point0_em_1
 		remove_modifier = buy_influence_2point0_em_2
@@ -3802,14 +4071,7 @@
 		remove_modifier = buy_influence_2point0_em_5</v>
       </c>
       <c r="S13" s="14" t="str">
-        <f>newline&amp;newline&amp;L13&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D13
-&amp;IF($F13&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F13*$J13*L$8,"")
-&amp;IF($G13&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G13*$J13*L$8,"")
-&amp;IF($H13&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H13*$J13*L$8,"")
-&amp;IF($I13&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I13*$J13*L$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">
 buy_influence_2point0_em_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -3819,14 +4081,7 @@
 }</v>
       </c>
       <c r="T13" s="15" t="str">
-        <f>newline&amp;newline&amp;M13&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D13
-&amp;IF($F13&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F13*$J13*M$8,"")
-&amp;IF($G13&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G13*$J13*M$8,"")
-&amp;IF($H13&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H13*$J13*M$8,"")
-&amp;IF($I13&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I13*$J13*M$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">
 buy_influence_2point0_em_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -3836,14 +4091,7 @@
 }</v>
       </c>
       <c r="U13" s="15" t="str">
-        <f>newline&amp;newline&amp;N13&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D13
-&amp;IF($F13&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F13*$J13*N$8,"")
-&amp;IF($G13&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G13*$J13*N$8,"")
-&amp;IF($H13&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H13*$J13*N$8,"")
-&amp;IF($I13&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I13*$J13*N$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">
 buy_influence_2point0_em_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -3853,14 +4101,7 @@
 }</v>
       </c>
       <c r="V13" s="15" t="str">
-        <f>newline&amp;newline&amp;O13&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D13
-&amp;IF($F13&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F13*$J13*O$8,"")
-&amp;IF($G13&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G13*$J13*O$8,"")
-&amp;IF($H13&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H13*$J13*O$8,"")
-&amp;IF($I13&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I13*$J13*O$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">
 buy_influence_2point0_em_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -3870,14 +4111,7 @@
 }</v>
       </c>
       <c r="W13" s="18" t="str">
-        <f>newline&amp;newline&amp;P13&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D13
-&amp;IF($F13&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F13*$J13*P$8,"")
-&amp;IF($G13&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G13*$J13*P$8,"")
-&amp;IF($H13&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H13*$J13*P$8,"")
-&amp;IF($I13&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I13*$J13*P$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">
 buy_influence_2point0_em_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -3887,7 +4121,7 @@
 }</v>
       </c>
       <c r="X13" s="16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
 buy_influence_2point0_em_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -3921,19 +4155,19 @@
 }</v>
       </c>
       <c r="Y13" s="25" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>buy_influence_2point0_em_name</v>
       </c>
       <c r="Z13" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>buy_influence_2point0_em_desc</v>
       </c>
       <c r="AA13" s="70" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_2point0_em_response</v>
       </c>
       <c r="AB13" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_em_name
 		trigger = {
@@ -3962,7 +4196,7 @@
 </v>
       </c>
       <c r="AC13" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_em_name
 		trigger = {
@@ -3992,7 +4226,7 @@
 </v>
       </c>
       <c r="AD13" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_em_name
 		trigger = {
@@ -4022,7 +4256,7 @@
 </v>
       </c>
       <c r="AE13" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_em_name
 		trigger = {
@@ -4052,7 +4286,7 @@
 </v>
       </c>
       <c r="AF13" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_em_name
 		trigger = {
@@ -4081,7 +4315,7 @@
 </v>
       </c>
       <c r="AG13" s="16" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_em_name
 		trigger = {
@@ -4213,32 +4447,32 @@
 </v>
       </c>
       <c r="AH13" s="14" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; L13 &amp; " = { text = " &amp; $AA13 &amp; " }"</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">
 				buy_influence_2point0_em_1 = { text = buy_influence_2point0_em_response }</v>
       </c>
       <c r="AI13" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; M13 &amp; " = { text = " &amp; $AA13 &amp; " }"</f>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">
 				buy_influence_2point0_em_2 = { text = buy_influence_2point0_em_response }</v>
       </c>
       <c r="AJ13" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; N13 &amp; " = { text = " &amp; $AA13 &amp; " }"</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">
 				buy_influence_2point0_em_3 = { text = buy_influence_2point0_em_response }</v>
       </c>
       <c r="AK13" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; O13 &amp; " = { text = " &amp; $AA13 &amp; " }"</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">
 				buy_influence_2point0_em_4 = { text = buy_influence_2point0_em_response }</v>
       </c>
       <c r="AL13" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; P13 &amp; " = { text = " &amp; $AA13 &amp; " }"</f>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">
 				buy_influence_2point0_em_5 = { text = buy_influence_2point0_em_response }</v>
       </c>
-      <c r="AM13" s="16" t="str">
-        <f t="shared" si="7"/>
+      <c r="AM13" s="18" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_2point0_em_1 = { text = buy_influence_2point0_em_response }
 				buy_influence_2point0_em_2 = { text = buy_influence_2point0_em_response }
@@ -4246,8 +4480,76 @@
 				buy_influence_2point0_em_4 = { text = buy_influence_2point0_em_response }
 				buy_influence_2point0_em_5 = { text = buy_influence_2point0_em_response }</v>
       </c>
+      <c r="AN13" s="14" t="str">
+        <f>newline &amp; space &amp; L13 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y13 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_1_name:0 "$buy_influence_2point0_em_name$"</v>
+      </c>
+      <c r="AO13" s="15" t="str">
+        <f>newline &amp; space &amp; M13 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y13 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_2_name:0 "$buy_influence_2point0_em_name$"</v>
+      </c>
+      <c r="AP13" s="15" t="str">
+        <f>newline &amp; space &amp; N13 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y13 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_3_name:0 "$buy_influence_2point0_em_name$"</v>
+      </c>
+      <c r="AQ13" s="15" t="str">
+        <f>newline &amp; space &amp; O13 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y13 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_4_name:0 "$buy_influence_2point0_em_name$"</v>
+      </c>
+      <c r="AR13" s="15" t="str">
+        <f>newline &amp; space &amp; P13 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y13 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_5_name:0 "$buy_influence_2point0_em_name$"</v>
+      </c>
+      <c r="AS13" s="18" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_1_name:0 "$buy_influence_2point0_em_name$"
+ buy_influence_2point0_em_2_name:0 "$buy_influence_2point0_em_name$"
+ buy_influence_2point0_em_3_name:0 "$buy_influence_2point0_em_name$"
+ buy_influence_2point0_em_4_name:0 "$buy_influence_2point0_em_name$"
+ buy_influence_2point0_em_5_name:0 "$buy_influence_2point0_em_name$"</v>
+      </c>
+      <c r="AT13" s="14" t="str">
+        <f>newline &amp; space &amp; L13 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z13 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_1_desc:0 "$buy_influence_2point0_em_desc$"</v>
+      </c>
+      <c r="AU13" s="15" t="str">
+        <f>newline &amp; space &amp; M13 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z13 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_2_desc:0 "$buy_influence_2point0_em_desc$"</v>
+      </c>
+      <c r="AV13" s="15" t="str">
+        <f>newline &amp; space &amp; N13 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z13 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_3_desc:0 "$buy_influence_2point0_em_desc$"</v>
+      </c>
+      <c r="AW13" s="15" t="str">
+        <f>newline &amp; space &amp; O13 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z13 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_4_desc:0 "$buy_influence_2point0_em_desc$"</v>
+      </c>
+      <c r="AX13" s="15" t="str">
+        <f>newline &amp; space &amp; P13 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z13 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_5_desc:0 "$buy_influence_2point0_em_desc$"</v>
+      </c>
+      <c r="AY13" s="16" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_1_desc:0 "$buy_influence_2point0_em_desc$"
+ buy_influence_2point0_em_2_desc:0 "$buy_influence_2point0_em_desc$"
+ buy_influence_2point0_em_3_desc:0 "$buy_influence_2point0_em_desc$"
+ buy_influence_2point0_em_4_desc:0 "$buy_influence_2point0_em_desc$"
+ buy_influence_2point0_em_5_desc:0 "$buy_influence_2point0_em_desc$"</v>
+      </c>
     </row>
-    <row r="14" spans="2:39" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:51" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B14" s="55" t="s">
         <v>12</v>
       </c>
@@ -4258,7 +4560,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>10</v>
       </c>
       <c r="F14" s="57"/>
@@ -4273,11 +4575,11 @@
         <v>1</v>
       </c>
       <c r="K14" s="14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>buy_influence_1point0_mf</v>
       </c>
       <c r="L14" s="36" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>buy_influence_1point0_mf_1</v>
       </c>
       <c r="M14" s="37" t="str">
@@ -4306,12 +4608,7 @@
 			has_modifier = buy_influence_1point0_mf_5</v>
       </c>
       <c r="R14" s="25" t="str">
-        <f xml:space="preserve">
-newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$L14
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$M14
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$N14
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$O14
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$P14</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">
 		remove_modifier = buy_influence_1point0_mf_1
 		remove_modifier = buy_influence_1point0_mf_2
@@ -4320,14 +4617,7 @@
 		remove_modifier = buy_influence_1point0_mf_5</v>
       </c>
       <c r="S14" s="14" t="str">
-        <f>newline&amp;newline&amp;L14&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D14
-&amp;IF($F14&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F14*$J14*L$8,"")
-&amp;IF($G14&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G14*$J14*L$8,"")
-&amp;IF($H14&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H14*$J14*L$8,"")
-&amp;IF($I14&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I14*$J14*L$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">
 buy_influence_1point0_mf_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -4337,14 +4627,7 @@
 }</v>
       </c>
       <c r="T14" s="15" t="str">
-        <f>newline&amp;newline&amp;M14&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D14
-&amp;IF($F14&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F14*$J14*M$8,"")
-&amp;IF($G14&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G14*$J14*M$8,"")
-&amp;IF($H14&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H14*$J14*M$8,"")
-&amp;IF($I14&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I14*$J14*M$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">
 buy_influence_1point0_mf_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -4354,14 +4637,7 @@
 }</v>
       </c>
       <c r="U14" s="15" t="str">
-        <f>newline&amp;newline&amp;N14&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D14
-&amp;IF($F14&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F14*$J14*N$8,"")
-&amp;IF($G14&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G14*$J14*N$8,"")
-&amp;IF($H14&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H14*$J14*N$8,"")
-&amp;IF($I14&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I14*$J14*N$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">
 buy_influence_1point0_mf_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -4371,14 +4647,7 @@
 }</v>
       </c>
       <c r="V14" s="15" t="str">
-        <f>newline&amp;newline&amp;O14&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D14
-&amp;IF($F14&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F14*$J14*O$8,"")
-&amp;IF($G14&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G14*$J14*O$8,"")
-&amp;IF($H14&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H14*$J14*O$8,"")
-&amp;IF($I14&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I14*$J14*O$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">
 buy_influence_1point0_mf_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -4388,14 +4657,7 @@
 }</v>
       </c>
       <c r="W14" s="18" t="str">
-        <f>newline&amp;newline&amp;P14&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D14
-&amp;IF($F14&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F14*$J14*P$8,"")
-&amp;IF($G14&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G14*$J14*P$8,"")
-&amp;IF($H14&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H14*$J14*P$8,"")
-&amp;IF($I14&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I14*$J14*P$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">
 buy_influence_1point0_mf_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -4405,7 +4667,7 @@
 }</v>
       </c>
       <c r="X14" s="16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
 buy_influence_1point0_mf_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -4439,19 +4701,19 @@
 }</v>
       </c>
       <c r="Y14" s="25" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>buy_influence_1point0_mf_name</v>
       </c>
       <c r="Z14" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>buy_influence_1point0_mf_desc</v>
       </c>
       <c r="AA14" s="70" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_1point0_mf_response</v>
       </c>
       <c r="AB14" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_mf_name
 		trigger = {
@@ -4480,7 +4742,7 @@
 </v>
       </c>
       <c r="AC14" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_mf_name
 		trigger = {
@@ -4510,7 +4772,7 @@
 </v>
       </c>
       <c r="AD14" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_mf_name
 		trigger = {
@@ -4540,7 +4802,7 @@
 </v>
       </c>
       <c r="AE14" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_mf_name
 		trigger = {
@@ -4570,7 +4832,7 @@
 </v>
       </c>
       <c r="AF14" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_mf_name
 		trigger = {
@@ -4599,7 +4861,7 @@
 </v>
       </c>
       <c r="AG14" s="16" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_mf_name
 		trigger = {
@@ -4731,32 +4993,32 @@
 </v>
       </c>
       <c r="AH14" s="14" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; L14 &amp; " = { text = " &amp; $AA14 &amp; " }"</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">
 				buy_influence_1point0_mf_1 = { text = buy_influence_1point0_mf_response }</v>
       </c>
       <c r="AI14" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; M14 &amp; " = { text = " &amp; $AA14 &amp; " }"</f>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">
 				buy_influence_1point0_mf_2 = { text = buy_influence_1point0_mf_response }</v>
       </c>
       <c r="AJ14" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; N14 &amp; " = { text = " &amp; $AA14 &amp; " }"</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">
 				buy_influence_1point0_mf_3 = { text = buy_influence_1point0_mf_response }</v>
       </c>
       <c r="AK14" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; O14 &amp; " = { text = " &amp; $AA14 &amp; " }"</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">
 				buy_influence_1point0_mf_4 = { text = buy_influence_1point0_mf_response }</v>
       </c>
       <c r="AL14" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; P14 &amp; " = { text = " &amp; $AA14 &amp; " }"</f>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">
 				buy_influence_1point0_mf_5 = { text = buy_influence_1point0_mf_response }</v>
       </c>
-      <c r="AM14" s="16" t="str">
-        <f t="shared" si="7"/>
+      <c r="AM14" s="18" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_1point0_mf_1 = { text = buy_influence_1point0_mf_response }
 				buy_influence_1point0_mf_2 = { text = buy_influence_1point0_mf_response }
@@ -4764,8 +5026,76 @@
 				buy_influence_1point0_mf_4 = { text = buy_influence_1point0_mf_response }
 				buy_influence_1point0_mf_5 = { text = buy_influence_1point0_mf_response }</v>
       </c>
+      <c r="AN14" s="14" t="str">
+        <f>newline &amp; space &amp; L14 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y14 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_1_name:0 "$buy_influence_1point0_mf_name$"</v>
+      </c>
+      <c r="AO14" s="15" t="str">
+        <f>newline &amp; space &amp; M14 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y14 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_2_name:0 "$buy_influence_1point0_mf_name$"</v>
+      </c>
+      <c r="AP14" s="15" t="str">
+        <f>newline &amp; space &amp; N14 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y14 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_3_name:0 "$buy_influence_1point0_mf_name$"</v>
+      </c>
+      <c r="AQ14" s="15" t="str">
+        <f>newline &amp; space &amp; O14 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y14 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_4_name:0 "$buy_influence_1point0_mf_name$"</v>
+      </c>
+      <c r="AR14" s="15" t="str">
+        <f>newline &amp; space &amp; P14 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y14 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_5_name:0 "$buy_influence_1point0_mf_name$"</v>
+      </c>
+      <c r="AS14" s="18" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_1_name:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point0_mf_2_name:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point0_mf_3_name:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point0_mf_4_name:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point0_mf_5_name:0 "$buy_influence_1point0_mf_name$"</v>
+      </c>
+      <c r="AT14" s="14" t="str">
+        <f>newline &amp; space &amp; L14 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z14 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_1_desc:0 "$buy_influence_1point0_mf_desc$"</v>
+      </c>
+      <c r="AU14" s="15" t="str">
+        <f>newline &amp; space &amp; M14 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z14 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_2_desc:0 "$buy_influence_1point0_mf_desc$"</v>
+      </c>
+      <c r="AV14" s="15" t="str">
+        <f>newline &amp; space &amp; N14 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z14 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_3_desc:0 "$buy_influence_1point0_mf_desc$"</v>
+      </c>
+      <c r="AW14" s="15" t="str">
+        <f>newline &amp; space &amp; O14 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z14 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_4_desc:0 "$buy_influence_1point0_mf_desc$"</v>
+      </c>
+      <c r="AX14" s="15" t="str">
+        <f>newline &amp; space &amp; P14 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z14 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_5_desc:0 "$buy_influence_1point0_mf_desc$"</v>
+      </c>
+      <c r="AY14" s="16" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_1_desc:0 "$buy_influence_1point0_mf_desc$"
+ buy_influence_1point0_mf_2_desc:0 "$buy_influence_1point0_mf_desc$"
+ buy_influence_1point0_mf_3_desc:0 "$buy_influence_1point0_mf_desc$"
+ buy_influence_1point0_mf_4_desc:0 "$buy_influence_1point0_mf_desc$"
+ buy_influence_1point0_mf_5_desc:0 "$buy_influence_1point0_mf_desc$"</v>
+      </c>
     </row>
-    <row r="15" spans="2:39" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:51" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B15" s="55" t="s">
         <v>12</v>
       </c>
@@ -4776,7 +5106,7 @@
         <v>1.5</v>
       </c>
       <c r="E15" s="43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>15</v>
       </c>
       <c r="F15" s="57"/>
@@ -4791,11 +5121,11 @@
         <v>1</v>
       </c>
       <c r="K15" s="14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>buy_influence_1point5_mf</v>
       </c>
       <c r="L15" s="36" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>buy_influence_1point5_mf_1</v>
       </c>
       <c r="M15" s="37" t="str">
@@ -4824,12 +5154,7 @@
 			has_modifier = buy_influence_1point5_mf_5</v>
       </c>
       <c r="R15" s="25" t="str">
-        <f xml:space="preserve">
-newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$L15
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$M15
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$N15
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$O15
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$P15</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">
 		remove_modifier = buy_influence_1point5_mf_1
 		remove_modifier = buy_influence_1point5_mf_2
@@ -4838,14 +5163,7 @@
 		remove_modifier = buy_influence_1point5_mf_5</v>
       </c>
       <c r="S15" s="14" t="str">
-        <f>newline&amp;newline&amp;L15&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D15
-&amp;IF($F15&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F15*$J15*L$8,"")
-&amp;IF($G15&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G15*$J15*L$8,"")
-&amp;IF($H15&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H15*$J15*L$8,"")
-&amp;IF($I15&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I15*$J15*L$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">
 buy_influence_1point5_mf_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -4855,14 +5173,7 @@
 }</v>
       </c>
       <c r="T15" s="15" t="str">
-        <f>newline&amp;newline&amp;M15&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D15
-&amp;IF($F15&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F15*$J15*M$8,"")
-&amp;IF($G15&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G15*$J15*M$8,"")
-&amp;IF($H15&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H15*$J15*M$8,"")
-&amp;IF($I15&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I15*$J15*M$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">
 buy_influence_1point5_mf_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -4872,14 +5183,7 @@
 }</v>
       </c>
       <c r="U15" s="15" t="str">
-        <f>newline&amp;newline&amp;N15&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D15
-&amp;IF($F15&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F15*$J15*N$8,"")
-&amp;IF($G15&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G15*$J15*N$8,"")
-&amp;IF($H15&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H15*$J15*N$8,"")
-&amp;IF($I15&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I15*$J15*N$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">
 buy_influence_1point5_mf_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -4889,14 +5193,7 @@
 }</v>
       </c>
       <c r="V15" s="15" t="str">
-        <f>newline&amp;newline&amp;O15&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D15
-&amp;IF($F15&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F15*$J15*O$8,"")
-&amp;IF($G15&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G15*$J15*O$8,"")
-&amp;IF($H15&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H15*$J15*O$8,"")
-&amp;IF($I15&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I15*$J15*O$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">
 buy_influence_1point5_mf_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -4906,14 +5203,7 @@
 }</v>
       </c>
       <c r="W15" s="18" t="str">
-        <f>newline&amp;newline&amp;P15&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D15
-&amp;IF($F15&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F15*$J15*P$8,"")
-&amp;IF($G15&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G15*$J15*P$8,"")
-&amp;IF($H15&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H15*$J15*P$8,"")
-&amp;IF($I15&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I15*$J15*P$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">
 buy_influence_1point5_mf_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -4923,7 +5213,7 @@
 }</v>
       </c>
       <c r="X15" s="16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
 buy_influence_1point5_mf_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -4957,19 +5247,19 @@
 }</v>
       </c>
       <c r="Y15" s="25" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>buy_influence_1point5_mf_name</v>
       </c>
       <c r="Z15" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>buy_influence_1point5_mf_desc</v>
       </c>
       <c r="AA15" s="70" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_1point5_mf_response</v>
       </c>
       <c r="AB15" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point5_mf_name
 		trigger = {
@@ -4998,7 +5288,7 @@
 </v>
       </c>
       <c r="AC15" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point5_mf_name
 		trigger = {
@@ -5028,7 +5318,7 @@
 </v>
       </c>
       <c r="AD15" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point5_mf_name
 		trigger = {
@@ -5058,7 +5348,7 @@
 </v>
       </c>
       <c r="AE15" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point5_mf_name
 		trigger = {
@@ -5088,7 +5378,7 @@
 </v>
       </c>
       <c r="AF15" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point5_mf_name
 		trigger = {
@@ -5117,7 +5407,7 @@
 </v>
       </c>
       <c r="AG15" s="16" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point5_mf_name
 		trigger = {
@@ -5249,32 +5539,32 @@
 </v>
       </c>
       <c r="AH15" s="14" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; L15 &amp; " = { text = " &amp; $AA15 &amp; " }"</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">
 				buy_influence_1point5_mf_1 = { text = buy_influence_1point5_mf_response }</v>
       </c>
       <c r="AI15" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; M15 &amp; " = { text = " &amp; $AA15 &amp; " }"</f>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">
 				buy_influence_1point5_mf_2 = { text = buy_influence_1point5_mf_response }</v>
       </c>
       <c r="AJ15" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; N15 &amp; " = { text = " &amp; $AA15 &amp; " }"</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">
 				buy_influence_1point5_mf_3 = { text = buy_influence_1point5_mf_response }</v>
       </c>
       <c r="AK15" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; O15 &amp; " = { text = " &amp; $AA15 &amp; " }"</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">
 				buy_influence_1point5_mf_4 = { text = buy_influence_1point5_mf_response }</v>
       </c>
       <c r="AL15" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; P15 &amp; " = { text = " &amp; $AA15 &amp; " }"</f>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">
 				buy_influence_1point5_mf_5 = { text = buy_influence_1point5_mf_response }</v>
       </c>
-      <c r="AM15" s="16" t="str">
-        <f t="shared" si="7"/>
+      <c r="AM15" s="18" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_1point5_mf_1 = { text = buy_influence_1point5_mf_response }
 				buy_influence_1point5_mf_2 = { text = buy_influence_1point5_mf_response }
@@ -5282,8 +5572,76 @@
 				buy_influence_1point5_mf_4 = { text = buy_influence_1point5_mf_response }
 				buy_influence_1point5_mf_5 = { text = buy_influence_1point5_mf_response }</v>
       </c>
+      <c r="AN15" s="14" t="str">
+        <f>newline &amp; space &amp; L15 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y15 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_1_name:0 "$buy_influence_1point5_mf_name$"</v>
+      </c>
+      <c r="AO15" s="15" t="str">
+        <f>newline &amp; space &amp; M15 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y15 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_2_name:0 "$buy_influence_1point5_mf_name$"</v>
+      </c>
+      <c r="AP15" s="15" t="str">
+        <f>newline &amp; space &amp; N15 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y15 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_3_name:0 "$buy_influence_1point5_mf_name$"</v>
+      </c>
+      <c r="AQ15" s="15" t="str">
+        <f>newline &amp; space &amp; O15 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y15 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_4_name:0 "$buy_influence_1point5_mf_name$"</v>
+      </c>
+      <c r="AR15" s="15" t="str">
+        <f>newline &amp; space &amp; P15 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y15 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_5_name:0 "$buy_influence_1point5_mf_name$"</v>
+      </c>
+      <c r="AS15" s="18" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_1_name:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_1point5_mf_2_name:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_1point5_mf_3_name:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_1point5_mf_4_name:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_1point5_mf_5_name:0 "$buy_influence_1point5_mf_name$"</v>
+      </c>
+      <c r="AT15" s="14" t="str">
+        <f>newline &amp; space &amp; L15 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z15 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_1_desc:0 "$buy_influence_1point5_mf_desc$"</v>
+      </c>
+      <c r="AU15" s="15" t="str">
+        <f>newline &amp; space &amp; M15 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z15 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_2_desc:0 "$buy_influence_1point5_mf_desc$"</v>
+      </c>
+      <c r="AV15" s="15" t="str">
+        <f>newline &amp; space &amp; N15 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z15 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_3_desc:0 "$buy_influence_1point5_mf_desc$"</v>
+      </c>
+      <c r="AW15" s="15" t="str">
+        <f>newline &amp; space &amp; O15 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z15 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_4_desc:0 "$buy_influence_1point5_mf_desc$"</v>
+      </c>
+      <c r="AX15" s="15" t="str">
+        <f>newline &amp; space &amp; P15 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z15 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_5_desc:0 "$buy_influence_1point5_mf_desc$"</v>
+      </c>
+      <c r="AY15" s="16" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_1_desc:0 "$buy_influence_1point5_mf_desc$"
+ buy_influence_1point5_mf_2_desc:0 "$buy_influence_1point5_mf_desc$"
+ buy_influence_1point5_mf_3_desc:0 "$buy_influence_1point5_mf_desc$"
+ buy_influence_1point5_mf_4_desc:0 "$buy_influence_1point5_mf_desc$"
+ buy_influence_1point5_mf_5_desc:0 "$buy_influence_1point5_mf_desc$"</v>
+      </c>
     </row>
-    <row r="16" spans="2:39" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:51" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B16" s="55" t="s">
         <v>12</v>
       </c>
@@ -5294,7 +5652,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>20</v>
       </c>
       <c r="F16" s="57"/>
@@ -5309,11 +5667,11 @@
         <v>1</v>
       </c>
       <c r="K16" s="14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>buy_influence_2point0_mf</v>
       </c>
       <c r="L16" s="36" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>buy_influence_2point0_mf_1</v>
       </c>
       <c r="M16" s="37" t="str">
@@ -5342,12 +5700,7 @@
 			has_modifier = buy_influence_2point0_mf_5</v>
       </c>
       <c r="R16" s="25" t="str">
-        <f xml:space="preserve">
-newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$L16
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$M16
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$N16
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$O16
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$P16</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">
 		remove_modifier = buy_influence_2point0_mf_1
 		remove_modifier = buy_influence_2point0_mf_2
@@ -5356,14 +5709,7 @@
 		remove_modifier = buy_influence_2point0_mf_5</v>
       </c>
       <c r="S16" s="14" t="str">
-        <f>newline&amp;newline&amp;L16&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D16
-&amp;IF($F16&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F16*$J16*L$8,"")
-&amp;IF($G16&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G16*$J16*L$8,"")
-&amp;IF($H16&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H16*$J16*L$8,"")
-&amp;IF($I16&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I16*$J16*L$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">
 buy_influence_2point0_mf_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -5373,14 +5719,7 @@
 }</v>
       </c>
       <c r="T16" s="15" t="str">
-        <f>newline&amp;newline&amp;M16&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D16
-&amp;IF($F16&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F16*$J16*M$8,"")
-&amp;IF($G16&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G16*$J16*M$8,"")
-&amp;IF($H16&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H16*$J16*M$8,"")
-&amp;IF($I16&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I16*$J16*M$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">
 buy_influence_2point0_mf_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -5390,14 +5729,7 @@
 }</v>
       </c>
       <c r="U16" s="15" t="str">
-        <f>newline&amp;newline&amp;N16&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D16
-&amp;IF($F16&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F16*$J16*N$8,"")
-&amp;IF($G16&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G16*$J16*N$8,"")
-&amp;IF($H16&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H16*$J16*N$8,"")
-&amp;IF($I16&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I16*$J16*N$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">
 buy_influence_2point0_mf_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -5407,14 +5739,7 @@
 }</v>
       </c>
       <c r="V16" s="15" t="str">
-        <f>newline&amp;newline&amp;O16&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D16
-&amp;IF($F16&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F16*$J16*O$8,"")
-&amp;IF($G16&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G16*$J16*O$8,"")
-&amp;IF($H16&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H16*$J16*O$8,"")
-&amp;IF($I16&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I16*$J16*O$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">
 buy_influence_2point0_mf_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -5424,14 +5749,7 @@
 }</v>
       </c>
       <c r="W16" s="18" t="str">
-        <f>newline&amp;newline&amp;P16&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D16
-&amp;IF($F16&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F16*$J16*P$8,"")
-&amp;IF($G16&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G16*$J16*P$8,"")
-&amp;IF($H16&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H16*$J16*P$8,"")
-&amp;IF($I16&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I16*$J16*P$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">
 buy_influence_2point0_mf_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -5441,7 +5759,7 @@
 }</v>
       </c>
       <c r="X16" s="16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
 buy_influence_2point0_mf_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -5475,19 +5793,19 @@
 }</v>
       </c>
       <c r="Y16" s="25" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>buy_influence_2point0_mf_name</v>
       </c>
       <c r="Z16" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>buy_influence_2point0_mf_desc</v>
       </c>
       <c r="AA16" s="70" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_2point0_mf_response</v>
       </c>
       <c r="AB16" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_mf_name
 		trigger = {
@@ -5516,7 +5834,7 @@
 </v>
       </c>
       <c r="AC16" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_mf_name
 		trigger = {
@@ -5546,7 +5864,7 @@
 </v>
       </c>
       <c r="AD16" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_mf_name
 		trigger = {
@@ -5576,7 +5894,7 @@
 </v>
       </c>
       <c r="AE16" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_mf_name
 		trigger = {
@@ -5606,7 +5924,7 @@
 </v>
       </c>
       <c r="AF16" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_mf_name
 		trigger = {
@@ -5635,7 +5953,7 @@
 </v>
       </c>
       <c r="AG16" s="16" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_mf_name
 		trigger = {
@@ -5767,32 +6085,32 @@
 </v>
       </c>
       <c r="AH16" s="14" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; L16 &amp; " = { text = " &amp; $AA16 &amp; " }"</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">
 				buy_influence_2point0_mf_1 = { text = buy_influence_2point0_mf_response }</v>
       </c>
       <c r="AI16" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; M16 &amp; " = { text = " &amp; $AA16 &amp; " }"</f>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">
 				buy_influence_2point0_mf_2 = { text = buy_influence_2point0_mf_response }</v>
       </c>
       <c r="AJ16" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; N16 &amp; " = { text = " &amp; $AA16 &amp; " }"</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">
 				buy_influence_2point0_mf_3 = { text = buy_influence_2point0_mf_response }</v>
       </c>
       <c r="AK16" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; O16 &amp; " = { text = " &amp; $AA16 &amp; " }"</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">
 				buy_influence_2point0_mf_4 = { text = buy_influence_2point0_mf_response }</v>
       </c>
       <c r="AL16" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; P16 &amp; " = { text = " &amp; $AA16 &amp; " }"</f>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">
 				buy_influence_2point0_mf_5 = { text = buy_influence_2point0_mf_response }</v>
       </c>
-      <c r="AM16" s="16" t="str">
-        <f t="shared" si="7"/>
+      <c r="AM16" s="18" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_2point0_mf_1 = { text = buy_influence_2point0_mf_response }
 				buy_influence_2point0_mf_2 = { text = buy_influence_2point0_mf_response }
@@ -5800,8 +6118,76 @@
 				buy_influence_2point0_mf_4 = { text = buy_influence_2point0_mf_response }
 				buy_influence_2point0_mf_5 = { text = buy_influence_2point0_mf_response }</v>
       </c>
+      <c r="AN16" s="14" t="str">
+        <f>newline &amp; space &amp; L16 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y16 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_1_name:0 "$buy_influence_2point0_mf_name$"</v>
+      </c>
+      <c r="AO16" s="15" t="str">
+        <f>newline &amp; space &amp; M16 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y16 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_2_name:0 "$buy_influence_2point0_mf_name$"</v>
+      </c>
+      <c r="AP16" s="15" t="str">
+        <f>newline &amp; space &amp; N16 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y16 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_3_name:0 "$buy_influence_2point0_mf_name$"</v>
+      </c>
+      <c r="AQ16" s="15" t="str">
+        <f>newline &amp; space &amp; O16 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y16 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_4_name:0 "$buy_influence_2point0_mf_name$"</v>
+      </c>
+      <c r="AR16" s="15" t="str">
+        <f>newline &amp; space &amp; P16 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y16 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_5_name:0 "$buy_influence_2point0_mf_name$"</v>
+      </c>
+      <c r="AS16" s="18" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_1_name:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_mf_2_name:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_mf_3_name:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_mf_4_name:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_mf_5_name:0 "$buy_influence_2point0_mf_name$"</v>
+      </c>
+      <c r="AT16" s="14" t="str">
+        <f>newline &amp; space &amp; L16 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z16 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_1_desc:0 "$buy_influence_2point0_mf_desc$"</v>
+      </c>
+      <c r="AU16" s="15" t="str">
+        <f>newline &amp; space &amp; M16 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z16 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_2_desc:0 "$buy_influence_2point0_mf_desc$"</v>
+      </c>
+      <c r="AV16" s="15" t="str">
+        <f>newline &amp; space &amp; N16 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z16 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_3_desc:0 "$buy_influence_2point0_mf_desc$"</v>
+      </c>
+      <c r="AW16" s="15" t="str">
+        <f>newline &amp; space &amp; O16 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z16 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_4_desc:0 "$buy_influence_2point0_mf_desc$"</v>
+      </c>
+      <c r="AX16" s="15" t="str">
+        <f>newline &amp; space &amp; P16 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z16 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_5_desc:0 "$buy_influence_2point0_mf_desc$"</v>
+      </c>
+      <c r="AY16" s="16" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_1_desc:0 "$buy_influence_2point0_mf_desc$"
+ buy_influence_2point0_mf_2_desc:0 "$buy_influence_2point0_mf_desc$"
+ buy_influence_2point0_mf_3_desc:0 "$buy_influence_2point0_mf_desc$"
+ buy_influence_2point0_mf_4_desc:0 "$buy_influence_2point0_mf_desc$"
+ buy_influence_2point0_mf_5_desc:0 "$buy_influence_2point0_mf_desc$"</v>
+      </c>
     </row>
-    <row r="17" spans="2:39" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:51" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B17" s="55" t="s">
         <v>14</v>
       </c>
@@ -5812,7 +6198,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>20</v>
       </c>
       <c r="F17" s="57">
@@ -5829,11 +6215,11 @@
         <v>1</v>
       </c>
       <c r="K17" s="14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>buy_influence_2point0_emc</v>
       </c>
       <c r="L17" s="36" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>buy_influence_2point0_emc_1</v>
       </c>
       <c r="M17" s="37" t="str">
@@ -5862,12 +6248,7 @@
 			has_modifier = buy_influence_2point0_emc_5</v>
       </c>
       <c r="R17" s="25" t="str">
-        <f xml:space="preserve">
-newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$L17
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$M17
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$N17
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$O17
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$P17</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">
 		remove_modifier = buy_influence_2point0_emc_1
 		remove_modifier = buy_influence_2point0_emc_2
@@ -5876,14 +6257,7 @@
 		remove_modifier = buy_influence_2point0_emc_5</v>
       </c>
       <c r="S17" s="14" t="str">
-        <f>newline&amp;newline&amp;L17&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D17
-&amp;IF($F17&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F17*$J17*L$8,"")
-&amp;IF($G17&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G17*$J17*L$8,"")
-&amp;IF($H17&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H17*$J17*L$8,"")
-&amp;IF($I17&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I17*$J17*L$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">
 buy_influence_2point0_emc_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -5894,14 +6268,7 @@
 }</v>
       </c>
       <c r="T17" s="15" t="str">
-        <f>newline&amp;newline&amp;M17&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D17
-&amp;IF($F17&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F17*$J17*M$8,"")
-&amp;IF($G17&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G17*$J17*M$8,"")
-&amp;IF($H17&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H17*$J17*M$8,"")
-&amp;IF($I17&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I17*$J17*M$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">
 buy_influence_2point0_emc_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -5912,14 +6279,7 @@
 }</v>
       </c>
       <c r="U17" s="15" t="str">
-        <f>newline&amp;newline&amp;N17&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D17
-&amp;IF($F17&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F17*$J17*N$8,"")
-&amp;IF($G17&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G17*$J17*N$8,"")
-&amp;IF($H17&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H17*$J17*N$8,"")
-&amp;IF($I17&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I17*$J17*N$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">
 buy_influence_2point0_emc_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -5930,14 +6290,7 @@
 }</v>
       </c>
       <c r="V17" s="15" t="str">
-        <f>newline&amp;newline&amp;O17&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D17
-&amp;IF($F17&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F17*$J17*O$8,"")
-&amp;IF($G17&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G17*$J17*O$8,"")
-&amp;IF($H17&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H17*$J17*O$8,"")
-&amp;IF($I17&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I17*$J17*O$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">
 buy_influence_2point0_emc_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -5948,14 +6301,7 @@
 }</v>
       </c>
       <c r="W17" s="18" t="str">
-        <f>newline&amp;newline&amp;P17&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D17
-&amp;IF($F17&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F17*$J17*P$8,"")
-&amp;IF($G17&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G17*$J17*P$8,"")
-&amp;IF($H17&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H17*$J17*P$8,"")
-&amp;IF($I17&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I17*$J17*P$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">
 buy_influence_2point0_emc_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -5966,7 +6312,7 @@
 }</v>
       </c>
       <c r="X17" s="16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
 buy_influence_2point0_emc_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6005,19 +6351,19 @@
 }</v>
       </c>
       <c r="Y17" s="25" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>buy_influence_2point0_emc_name</v>
       </c>
       <c r="Z17" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>buy_influence_2point0_emc_desc</v>
       </c>
       <c r="AA17" s="70" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_2point0_emc_response</v>
       </c>
       <c r="AB17" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_emc_name
 		trigger = {
@@ -6046,7 +6392,7 @@
 </v>
       </c>
       <c r="AC17" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_emc_name
 		trigger = {
@@ -6076,7 +6422,7 @@
 </v>
       </c>
       <c r="AD17" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_emc_name
 		trigger = {
@@ -6106,7 +6452,7 @@
 </v>
       </c>
       <c r="AE17" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_emc_name
 		trigger = {
@@ -6136,7 +6482,7 @@
 </v>
       </c>
       <c r="AF17" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_emc_name
 		trigger = {
@@ -6165,7 +6511,7 @@
 </v>
       </c>
       <c r="AG17" s="16" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_emc_name
 		trigger = {
@@ -6297,32 +6643,32 @@
 </v>
       </c>
       <c r="AH17" s="14" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; L17 &amp; " = { text = " &amp; $AA17 &amp; " }"</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">
 				buy_influence_2point0_emc_1 = { text = buy_influence_2point0_emc_response }</v>
       </c>
       <c r="AI17" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; M17 &amp; " = { text = " &amp; $AA17 &amp; " }"</f>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">
 				buy_influence_2point0_emc_2 = { text = buy_influence_2point0_emc_response }</v>
       </c>
       <c r="AJ17" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; N17 &amp; " = { text = " &amp; $AA17 &amp; " }"</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">
 				buy_influence_2point0_emc_3 = { text = buy_influence_2point0_emc_response }</v>
       </c>
       <c r="AK17" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; O17 &amp; " = { text = " &amp; $AA17 &amp; " }"</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">
 				buy_influence_2point0_emc_4 = { text = buy_influence_2point0_emc_response }</v>
       </c>
       <c r="AL17" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; P17 &amp; " = { text = " &amp; $AA17 &amp; " }"</f>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">
 				buy_influence_2point0_emc_5 = { text = buy_influence_2point0_emc_response }</v>
       </c>
-      <c r="AM17" s="16" t="str">
-        <f t="shared" si="7"/>
+      <c r="AM17" s="18" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_2point0_emc_1 = { text = buy_influence_2point0_emc_response }
 				buy_influence_2point0_emc_2 = { text = buy_influence_2point0_emc_response }
@@ -6330,8 +6676,76 @@
 				buy_influence_2point0_emc_4 = { text = buy_influence_2point0_emc_response }
 				buy_influence_2point0_emc_5 = { text = buy_influence_2point0_emc_response }</v>
       </c>
+      <c r="AN17" s="14" t="str">
+        <f>newline &amp; space &amp; L17 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y17 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_1_name:0 "$buy_influence_2point0_emc_name$"</v>
+      </c>
+      <c r="AO17" s="15" t="str">
+        <f>newline &amp; space &amp; M17 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y17 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_2_name:0 "$buy_influence_2point0_emc_name$"</v>
+      </c>
+      <c r="AP17" s="15" t="str">
+        <f>newline &amp; space &amp; N17 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y17 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_3_name:0 "$buy_influence_2point0_emc_name$"</v>
+      </c>
+      <c r="AQ17" s="15" t="str">
+        <f>newline &amp; space &amp; O17 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y17 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_4_name:0 "$buy_influence_2point0_emc_name$"</v>
+      </c>
+      <c r="AR17" s="15" t="str">
+        <f>newline &amp; space &amp; P17 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y17 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_5_name:0 "$buy_influence_2point0_emc_name$"</v>
+      </c>
+      <c r="AS17" s="18" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_1_name:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_2point0_emc_2_name:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_2point0_emc_3_name:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_2point0_emc_4_name:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_2point0_emc_5_name:0 "$buy_influence_2point0_emc_name$"</v>
+      </c>
+      <c r="AT17" s="14" t="str">
+        <f>newline &amp; space &amp; L17 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z17 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_1_desc:0 "$buy_influence_2point0_emc_desc$"</v>
+      </c>
+      <c r="AU17" s="15" t="str">
+        <f>newline &amp; space &amp; M17 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z17 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_2_desc:0 "$buy_influence_2point0_emc_desc$"</v>
+      </c>
+      <c r="AV17" s="15" t="str">
+        <f>newline &amp; space &amp; N17 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z17 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_3_desc:0 "$buy_influence_2point0_emc_desc$"</v>
+      </c>
+      <c r="AW17" s="15" t="str">
+        <f>newline &amp; space &amp; O17 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z17 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_4_desc:0 "$buy_influence_2point0_emc_desc$"</v>
+      </c>
+      <c r="AX17" s="15" t="str">
+        <f>newline &amp; space &amp; P17 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z17 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_5_desc:0 "$buy_influence_2point0_emc_desc$"</v>
+      </c>
+      <c r="AY17" s="16" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_1_desc:0 "$buy_influence_2point0_emc_desc$"
+ buy_influence_2point0_emc_2_desc:0 "$buy_influence_2point0_emc_desc$"
+ buy_influence_2point0_emc_3_desc:0 "$buy_influence_2point0_emc_desc$"
+ buy_influence_2point0_emc_4_desc:0 "$buy_influence_2point0_emc_desc$"
+ buy_influence_2point0_emc_5_desc:0 "$buy_influence_2point0_emc_desc$"</v>
+      </c>
     </row>
-    <row r="18" spans="2:39" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:51" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B18" s="55" t="s">
         <v>14</v>
       </c>
@@ -6342,7 +6756,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>25</v>
       </c>
       <c r="F18" s="57">
@@ -6359,11 +6773,11 @@
         <v>1</v>
       </c>
       <c r="K18" s="14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>buy_influence_3point0_emc</v>
       </c>
       <c r="L18" s="36" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>buy_influence_3point0_emc_1</v>
       </c>
       <c r="M18" s="37" t="str">
@@ -6392,12 +6806,7 @@
 			has_modifier = buy_influence_3point0_emc_5</v>
       </c>
       <c r="R18" s="25" t="str">
-        <f xml:space="preserve">
-newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$L18
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$M18
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$N18
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$O18
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$P18</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">
 		remove_modifier = buy_influence_3point0_emc_1
 		remove_modifier = buy_influence_3point0_emc_2
@@ -6406,14 +6815,7 @@
 		remove_modifier = buy_influence_3point0_emc_5</v>
       </c>
       <c r="S18" s="14" t="str">
-        <f>newline&amp;newline&amp;L18&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D18
-&amp;IF($F18&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F18*$J18*L$8,"")
-&amp;IF($G18&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G18*$J18*L$8,"")
-&amp;IF($H18&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H18*$J18*L$8,"")
-&amp;IF($I18&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I18*$J18*L$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">
 buy_influence_3point0_emc_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6424,14 +6826,7 @@
 }</v>
       </c>
       <c r="T18" s="15" t="str">
-        <f>newline&amp;newline&amp;M18&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D18
-&amp;IF($F18&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F18*$J18*M$8,"")
-&amp;IF($G18&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G18*$J18*M$8,"")
-&amp;IF($H18&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H18*$J18*M$8,"")
-&amp;IF($I18&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I18*$J18*M$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">
 buy_influence_3point0_emc_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6442,14 +6837,7 @@
 }</v>
       </c>
       <c r="U18" s="15" t="str">
-        <f>newline&amp;newline&amp;N18&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D18
-&amp;IF($F18&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F18*$J18*N$8,"")
-&amp;IF($G18&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G18*$J18*N$8,"")
-&amp;IF($H18&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H18*$J18*N$8,"")
-&amp;IF($I18&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I18*$J18*N$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">
 buy_influence_3point0_emc_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6460,14 +6848,7 @@
 }</v>
       </c>
       <c r="V18" s="15" t="str">
-        <f>newline&amp;newline&amp;O18&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D18
-&amp;IF($F18&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F18*$J18*O$8,"")
-&amp;IF($G18&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G18*$J18*O$8,"")
-&amp;IF($H18&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H18*$J18*O$8,"")
-&amp;IF($I18&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I18*$J18*O$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">
 buy_influence_3point0_emc_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6478,14 +6859,7 @@
 }</v>
       </c>
       <c r="W18" s="18" t="str">
-        <f>newline&amp;newline&amp;P18&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D18
-&amp;IF($F18&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F18*$J18*P$8,"")
-&amp;IF($G18&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G18*$J18*P$8,"")
-&amp;IF($H18&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H18*$J18*P$8,"")
-&amp;IF($I18&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I18*$J18*P$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">
 buy_influence_3point0_emc_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6496,7 +6870,7 @@
 }</v>
       </c>
       <c r="X18" s="16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
 buy_influence_3point0_emc_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6535,19 +6909,19 @@
 }</v>
       </c>
       <c r="Y18" s="25" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>buy_influence_3point0_emc_name</v>
       </c>
       <c r="Z18" s="15" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>buy_influence_3point0_emc_desc</v>
       </c>
       <c r="AA18" s="70" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_3point0_emc_response</v>
       </c>
       <c r="AB18" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_3point0_emc_name
 		trigger = {
@@ -6576,7 +6950,7 @@
 </v>
       </c>
       <c r="AC18" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_3point0_emc_name
 		trigger = {
@@ -6606,7 +6980,7 @@
 </v>
       </c>
       <c r="AD18" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_3point0_emc_name
 		trigger = {
@@ -6636,7 +7010,7 @@
 </v>
       </c>
       <c r="AE18" s="15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_3point0_emc_name
 		trigger = {
@@ -6666,7 +7040,7 @@
 </v>
       </c>
       <c r="AF18" s="15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_3point0_emc_name
 		trigger = {
@@ -6695,7 +7069,7 @@
 </v>
       </c>
       <c r="AG18" s="16" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_3point0_emc_name
 		trigger = {
@@ -6827,32 +7201,32 @@
 </v>
       </c>
       <c r="AH18" s="14" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; L18 &amp; " = { text = " &amp; $AA18 &amp; " }"</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">
 				buy_influence_3point0_emc_1 = { text = buy_influence_3point0_emc_response }</v>
       </c>
       <c r="AI18" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; M18 &amp; " = { text = " &amp; $AA18 &amp; " }"</f>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">
 				buy_influence_3point0_emc_2 = { text = buy_influence_3point0_emc_response }</v>
       </c>
       <c r="AJ18" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; N18 &amp; " = { text = " &amp; $AA18 &amp; " }"</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">
 				buy_influence_3point0_emc_3 = { text = buy_influence_3point0_emc_response }</v>
       </c>
       <c r="AK18" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; O18 &amp; " = { text = " &amp; $AA18 &amp; " }"</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">
 				buy_influence_3point0_emc_4 = { text = buy_influence_3point0_emc_response }</v>
       </c>
       <c r="AL18" s="15" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; P18 &amp; " = { text = " &amp; $AA18 &amp; " }"</f>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">
 				buy_influence_3point0_emc_5 = { text = buy_influence_3point0_emc_response }</v>
       </c>
-      <c r="AM18" s="16" t="str">
-        <f t="shared" si="7"/>
+      <c r="AM18" s="18" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_3point0_emc_1 = { text = buy_influence_3point0_emc_response }
 				buy_influence_3point0_emc_2 = { text = buy_influence_3point0_emc_response }
@@ -6860,8 +7234,76 @@
 				buy_influence_3point0_emc_4 = { text = buy_influence_3point0_emc_response }
 				buy_influence_3point0_emc_5 = { text = buy_influence_3point0_emc_response }</v>
       </c>
+      <c r="AN18" s="14" t="str">
+        <f>newline &amp; space &amp; L18 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y18 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_1_name:0 "$buy_influence_3point0_emc_name$"</v>
+      </c>
+      <c r="AO18" s="15" t="str">
+        <f>newline &amp; space &amp; M18 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y18 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_2_name:0 "$buy_influence_3point0_emc_name$"</v>
+      </c>
+      <c r="AP18" s="15" t="str">
+        <f>newline &amp; space &amp; N18 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y18 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_3_name:0 "$buy_influence_3point0_emc_name$"</v>
+      </c>
+      <c r="AQ18" s="15" t="str">
+        <f>newline &amp; space &amp; O18 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y18 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_4_name:0 "$buy_influence_3point0_emc_name$"</v>
+      </c>
+      <c r="AR18" s="15" t="str">
+        <f>newline &amp; space &amp; P18 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y18 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_5_name:0 "$buy_influence_3point0_emc_name$"</v>
+      </c>
+      <c r="AS18" s="18" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_1_name:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_3point0_emc_2_name:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_3point0_emc_3_name:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_3point0_emc_4_name:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_3point0_emc_5_name:0 "$buy_influence_3point0_emc_name$"</v>
+      </c>
+      <c r="AT18" s="14" t="str">
+        <f>newline &amp; space &amp; L18 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z18 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_1_desc:0 "$buy_influence_3point0_emc_desc$"</v>
+      </c>
+      <c r="AU18" s="15" t="str">
+        <f>newline &amp; space &amp; M18 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z18 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_2_desc:0 "$buy_influence_3point0_emc_desc$"</v>
+      </c>
+      <c r="AV18" s="15" t="str">
+        <f>newline &amp; space &amp; N18 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z18 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_3_desc:0 "$buy_influence_3point0_emc_desc$"</v>
+      </c>
+      <c r="AW18" s="15" t="str">
+        <f>newline &amp; space &amp; O18 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z18 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_4_desc:0 "$buy_influence_3point0_emc_desc$"</v>
+      </c>
+      <c r="AX18" s="15" t="str">
+        <f>newline &amp; space &amp; P18 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z18 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_5_desc:0 "$buy_influence_3point0_emc_desc$"</v>
+      </c>
+      <c r="AY18" s="16" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_1_desc:0 "$buy_influence_3point0_emc_desc$"
+ buy_influence_3point0_emc_2_desc:0 "$buy_influence_3point0_emc_desc$"
+ buy_influence_3point0_emc_3_desc:0 "$buy_influence_3point0_emc_desc$"
+ buy_influence_3point0_emc_4_desc:0 "$buy_influence_3point0_emc_desc$"
+ buy_influence_3point0_emc_5_desc:0 "$buy_influence_3point0_emc_desc$"</v>
+      </c>
     </row>
-    <row r="19" spans="2:39" s="2" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:51" s="2" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="59" t="s">
         <v>14</v>
       </c>
@@ -6872,7 +7314,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>25</v>
       </c>
       <c r="F19" s="61">
@@ -6889,11 +7331,11 @@
         <v>1</v>
       </c>
       <c r="K19" s="19" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>buy_influence_4point0_emc</v>
       </c>
       <c r="L19" s="39" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>buy_influence_4point0_emc_1</v>
       </c>
       <c r="M19" s="40" t="str">
@@ -6922,12 +7364,7 @@
 			has_modifier = buy_influence_4point0_emc_5</v>
       </c>
       <c r="R19" s="26" t="str">
-        <f xml:space="preserve">
-newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$L19
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$M19
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$N19
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$O19
-&amp;newline&amp;tab&amp;tab&amp;"remove_modifier = "&amp;$P19</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">
 		remove_modifier = buy_influence_4point0_emc_1
 		remove_modifier = buy_influence_4point0_emc_2
@@ -6936,14 +7373,7 @@
 		remove_modifier = buy_influence_4point0_emc_5</v>
       </c>
       <c r="S19" s="19" t="str">
-        <f>newline&amp;newline&amp;L19&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D19
-&amp;IF($F19&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F19*$J19*L$8,"")
-&amp;IF($G19&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G19*$J19*L$8,"")
-&amp;IF($H19&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H19*$J19*L$8,"")
-&amp;IF($I19&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I19*$J19*L$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">
 buy_influence_4point0_emc_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6954,14 +7384,7 @@
 }</v>
       </c>
       <c r="T19" s="20" t="str">
-        <f>newline&amp;newline&amp;M19&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D19
-&amp;IF($F19&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F19*$J19*M$8,"")
-&amp;IF($G19&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G19*$J19*M$8,"")
-&amp;IF($H19&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H19*$J19*M$8,"")
-&amp;IF($I19&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I19*$J19*M$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">
 buy_influence_4point0_emc_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6972,14 +7395,7 @@
 }</v>
       </c>
       <c r="U19" s="20" t="str">
-        <f>newline&amp;newline&amp;N19&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D19
-&amp;IF($F19&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F19*$J19*N$8,"")
-&amp;IF($G19&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G19*$J19*N$8,"")
-&amp;IF($H19&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H19*$J19*N$8,"")
-&amp;IF($I19&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I19*$J19*N$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">
 buy_influence_4point0_emc_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6990,14 +7406,7 @@
 }</v>
       </c>
       <c r="V19" s="20" t="str">
-        <f>newline&amp;newline&amp;O19&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D19
-&amp;IF($F19&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F19*$J19*O$8,"")
-&amp;IF($G19&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G19*$J19*O$8,"")
-&amp;IF($H19&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H19*$J19*O$8,"")
-&amp;IF($I19&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I19*$J19*O$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">
 buy_influence_4point0_emc_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -7008,14 +7417,7 @@
 }</v>
       </c>
       <c r="W19" s="23" t="str">
-        <f>newline&amp;newline&amp;P19&amp;" = {"
-&amp;newline&amp;tab&amp;"icon = " &amp; doublequote &amp; "gfx/interface/icons/modifiers/mod_country_previous_deals.dds" &amp; doublequote
-&amp;newline&amp;tab&amp;"country_base_influence_produces_add = "&amp;$D19
-&amp;IF($F19&gt;0,newline&amp;tab&amp;"country_base_energy_produces_add = -"&amp;$F19*$J19*P$8,"")
-&amp;IF($G19&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G19*$J19*P$8,"")
-&amp;IF($H19&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H19*$J19*P$8,"")
-&amp;IF($I19&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I19*$J19*P$8,"")
-&amp;newline&amp;"}"</f>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">
 buy_influence_4point0_emc_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -7026,7 +7428,7 @@
 }</v>
       </c>
       <c r="X19" s="21" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
 buy_influence_4point0_emc_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -7065,19 +7467,19 @@
 }</v>
       </c>
       <c r="Y19" s="26" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>buy_influence_4point0_emc_name</v>
       </c>
       <c r="Z19" s="20" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>buy_influence_4point0_emc_desc</v>
       </c>
       <c r="AA19" s="71" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_4point0_emc_response</v>
       </c>
       <c r="AB19" s="19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_4point0_emc_name
 		trigger = {
@@ -7106,7 +7508,7 @@
 </v>
       </c>
       <c r="AC19" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_4point0_emc_name
 		trigger = {
@@ -7136,7 +7538,7 @@
 </v>
       </c>
       <c r="AD19" s="20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_4point0_emc_name
 		trigger = {
@@ -7166,7 +7568,7 @@
 </v>
       </c>
       <c r="AE19" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_4point0_emc_name
 		trigger = {
@@ -7196,7 +7598,7 @@
 </v>
       </c>
       <c r="AF19" s="20" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_4point0_emc_name
 		trigger = {
@@ -7225,7 +7627,7 @@
 </v>
       </c>
       <c r="AG19" s="21" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="28"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_4point0_emc_name
 		trigger = {
@@ -7357,32 +7759,32 @@
 </v>
       </c>
       <c r="AH19" s="19" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; L19 &amp; " = { text = " &amp; $AA19 &amp; " }"</f>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">
 				buy_influence_4point0_emc_1 = { text = buy_influence_4point0_emc_response }</v>
       </c>
       <c r="AI19" s="20" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; M19 &amp; " = { text = " &amp; $AA19 &amp; " }"</f>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">
 				buy_influence_4point0_emc_2 = { text = buy_influence_4point0_emc_response }</v>
       </c>
       <c r="AJ19" s="20" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; N19 &amp; " = { text = " &amp; $AA19 &amp; " }"</f>
+        <f t="shared" si="15"/>
         <v xml:space="preserve">
 				buy_influence_4point0_emc_3 = { text = buy_influence_4point0_emc_response }</v>
       </c>
       <c r="AK19" s="20" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; O19 &amp; " = { text = " &amp; $AA19 &amp; " }"</f>
+        <f t="shared" si="16"/>
         <v xml:space="preserve">
 				buy_influence_4point0_emc_4 = { text = buy_influence_4point0_emc_response }</v>
       </c>
       <c r="AL19" s="20" t="str">
-        <f>newline &amp; tab &amp; tab &amp; tab &amp; tab &amp; P19 &amp; " = { text = " &amp; $AA19 &amp; " }"</f>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">
 				buy_influence_4point0_emc_5 = { text = buy_influence_4point0_emc_response }</v>
       </c>
-      <c r="AM19" s="21" t="str">
-        <f t="shared" si="7"/>
+      <c r="AM19" s="23" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_4point0_emc_1 = { text = buy_influence_4point0_emc_response }
 				buy_influence_4point0_emc_2 = { text = buy_influence_4point0_emc_response }
@@ -7390,8 +7792,76 @@
 				buy_influence_4point0_emc_4 = { text = buy_influence_4point0_emc_response }
 				buy_influence_4point0_emc_5 = { text = buy_influence_4point0_emc_response }</v>
       </c>
+      <c r="AN19" s="19" t="str">
+        <f>newline &amp; space &amp; L19 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y19 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_1_name:0 "$buy_influence_4point0_emc_name$"</v>
+      </c>
+      <c r="AO19" s="20" t="str">
+        <f>newline &amp; space &amp; M19 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y19 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_2_name:0 "$buy_influence_4point0_emc_name$"</v>
+      </c>
+      <c r="AP19" s="20" t="str">
+        <f>newline &amp; space &amp; N19 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y19 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_3_name:0 "$buy_influence_4point0_emc_name$"</v>
+      </c>
+      <c r="AQ19" s="20" t="str">
+        <f>newline &amp; space &amp; O19 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y19 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_4_name:0 "$buy_influence_4point0_emc_name$"</v>
+      </c>
+      <c r="AR19" s="20" t="str">
+        <f>newline &amp; space &amp; P19 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y19 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_5_name:0 "$buy_influence_4point0_emc_name$"</v>
+      </c>
+      <c r="AS19" s="23" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_1_name:0 "$buy_influence_4point0_emc_name$"
+ buy_influence_4point0_emc_2_name:0 "$buy_influence_4point0_emc_name$"
+ buy_influence_4point0_emc_3_name:0 "$buy_influence_4point0_emc_name$"
+ buy_influence_4point0_emc_4_name:0 "$buy_influence_4point0_emc_name$"
+ buy_influence_4point0_emc_5_name:0 "$buy_influence_4point0_emc_name$"</v>
+      </c>
+      <c r="AT19" s="19" t="str">
+        <f>newline &amp; space &amp; L19 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z19 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_1_desc:0 "$buy_influence_4point0_emc_desc$"</v>
+      </c>
+      <c r="AU19" s="20" t="str">
+        <f>newline &amp; space &amp; M19 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z19 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_2_desc:0 "$buy_influence_4point0_emc_desc$"</v>
+      </c>
+      <c r="AV19" s="20" t="str">
+        <f>newline &amp; space &amp; N19 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z19 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_3_desc:0 "$buy_influence_4point0_emc_desc$"</v>
+      </c>
+      <c r="AW19" s="20" t="str">
+        <f>newline &amp; space &amp; O19 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z19 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_4_desc:0 "$buy_influence_4point0_emc_desc$"</v>
+      </c>
+      <c r="AX19" s="20" t="str">
+        <f>newline &amp; space &amp; P19 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z19 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_5_desc:0 "$buy_influence_4point0_emc_desc$"</v>
+      </c>
+      <c r="AY19" s="21" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_1_desc:0 "$buy_influence_4point0_emc_desc$"
+ buy_influence_4point0_emc_2_desc:0 "$buy_influence_4point0_emc_desc$"
+ buy_influence_4point0_emc_3_desc:0 "$buy_influence_4point0_emc_desc$"
+ buy_influence_4point0_emc_4_desc:0 "$buy_influence_4point0_emc_desc$"
+ buy_influence_4point0_emc_5_desc:0 "$buy_influence_4point0_emc_desc$"</v>
+      </c>
     </row>
-    <row r="20" spans="2:39" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:51" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="Q20" s="11" t="str">
         <f xml:space="preserve">
 tab &amp; tab &amp; "#Generated code: Does the current (country) scope have any of the modifiers added by this mod?"
@@ -7855,11 +8325,11 @@
 	country_base_consumer_goods_produces_add = -300
 }</v>
       </c>
-      <c r="AB20" s="74"/>
-      <c r="AC20" s="74"/>
-      <c r="AD20" s="74"/>
-      <c r="AE20" s="74"/>
-      <c r="AF20" s="74"/>
+      <c r="AB20" s="73"/>
+      <c r="AC20" s="73"/>
+      <c r="AD20" s="73"/>
+      <c r="AE20" s="73"/>
+      <c r="AF20" s="73"/>
       <c r="AG20" s="30" t="str">
         <f>"#################################################################" &amp; newline &amp;
 "# Begin generated code: Purchase options" &amp; newline &amp;
@@ -9346,14 +9816,131 @@
 				buy_influence_4point0_emc_5 = { text = buy_influence_4point0_emc_response }
 				#End of generated code</v>
       </c>
+      <c r="AS20" s="30" t="str">
+        <f>space &amp; "#Generated code: Set modifier names equal to the generic (non-pop-dependent) name for each modifier" &amp;
+CONCATENATE(AS9,AS10,AS11,AS12,AS13,AS14,AS15,AS16,AS17,AS18,AS19)</f>
+        <v xml:space="preserve"> #Generated code: Set modifier names equal to the generic (non-pop-dependent) name for each modifier
+ buy_influence_0point5_e_1_name:0 "$buy_influence_0point5_e_name$"
+ buy_influence_0point5_e_2_name:0 "$buy_influence_0point5_e_name$"
+ buy_influence_0point5_e_3_name:0 "$buy_influence_0point5_e_name$"
+ buy_influence_0point5_e_4_name:0 "$buy_influence_0point5_e_name$"
+ buy_influence_0point5_e_5_name:0 "$buy_influence_0point5_e_name$"
+ buy_influence_1point0_e_1_name:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_e_2_name:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_e_3_name:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_e_4_name:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_e_5_name:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_em_1_name:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point0_em_2_name:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point0_em_3_name:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point0_em_4_name:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point0_em_5_name:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point5_em_1_name:0 "$buy_influence_1point5_em_name$"
+ buy_influence_1point5_em_2_name:0 "$buy_influence_1point5_em_name$"
+ buy_influence_1point5_em_3_name:0 "$buy_influence_1point5_em_name$"
+ buy_influence_1point5_em_4_name:0 "$buy_influence_1point5_em_name$"
+ buy_influence_1point5_em_5_name:0 "$buy_influence_1point5_em_name$"
+ buy_influence_2point0_em_1_name:0 "$buy_influence_2point0_em_name$"
+ buy_influence_2point0_em_2_name:0 "$buy_influence_2point0_em_name$"
+ buy_influence_2point0_em_3_name:0 "$buy_influence_2point0_em_name$"
+ buy_influence_2point0_em_4_name:0 "$buy_influence_2point0_em_name$"
+ buy_influence_2point0_em_5_name:0 "$buy_influence_2point0_em_name$"
+ buy_influence_1point0_mf_1_name:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point0_mf_2_name:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point0_mf_3_name:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point0_mf_4_name:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point0_mf_5_name:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point5_mf_1_name:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_1point5_mf_2_name:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_1point5_mf_3_name:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_1point5_mf_4_name:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_1point5_mf_5_name:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_2point0_mf_1_name:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_mf_2_name:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_mf_3_name:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_mf_4_name:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_mf_5_name:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_emc_1_name:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_2point0_emc_2_name:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_2point0_emc_3_name:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_2point0_emc_4_name:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_2point0_emc_5_name:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_3point0_emc_1_name:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_3point0_emc_2_name:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_3point0_emc_3_name:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_3point0_emc_4_name:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_3point0_emc_5_name:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_4point0_emc_1_name:0 "$buy_influence_4point0_emc_name$"
+ buy_influence_4point0_emc_2_name:0 "$buy_influence_4point0_emc_name$"
+ buy_influence_4point0_emc_3_name:0 "$buy_influence_4point0_emc_name$"
+ buy_influence_4point0_emc_4_name:0 "$buy_influence_4point0_emc_name$"
+ buy_influence_4point0_emc_5_name:0 "$buy_influence_4point0_emc_name$"</v>
+      </c>
+      <c r="AY20" s="30" t="str">
+        <f>space &amp; "#Generated code: Set modifier descriptions equal to the generic (non-pop-dependent) description for each modifier" &amp;
+CONCATENATE(AY9,AY10,AY11,AY12,AY13,AY14,AY15,AY16,AY17,AY18,AY19)</f>
+        <v xml:space="preserve"> #Generated code: Set modifier descriptions equal to the generic (non-pop-dependent) description for each modifier
+ buy_influence_0point5_e_1_desc:0 "$buy_influence_0point5_e_desc$"
+ buy_influence_0point5_e_2_desc:0 "$buy_influence_0point5_e_desc$"
+ buy_influence_0point5_e_3_desc:0 "$buy_influence_0point5_e_desc$"
+ buy_influence_0point5_e_4_desc:0 "$buy_influence_0point5_e_desc$"
+ buy_influence_0point5_e_5_desc:0 "$buy_influence_0point5_e_desc$"
+ buy_influence_1point0_e_1_desc:0 "$buy_influence_1point0_e_desc$"
+ buy_influence_1point0_e_2_desc:0 "$buy_influence_1point0_e_desc$"
+ buy_influence_1point0_e_3_desc:0 "$buy_influence_1point0_e_desc$"
+ buy_influence_1point0_e_4_desc:0 "$buy_influence_1point0_e_desc$"
+ buy_influence_1point0_e_5_desc:0 "$buy_influence_1point0_e_desc$"
+ buy_influence_1point0_em_1_desc:0 "$buy_influence_1point0_em_desc$"
+ buy_influence_1point0_em_2_desc:0 "$buy_influence_1point0_em_desc$"
+ buy_influence_1point0_em_3_desc:0 "$buy_influence_1point0_em_desc$"
+ buy_influence_1point0_em_4_desc:0 "$buy_influence_1point0_em_desc$"
+ buy_influence_1point0_em_5_desc:0 "$buy_influence_1point0_em_desc$"
+ buy_influence_1point5_em_1_desc:0 "$buy_influence_1point5_em_desc$"
+ buy_influence_1point5_em_2_desc:0 "$buy_influence_1point5_em_desc$"
+ buy_influence_1point5_em_3_desc:0 "$buy_influence_1point5_em_desc$"
+ buy_influence_1point5_em_4_desc:0 "$buy_influence_1point5_em_desc$"
+ buy_influence_1point5_em_5_desc:0 "$buy_influence_1point5_em_desc$"
+ buy_influence_2point0_em_1_desc:0 "$buy_influence_2point0_em_desc$"
+ buy_influence_2point0_em_2_desc:0 "$buy_influence_2point0_em_desc$"
+ buy_influence_2point0_em_3_desc:0 "$buy_influence_2point0_em_desc$"
+ buy_influence_2point0_em_4_desc:0 "$buy_influence_2point0_em_desc$"
+ buy_influence_2point0_em_5_desc:0 "$buy_influence_2point0_em_desc$"
+ buy_influence_1point0_mf_1_desc:0 "$buy_influence_1point0_mf_desc$"
+ buy_influence_1point0_mf_2_desc:0 "$buy_influence_1point0_mf_desc$"
+ buy_influence_1point0_mf_3_desc:0 "$buy_influence_1point0_mf_desc$"
+ buy_influence_1point0_mf_4_desc:0 "$buy_influence_1point0_mf_desc$"
+ buy_influence_1point0_mf_5_desc:0 "$buy_influence_1point0_mf_desc$"
+ buy_influence_1point5_mf_1_desc:0 "$buy_influence_1point5_mf_desc$"
+ buy_influence_1point5_mf_2_desc:0 "$buy_influence_1point5_mf_desc$"
+ buy_influence_1point5_mf_3_desc:0 "$buy_influence_1point5_mf_desc$"
+ buy_influence_1point5_mf_4_desc:0 "$buy_influence_1point5_mf_desc$"
+ buy_influence_1point5_mf_5_desc:0 "$buy_influence_1point5_mf_desc$"
+ buy_influence_2point0_mf_1_desc:0 "$buy_influence_2point0_mf_desc$"
+ buy_influence_2point0_mf_2_desc:0 "$buy_influence_2point0_mf_desc$"
+ buy_influence_2point0_mf_3_desc:0 "$buy_influence_2point0_mf_desc$"
+ buy_influence_2point0_mf_4_desc:0 "$buy_influence_2point0_mf_desc$"
+ buy_influence_2point0_mf_5_desc:0 "$buy_influence_2point0_mf_desc$"
+ buy_influence_2point0_emc_1_desc:0 "$buy_influence_2point0_emc_desc$"
+ buy_influence_2point0_emc_2_desc:0 "$buy_influence_2point0_emc_desc$"
+ buy_influence_2point0_emc_3_desc:0 "$buy_influence_2point0_emc_desc$"
+ buy_influence_2point0_emc_4_desc:0 "$buy_influence_2point0_emc_desc$"
+ buy_influence_2point0_emc_5_desc:0 "$buy_influence_2point0_emc_desc$"
+ buy_influence_3point0_emc_1_desc:0 "$buy_influence_3point0_emc_desc$"
+ buy_influence_3point0_emc_2_desc:0 "$buy_influence_3point0_emc_desc$"
+ buy_influence_3point0_emc_3_desc:0 "$buy_influence_3point0_emc_desc$"
+ buy_influence_3point0_emc_4_desc:0 "$buy_influence_3point0_emc_desc$"
+ buy_influence_3point0_emc_5_desc:0 "$buy_influence_3point0_emc_desc$"
+ buy_influence_4point0_emc_1_desc:0 "$buy_influence_4point0_emc_desc$"
+ buy_influence_4point0_emc_2_desc:0 "$buy_influence_4point0_emc_desc$"
+ buy_influence_4point0_emc_3_desc:0 "$buy_influence_4point0_emc_desc$"
+ buy_influence_4point0_emc_4_desc:0 "$buy_influence_4point0_emc_desc$"
+ buy_influence_4point0_emc_5_desc:0 "$buy_influence_4point0_emc_desc$"</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="AH6:AM7"/>
-    <mergeCell ref="AB6:AG7"/>
-    <mergeCell ref="Y6:AA7"/>
-    <mergeCell ref="K6:P7"/>
-    <mergeCell ref="E6:E8"/>
+  <mergeCells count="15">
+    <mergeCell ref="AN6:AS7"/>
+    <mergeCell ref="AT6:AY7"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="S6:X7"/>
     <mergeCell ref="Q6:Q8"/>
@@ -9362,6 +9949,11 @@
     <mergeCell ref="D6:D8"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="R6:R8"/>
+    <mergeCell ref="AH6:AM7"/>
+    <mergeCell ref="AB6:AG7"/>
+    <mergeCell ref="Y6:AA7"/>
+    <mergeCell ref="K6:P7"/>
+    <mergeCell ref="E6:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Buy Influence: Further localisation updates; (hopefully) fixed the flags controlling purchase screen text; added reselect option after purchase
</commit_message>
<xml_diff>
--- a/buy_influence/CodeGen.xlsx
+++ b/buy_influence/CodeGen.xlsx
@@ -240,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -768,17 +768,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -949,6 +938,51 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -994,52 +1028,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1343,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AY20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AS20" sqref="AS20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
@@ -1363,9 +1352,8 @@
     <col min="33" max="33" width="9.06640625" style="1" collapsed="1"/>
     <col min="34" max="38" width="9.06640625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="39" max="39" width="9.06640625" style="1" collapsed="1"/>
-    <col min="40" max="44" width="0" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="9.06640625" style="1" collapsed="1"/>
-    <col min="46" max="16384" width="9.06640625" style="1"/>
+    <col min="40" max="44" width="9.06640625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:51" x14ac:dyDescent="0.45">
@@ -1493,144 +1481,144 @@
     </row>
     <row r="5" spans="2:51" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="6" spans="2:51" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="89" t="s">
+      <c r="C6" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="89" t="s">
+      <c r="D6" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="89" t="s">
+      <c r="E6" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="75" t="s">
+      <c r="F6" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="76"/>
-      <c r="J6" s="89" t="s">
+      <c r="G6" s="90"/>
+      <c r="H6" s="90"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="74" t="s">
+      <c r="K6" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="75"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="75"/>
-      <c r="O6" s="75"/>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="89" t="s">
+      <c r="L6" s="90"/>
+      <c r="M6" s="90"/>
+      <c r="N6" s="90"/>
+      <c r="O6" s="90"/>
+      <c r="P6" s="91"/>
+      <c r="Q6" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="R6" s="89" t="s">
+      <c r="R6" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="S6" s="74" t="s">
+      <c r="S6" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="T6" s="75"/>
-      <c r="U6" s="75"/>
-      <c r="V6" s="75"/>
-      <c r="W6" s="75"/>
-      <c r="X6" s="76"/>
-      <c r="Y6" s="74" t="s">
+      <c r="T6" s="90"/>
+      <c r="U6" s="90"/>
+      <c r="V6" s="90"/>
+      <c r="W6" s="90"/>
+      <c r="X6" s="91"/>
+      <c r="Y6" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="Z6" s="75"/>
-      <c r="AA6" s="76"/>
-      <c r="AB6" s="80" t="s">
+      <c r="Z6" s="90"/>
+      <c r="AA6" s="91"/>
+      <c r="AB6" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="AC6" s="81"/>
-      <c r="AD6" s="81"/>
-      <c r="AE6" s="81"/>
-      <c r="AF6" s="81"/>
-      <c r="AG6" s="82"/>
-      <c r="AH6" s="74" t="s">
+      <c r="AC6" s="96"/>
+      <c r="AD6" s="96"/>
+      <c r="AE6" s="96"/>
+      <c r="AF6" s="96"/>
+      <c r="AG6" s="97"/>
+      <c r="AH6" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="AI6" s="75"/>
-      <c r="AJ6" s="75"/>
-      <c r="AK6" s="75"/>
-      <c r="AL6" s="75"/>
-      <c r="AM6" s="75"/>
-      <c r="AN6" s="95" t="s">
+      <c r="AI6" s="90"/>
+      <c r="AJ6" s="90"/>
+      <c r="AK6" s="90"/>
+      <c r="AL6" s="90"/>
+      <c r="AM6" s="91"/>
+      <c r="AN6" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="AO6" s="96"/>
-      <c r="AP6" s="96"/>
-      <c r="AQ6" s="96"/>
-      <c r="AR6" s="96"/>
-      <c r="AS6" s="102"/>
-      <c r="AT6" s="95" t="s">
+      <c r="AO6" s="79"/>
+      <c r="AP6" s="79"/>
+      <c r="AQ6" s="79"/>
+      <c r="AR6" s="79"/>
+      <c r="AS6" s="80"/>
+      <c r="AT6" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="AU6" s="96"/>
-      <c r="AV6" s="96"/>
-      <c r="AW6" s="96"/>
-      <c r="AX6" s="96"/>
-      <c r="AY6" s="97"/>
+      <c r="AU6" s="79"/>
+      <c r="AV6" s="79"/>
+      <c r="AW6" s="79"/>
+      <c r="AX6" s="79"/>
+      <c r="AY6" s="84"/>
     </row>
     <row r="7" spans="2:51" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="90"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="86"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="87"/>
-      <c r="N7" s="87"/>
-      <c r="O7" s="87"/>
-      <c r="P7" s="88"/>
-      <c r="Q7" s="90"/>
-      <c r="R7" s="90"/>
-      <c r="S7" s="77"/>
-      <c r="T7" s="78"/>
-      <c r="U7" s="78"/>
-      <c r="V7" s="78"/>
-      <c r="W7" s="78"/>
-      <c r="X7" s="79"/>
-      <c r="Y7" s="77"/>
-      <c r="Z7" s="78"/>
-      <c r="AA7" s="79"/>
-      <c r="AB7" s="83"/>
-      <c r="AC7" s="84"/>
-      <c r="AD7" s="84"/>
-      <c r="AE7" s="84"/>
-      <c r="AF7" s="84"/>
-      <c r="AG7" s="85"/>
-      <c r="AH7" s="77"/>
-      <c r="AI7" s="78"/>
-      <c r="AJ7" s="78"/>
-      <c r="AK7" s="78"/>
-      <c r="AL7" s="78"/>
-      <c r="AM7" s="78"/>
-      <c r="AN7" s="98"/>
-      <c r="AO7" s="93"/>
-      <c r="AP7" s="93"/>
-      <c r="AQ7" s="93"/>
-      <c r="AR7" s="93"/>
-      <c r="AS7" s="103"/>
-      <c r="AT7" s="98"/>
-      <c r="AU7" s="93"/>
-      <c r="AV7" s="93"/>
-      <c r="AW7" s="93"/>
-      <c r="AX7" s="93"/>
-      <c r="AY7" s="99"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="93"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="102"/>
+      <c r="M7" s="102"/>
+      <c r="N7" s="102"/>
+      <c r="O7" s="102"/>
+      <c r="P7" s="103"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
+      <c r="S7" s="92"/>
+      <c r="T7" s="93"/>
+      <c r="U7" s="93"/>
+      <c r="V7" s="93"/>
+      <c r="W7" s="93"/>
+      <c r="X7" s="94"/>
+      <c r="Y7" s="92"/>
+      <c r="Z7" s="93"/>
+      <c r="AA7" s="94"/>
+      <c r="AB7" s="98"/>
+      <c r="AC7" s="99"/>
+      <c r="AD7" s="99"/>
+      <c r="AE7" s="99"/>
+      <c r="AF7" s="99"/>
+      <c r="AG7" s="100"/>
+      <c r="AH7" s="92"/>
+      <c r="AI7" s="93"/>
+      <c r="AJ7" s="93"/>
+      <c r="AK7" s="93"/>
+      <c r="AL7" s="93"/>
+      <c r="AM7" s="94"/>
+      <c r="AN7" s="81"/>
+      <c r="AO7" s="82"/>
+      <c r="AP7" s="82"/>
+      <c r="AQ7" s="82"/>
+      <c r="AR7" s="82"/>
+      <c r="AS7" s="83"/>
+      <c r="AT7" s="81"/>
+      <c r="AU7" s="82"/>
+      <c r="AV7" s="82"/>
+      <c r="AW7" s="82"/>
+      <c r="AX7" s="82"/>
+      <c r="AY7" s="85"/>
     </row>
     <row r="8" spans="2:51" s="3" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="91"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="91"/>
-      <c r="E8" s="91"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
       <c r="F8" s="31" t="s">
         <v>4</v>
       </c>
@@ -1643,7 +1631,7 @@
       <c r="I8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="91"/>
+      <c r="J8" s="88"/>
       <c r="K8" s="9" t="s">
         <v>29</v>
       </c>
@@ -1662,8 +1650,8 @@
       <c r="P8" s="7">
         <v>5</v>
       </c>
-      <c r="Q8" s="91"/>
-      <c r="R8" s="91"/>
+      <c r="Q8" s="88"/>
+      <c r="R8" s="88"/>
       <c r="S8" s="9">
         <f>L8</f>
         <v>1</v>
@@ -1729,43 +1717,43 @@
       <c r="AL8" s="4">
         <v>5</v>
       </c>
-      <c r="AM8" s="10" t="s">
+      <c r="AM8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AN8" s="100">
+      <c r="AN8" s="75">
         <v>1</v>
       </c>
-      <c r="AO8" s="94">
+      <c r="AO8" s="74">
         <v>2</v>
       </c>
-      <c r="AP8" s="94">
+      <c r="AP8" s="74">
         <v>3</v>
       </c>
-      <c r="AQ8" s="94">
+      <c r="AQ8" s="74">
         <v>4</v>
       </c>
-      <c r="AR8" s="94">
+      <c r="AR8" s="74">
         <v>5</v>
       </c>
-      <c r="AS8" s="104" t="s">
+      <c r="AS8" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="AT8" s="100">
+      <c r="AT8" s="75">
         <v>1</v>
       </c>
-      <c r="AU8" s="94">
+      <c r="AU8" s="74">
         <v>2</v>
       </c>
-      <c r="AV8" s="94">
+      <c r="AV8" s="74">
         <v>3</v>
       </c>
-      <c r="AW8" s="94">
+      <c r="AW8" s="74">
         <v>4</v>
       </c>
-      <c r="AX8" s="94">
+      <c r="AX8" s="74">
         <v>5</v>
       </c>
-      <c r="AY8" s="101" t="s">
+      <c r="AY8" s="76" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2299,7 +2287,7 @@
         <v xml:space="preserve">
 				buy_influence_0point5_e_5 = { text = buy_influence_0point5_e_response }</v>
       </c>
-      <c r="AM9" s="92" t="str">
+      <c r="AM9" s="104" t="str">
         <f t="shared" ref="AM9:AM19" si="18">CONCATENATE(AH9,AI9,AJ9,AK9,AL9)</f>
         <v xml:space="preserve">
 				buy_influence_0point5_e_1 = { text = buy_influence_0point5_e_response }
@@ -2309,66 +2297,66 @@
 				buy_influence_0point5_e_5 = { text = buy_influence_0point5_e_response }</v>
       </c>
       <c r="AN9" s="14" t="str">
-        <f>newline &amp; space &amp; L9 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y9 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_0point5_e_1_name:0 "$buy_influence_0point5_e_name$"</v>
+        <f>newline &amp; space &amp; L9 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y9 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_1:0 "$buy_influence_0point5_e_name$"</v>
       </c>
       <c r="AO9" s="15" t="str">
-        <f>newline &amp; space &amp; M9 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y9 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_0point5_e_2_name:0 "$buy_influence_0point5_e_name$"</v>
+        <f>newline &amp; space &amp; M9 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y9 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_2:0 "$buy_influence_0point5_e_name$"</v>
       </c>
       <c r="AP9" s="15" t="str">
-        <f>newline &amp; space &amp; N9 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y9 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_0point5_e_3_name:0 "$buy_influence_0point5_e_name$"</v>
+        <f>newline &amp; space &amp; N9 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y9 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_3:0 "$buy_influence_0point5_e_name$"</v>
       </c>
       <c r="AQ9" s="15" t="str">
-        <f>newline &amp; space &amp; O9 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y9 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_0point5_e_4_name:0 "$buy_influence_0point5_e_name$"</v>
+        <f>newline &amp; space &amp; O9 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y9 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_4:0 "$buy_influence_0point5_e_name$"</v>
       </c>
       <c r="AR9" s="15" t="str">
-        <f>newline &amp; space &amp; P9 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y9 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_0point5_e_5_name:0 "$buy_influence_0point5_e_name$"</v>
+        <f>newline &amp; space &amp; P9 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y9 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_0point5_e_5:0 "$buy_influence_0point5_e_name$"</v>
       </c>
       <c r="AS9" s="18" t="str">
         <f t="shared" ref="AS9:AS19" si="19">CONCATENATE(AN9,AO9,AP9,AQ9,AR9)</f>
         <v xml:space="preserve">
- buy_influence_0point5_e_1_name:0 "$buy_influence_0point5_e_name$"
- buy_influence_0point5_e_2_name:0 "$buy_influence_0point5_e_name$"
- buy_influence_0point5_e_3_name:0 "$buy_influence_0point5_e_name$"
- buy_influence_0point5_e_4_name:0 "$buy_influence_0point5_e_name$"
- buy_influence_0point5_e_5_name:0 "$buy_influence_0point5_e_name$"</v>
+ buy_influence_0point5_e_1:0 "$buy_influence_0point5_e_name$"
+ buy_influence_0point5_e_2:0 "$buy_influence_0point5_e_name$"
+ buy_influence_0point5_e_3:0 "$buy_influence_0point5_e_name$"
+ buy_influence_0point5_e_4:0 "$buy_influence_0point5_e_name$"
+ buy_influence_0point5_e_5:0 "$buy_influence_0point5_e_name$"</v>
       </c>
       <c r="AT9" s="14" t="str">
-        <f>newline &amp; space &amp; L9 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z9 &amp; "$" &amp; doublequote</f>
+        <f t="shared" ref="AT9:AT19" si="20">newline &amp; space &amp; L9 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z9 &amp; "$" &amp; doublequote</f>
         <v xml:space="preserve">
  buy_influence_0point5_e_1_desc:0 "$buy_influence_0point5_e_desc$"</v>
       </c>
       <c r="AU9" s="15" t="str">
-        <f>newline &amp; space &amp; M9 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z9 &amp; "$" &amp; doublequote</f>
+        <f t="shared" ref="AU9:AU19" si="21">newline &amp; space &amp; M9 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z9 &amp; "$" &amp; doublequote</f>
         <v xml:space="preserve">
  buy_influence_0point5_e_2_desc:0 "$buy_influence_0point5_e_desc$"</v>
       </c>
       <c r="AV9" s="15" t="str">
-        <f>newline &amp; space &amp; N9 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z9 &amp; "$" &amp; doublequote</f>
+        <f t="shared" ref="AV9:AV19" si="22">newline &amp; space &amp; N9 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z9 &amp; "$" &amp; doublequote</f>
         <v xml:space="preserve">
  buy_influence_0point5_e_3_desc:0 "$buy_influence_0point5_e_desc$"</v>
       </c>
       <c r="AW9" s="15" t="str">
-        <f>newline &amp; space &amp; O9 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z9 &amp; "$" &amp; doublequote</f>
+        <f t="shared" ref="AW9:AW19" si="23">newline &amp; space &amp; O9 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z9 &amp; "$" &amp; doublequote</f>
         <v xml:space="preserve">
  buy_influence_0point5_e_4_desc:0 "$buy_influence_0point5_e_desc$"</v>
       </c>
       <c r="AX9" s="15" t="str">
-        <f>newline &amp; space &amp; P9 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z9 &amp; "$" &amp; doublequote</f>
+        <f t="shared" ref="AX9:AX19" si="24">newline &amp; space &amp; P9 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z9 &amp; "$" &amp; doublequote</f>
         <v xml:space="preserve">
  buy_influence_0point5_e_5_desc:0 "$buy_influence_0point5_e_desc$"</v>
       </c>
       <c r="AY9" s="16" t="str">
-        <f t="shared" ref="AY9:AY19" si="20">CONCATENATE(AT9,AU9,AV9,AW9,AX9)</f>
+        <f t="shared" ref="AY9:AY19" si="25">CONCATENATE(AT9,AU9,AV9,AW9,AX9)</f>
         <v xml:space="preserve">
  buy_influence_0point5_e_1_desc:0 "$buy_influence_0point5_e_desc$"
  buy_influence_0point5_e_2_desc:0 "$buy_influence_0point5_e_desc$"
@@ -2388,7 +2376,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="43">
-        <f t="shared" ref="E10:E19" si="21">MIN(25,10*D10)</f>
+        <f t="shared" ref="E10:E19" si="26">MIN(25,10*D10)</f>
         <v>10</v>
       </c>
       <c r="F10" s="57">
@@ -2401,11 +2389,11 @@
         <v>1</v>
       </c>
       <c r="K10" s="14" t="str">
-        <f t="shared" ref="K10:K19" si="22">"buy_influence_"&amp;ROUNDDOWN($D10,0)&amp;"point"&amp;(ROUNDDOWN($D10*10,0)-(ROUNDDOWN($D10,0)*10))&amp;"_"&amp;$C10</f>
+        <f t="shared" ref="K10:K19" si="27">"buy_influence_"&amp;ROUNDDOWN($D10,0)&amp;"point"&amp;(ROUNDDOWN($D10*10,0)-(ROUNDDOWN($D10,0)*10))&amp;"_"&amp;$C10</f>
         <v>buy_influence_1point0_e</v>
       </c>
       <c r="L10" s="36" t="str">
-        <f t="shared" ref="L10:L19" si="23">$K10&amp;"_"&amp;L$8</f>
+        <f t="shared" ref="L10:L19" si="28">$K10&amp;"_"&amp;L$8</f>
         <v>buy_influence_1point0_e_1</v>
       </c>
       <c r="M10" s="37" t="str">
@@ -2488,7 +2476,7 @@
 }</v>
       </c>
       <c r="X10" s="16" t="str">
-        <f t="shared" ref="X10:X19" si="24">CONCATENATE(S10,T10,U10,V10,W10)</f>
+        <f t="shared" ref="X10:X19" si="29">CONCATENATE(S10,T10,U10,V10,W10)</f>
         <v xml:space="preserve">
 buy_influence_1point0_e_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -2517,15 +2505,15 @@
 }</v>
       </c>
       <c r="Y10" s="25" t="str">
-        <f t="shared" ref="Y10:Y19" si="25">$K10&amp;"_name"</f>
+        <f t="shared" ref="Y10:Y19" si="30">$K10&amp;"_name"</f>
         <v>buy_influence_1point0_e_name</v>
       </c>
       <c r="Z10" s="15" t="str">
-        <f t="shared" ref="Z10:Z19" si="26">$K10&amp;"_desc"</f>
+        <f t="shared" ref="Z10:Z19" si="31">$K10&amp;"_desc"</f>
         <v>buy_influence_1point0_e_desc</v>
       </c>
       <c r="AA10" s="70" t="str">
-        <f t="shared" ref="AA10:AA19" si="27">$K10&amp;"_response"</f>
+        <f t="shared" ref="AA10:AA19" si="32">$K10&amp;"_response"</f>
         <v>buy_influence_1point0_e_response</v>
       </c>
       <c r="AB10" s="14" t="str">
@@ -2677,7 +2665,7 @@
 </v>
       </c>
       <c r="AG10" s="16" t="str">
-        <f t="shared" ref="AG10:AG19" si="28">CONCATENATE(AB10,AC10,AD10,AE10,AF10)</f>
+        <f t="shared" ref="AG10:AG19" si="33">CONCATENATE(AB10,AC10,AD10,AE10,AF10)</f>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_e_name
 		trigger = {
@@ -2833,7 +2821,7 @@
         <v xml:space="preserve">
 				buy_influence_1point0_e_5 = { text = buy_influence_1point0_e_response }</v>
       </c>
-      <c r="AM10" s="18" t="str">
+      <c r="AM10" s="16" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_1point0_e_1 = { text = buy_influence_1point0_e_response }
@@ -2843,66 +2831,66 @@
 				buy_influence_1point0_e_5 = { text = buy_influence_1point0_e_response }</v>
       </c>
       <c r="AN10" s="14" t="str">
-        <f>newline &amp; space &amp; L10 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y10 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point0_e_1_name:0 "$buy_influence_1point0_e_name$"</v>
+        <f>newline &amp; space &amp; L10 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y10 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_1:0 "$buy_influence_1point0_e_name$"</v>
       </c>
       <c r="AO10" s="15" t="str">
-        <f>newline &amp; space &amp; M10 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y10 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point0_e_2_name:0 "$buy_influence_1point0_e_name$"</v>
+        <f>newline &amp; space &amp; M10 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y10 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_2:0 "$buy_influence_1point0_e_name$"</v>
       </c>
       <c r="AP10" s="15" t="str">
-        <f>newline &amp; space &amp; N10 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y10 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point0_e_3_name:0 "$buy_influence_1point0_e_name$"</v>
+        <f>newline &amp; space &amp; N10 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y10 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_3:0 "$buy_influence_1point0_e_name$"</v>
       </c>
       <c r="AQ10" s="15" t="str">
-        <f>newline &amp; space &amp; O10 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y10 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point0_e_4_name:0 "$buy_influence_1point0_e_name$"</v>
+        <f>newline &amp; space &amp; O10 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y10 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_4:0 "$buy_influence_1point0_e_name$"</v>
       </c>
       <c r="AR10" s="15" t="str">
-        <f>newline &amp; space &amp; P10 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y10 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point0_e_5_name:0 "$buy_influence_1point0_e_name$"</v>
+        <f>newline &amp; space &amp; P10 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y10 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_e_5:0 "$buy_influence_1point0_e_name$"</v>
       </c>
       <c r="AS10" s="18" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">
- buy_influence_1point0_e_1_name:0 "$buy_influence_1point0_e_name$"
- buy_influence_1point0_e_2_name:0 "$buy_influence_1point0_e_name$"
- buy_influence_1point0_e_3_name:0 "$buy_influence_1point0_e_name$"
- buy_influence_1point0_e_4_name:0 "$buy_influence_1point0_e_name$"
- buy_influence_1point0_e_5_name:0 "$buy_influence_1point0_e_name$"</v>
+ buy_influence_1point0_e_1:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_e_2:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_e_3:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_e_4:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_e_5:0 "$buy_influence_1point0_e_name$"</v>
       </c>
       <c r="AT10" s="14" t="str">
-        <f>newline &amp; space &amp; L10 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z10 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">
  buy_influence_1point0_e_1_desc:0 "$buy_influence_1point0_e_desc$"</v>
       </c>
       <c r="AU10" s="15" t="str">
-        <f>newline &amp; space &amp; M10 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z10 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">
  buy_influence_1point0_e_2_desc:0 "$buy_influence_1point0_e_desc$"</v>
       </c>
       <c r="AV10" s="15" t="str">
-        <f>newline &amp; space &amp; N10 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z10 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="22"/>
         <v xml:space="preserve">
  buy_influence_1point0_e_3_desc:0 "$buy_influence_1point0_e_desc$"</v>
       </c>
       <c r="AW10" s="15" t="str">
-        <f>newline &amp; space &amp; O10 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z10 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="23"/>
         <v xml:space="preserve">
  buy_influence_1point0_e_4_desc:0 "$buy_influence_1point0_e_desc$"</v>
       </c>
       <c r="AX10" s="15" t="str">
-        <f>newline &amp; space &amp; P10 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z10 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
  buy_influence_1point0_e_5_desc:0 "$buy_influence_1point0_e_desc$"</v>
       </c>
       <c r="AY10" s="16" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v xml:space="preserve">
  buy_influence_1point0_e_1_desc:0 "$buy_influence_1point0_e_desc$"
  buy_influence_1point0_e_2_desc:0 "$buy_influence_1point0_e_desc$"
@@ -2922,7 +2910,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="43">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="F11" s="57">
@@ -2937,11 +2925,11 @@
         <v>1</v>
       </c>
       <c r="K11" s="14" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_1point0_em</v>
       </c>
       <c r="L11" s="36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>buy_influence_1point0_em_1</v>
       </c>
       <c r="M11" s="37" t="str">
@@ -3029,7 +3017,7 @@
 }</v>
       </c>
       <c r="X11" s="16" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">
 buy_influence_1point0_em_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -3063,15 +3051,15 @@
 }</v>
       </c>
       <c r="Y11" s="25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>buy_influence_1point0_em_name</v>
       </c>
       <c r="Z11" s="15" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>buy_influence_1point0_em_desc</v>
       </c>
       <c r="AA11" s="70" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>buy_influence_1point0_em_response</v>
       </c>
       <c r="AB11" s="14" t="str">
@@ -3223,7 +3211,7 @@
 </v>
       </c>
       <c r="AG11" s="16" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_em_name
 		trigger = {
@@ -3379,7 +3367,7 @@
         <v xml:space="preserve">
 				buy_influence_1point0_em_5 = { text = buy_influence_1point0_em_response }</v>
       </c>
-      <c r="AM11" s="18" t="str">
+      <c r="AM11" s="16" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_1point0_em_1 = { text = buy_influence_1point0_em_response }
@@ -3389,66 +3377,66 @@
 				buy_influence_1point0_em_5 = { text = buy_influence_1point0_em_response }</v>
       </c>
       <c r="AN11" s="14" t="str">
-        <f>newline &amp; space &amp; L11 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y11 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point0_em_1_name:0 "$buy_influence_1point0_em_name$"</v>
+        <f>newline &amp; space &amp; L11 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y11 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_1:0 "$buy_influence_1point0_em_name$"</v>
       </c>
       <c r="AO11" s="15" t="str">
-        <f>newline &amp; space &amp; M11 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y11 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point0_em_2_name:0 "$buy_influence_1point0_em_name$"</v>
+        <f>newline &amp; space &amp; M11 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y11 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_2:0 "$buy_influence_1point0_em_name$"</v>
       </c>
       <c r="AP11" s="15" t="str">
-        <f>newline &amp; space &amp; N11 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y11 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point0_em_3_name:0 "$buy_influence_1point0_em_name$"</v>
+        <f>newline &amp; space &amp; N11 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y11 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_3:0 "$buy_influence_1point0_em_name$"</v>
       </c>
       <c r="AQ11" s="15" t="str">
-        <f>newline &amp; space &amp; O11 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y11 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point0_em_4_name:0 "$buy_influence_1point0_em_name$"</v>
+        <f>newline &amp; space &amp; O11 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y11 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_4:0 "$buy_influence_1point0_em_name$"</v>
       </c>
       <c r="AR11" s="15" t="str">
-        <f>newline &amp; space &amp; P11 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y11 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point0_em_5_name:0 "$buy_influence_1point0_em_name$"</v>
+        <f>newline &amp; space &amp; P11 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y11 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_em_5:0 "$buy_influence_1point0_em_name$"</v>
       </c>
       <c r="AS11" s="18" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">
- buy_influence_1point0_em_1_name:0 "$buy_influence_1point0_em_name$"
- buy_influence_1point0_em_2_name:0 "$buy_influence_1point0_em_name$"
- buy_influence_1point0_em_3_name:0 "$buy_influence_1point0_em_name$"
- buy_influence_1point0_em_4_name:0 "$buy_influence_1point0_em_name$"
- buy_influence_1point0_em_5_name:0 "$buy_influence_1point0_em_name$"</v>
+ buy_influence_1point0_em_1:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point0_em_2:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point0_em_3:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point0_em_4:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point0_em_5:0 "$buy_influence_1point0_em_name$"</v>
       </c>
       <c r="AT11" s="14" t="str">
-        <f>newline &amp; space &amp; L11 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z11 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">
  buy_influence_1point0_em_1_desc:0 "$buy_influence_1point0_em_desc$"</v>
       </c>
       <c r="AU11" s="15" t="str">
-        <f>newline &amp; space &amp; M11 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z11 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">
  buy_influence_1point0_em_2_desc:0 "$buy_influence_1point0_em_desc$"</v>
       </c>
       <c r="AV11" s="15" t="str">
-        <f>newline &amp; space &amp; N11 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z11 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="22"/>
         <v xml:space="preserve">
  buy_influence_1point0_em_3_desc:0 "$buy_influence_1point0_em_desc$"</v>
       </c>
       <c r="AW11" s="15" t="str">
-        <f>newline &amp; space &amp; O11 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z11 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="23"/>
         <v xml:space="preserve">
  buy_influence_1point0_em_4_desc:0 "$buy_influence_1point0_em_desc$"</v>
       </c>
       <c r="AX11" s="15" t="str">
-        <f>newline &amp; space &amp; P11 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z11 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
  buy_influence_1point0_em_5_desc:0 "$buy_influence_1point0_em_desc$"</v>
       </c>
       <c r="AY11" s="16" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v xml:space="preserve">
  buy_influence_1point0_em_1_desc:0 "$buy_influence_1point0_em_desc$"
  buy_influence_1point0_em_2_desc:0 "$buy_influence_1point0_em_desc$"
@@ -3468,7 +3456,7 @@
         <v>1.5</v>
       </c>
       <c r="E12" s="43">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>15</v>
       </c>
       <c r="F12" s="57">
@@ -3483,11 +3471,11 @@
         <v>1</v>
       </c>
       <c r="K12" s="14" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_1point5_em</v>
       </c>
       <c r="L12" s="36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>buy_influence_1point5_em_1</v>
       </c>
       <c r="M12" s="37" t="str">
@@ -3575,7 +3563,7 @@
 }</v>
       </c>
       <c r="X12" s="16" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">
 buy_influence_1point5_em_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -3609,15 +3597,15 @@
 }</v>
       </c>
       <c r="Y12" s="25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>buy_influence_1point5_em_name</v>
       </c>
       <c r="Z12" s="15" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>buy_influence_1point5_em_desc</v>
       </c>
       <c r="AA12" s="70" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>buy_influence_1point5_em_response</v>
       </c>
       <c r="AB12" s="14" t="str">
@@ -3769,7 +3757,7 @@
 </v>
       </c>
       <c r="AG12" s="16" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point5_em_name
 		trigger = {
@@ -3925,7 +3913,7 @@
         <v xml:space="preserve">
 				buy_influence_1point5_em_5 = { text = buy_influence_1point5_em_response }</v>
       </c>
-      <c r="AM12" s="18" t="str">
+      <c r="AM12" s="16" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_1point5_em_1 = { text = buy_influence_1point5_em_response }
@@ -3935,66 +3923,66 @@
 				buy_influence_1point5_em_5 = { text = buy_influence_1point5_em_response }</v>
       </c>
       <c r="AN12" s="14" t="str">
-        <f>newline &amp; space &amp; L12 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y12 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point5_em_1_name:0 "$buy_influence_1point5_em_name$"</v>
+        <f>newline &amp; space &amp; L12 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y12 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_1:0 "$buy_influence_1point5_em_name$"</v>
       </c>
       <c r="AO12" s="15" t="str">
-        <f>newline &amp; space &amp; M12 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y12 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point5_em_2_name:0 "$buy_influence_1point5_em_name$"</v>
+        <f>newline &amp; space &amp; M12 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y12 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_2:0 "$buy_influence_1point5_em_name$"</v>
       </c>
       <c r="AP12" s="15" t="str">
-        <f>newline &amp; space &amp; N12 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y12 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point5_em_3_name:0 "$buy_influence_1point5_em_name$"</v>
+        <f>newline &amp; space &amp; N12 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y12 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_3:0 "$buy_influence_1point5_em_name$"</v>
       </c>
       <c r="AQ12" s="15" t="str">
-        <f>newline &amp; space &amp; O12 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y12 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point5_em_4_name:0 "$buy_influence_1point5_em_name$"</v>
+        <f>newline &amp; space &amp; O12 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y12 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_4:0 "$buy_influence_1point5_em_name$"</v>
       </c>
       <c r="AR12" s="15" t="str">
-        <f>newline &amp; space &amp; P12 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y12 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point5_em_5_name:0 "$buy_influence_1point5_em_name$"</v>
+        <f>newline &amp; space &amp; P12 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y12 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_em_5:0 "$buy_influence_1point5_em_name$"</v>
       </c>
       <c r="AS12" s="18" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">
- buy_influence_1point5_em_1_name:0 "$buy_influence_1point5_em_name$"
- buy_influence_1point5_em_2_name:0 "$buy_influence_1point5_em_name$"
- buy_influence_1point5_em_3_name:0 "$buy_influence_1point5_em_name$"
- buy_influence_1point5_em_4_name:0 "$buy_influence_1point5_em_name$"
- buy_influence_1point5_em_5_name:0 "$buy_influence_1point5_em_name$"</v>
+ buy_influence_1point5_em_1:0 "$buy_influence_1point5_em_name$"
+ buy_influence_1point5_em_2:0 "$buy_influence_1point5_em_name$"
+ buy_influence_1point5_em_3:0 "$buy_influence_1point5_em_name$"
+ buy_influence_1point5_em_4:0 "$buy_influence_1point5_em_name$"
+ buy_influence_1point5_em_5:0 "$buy_influence_1point5_em_name$"</v>
       </c>
       <c r="AT12" s="14" t="str">
-        <f>newline &amp; space &amp; L12 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z12 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">
  buy_influence_1point5_em_1_desc:0 "$buy_influence_1point5_em_desc$"</v>
       </c>
       <c r="AU12" s="15" t="str">
-        <f>newline &amp; space &amp; M12 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z12 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">
  buy_influence_1point5_em_2_desc:0 "$buy_influence_1point5_em_desc$"</v>
       </c>
       <c r="AV12" s="15" t="str">
-        <f>newline &amp; space &amp; N12 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z12 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="22"/>
         <v xml:space="preserve">
  buy_influence_1point5_em_3_desc:0 "$buy_influence_1point5_em_desc$"</v>
       </c>
       <c r="AW12" s="15" t="str">
-        <f>newline &amp; space &amp; O12 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z12 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="23"/>
         <v xml:space="preserve">
  buy_influence_1point5_em_4_desc:0 "$buy_influence_1point5_em_desc$"</v>
       </c>
       <c r="AX12" s="15" t="str">
-        <f>newline &amp; space &amp; P12 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z12 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
  buy_influence_1point5_em_5_desc:0 "$buy_influence_1point5_em_desc$"</v>
       </c>
       <c r="AY12" s="16" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v xml:space="preserve">
  buy_influence_1point5_em_1_desc:0 "$buy_influence_1point5_em_desc$"
  buy_influence_1point5_em_2_desc:0 "$buy_influence_1point5_em_desc$"
@@ -4014,7 +4002,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="43">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>20</v>
       </c>
       <c r="F13" s="57">
@@ -4029,11 +4017,11 @@
         <v>1</v>
       </c>
       <c r="K13" s="14" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_2point0_em</v>
       </c>
       <c r="L13" s="36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>buy_influence_2point0_em_1</v>
       </c>
       <c r="M13" s="37" t="str">
@@ -4121,7 +4109,7 @@
 }</v>
       </c>
       <c r="X13" s="16" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">
 buy_influence_2point0_em_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -4155,15 +4143,15 @@
 }</v>
       </c>
       <c r="Y13" s="25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>buy_influence_2point0_em_name</v>
       </c>
       <c r="Z13" s="15" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>buy_influence_2point0_em_desc</v>
       </c>
       <c r="AA13" s="70" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>buy_influence_2point0_em_response</v>
       </c>
       <c r="AB13" s="14" t="str">
@@ -4315,7 +4303,7 @@
 </v>
       </c>
       <c r="AG13" s="16" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_em_name
 		trigger = {
@@ -4471,7 +4459,7 @@
         <v xml:space="preserve">
 				buy_influence_2point0_em_5 = { text = buy_influence_2point0_em_response }</v>
       </c>
-      <c r="AM13" s="18" t="str">
+      <c r="AM13" s="16" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_2point0_em_1 = { text = buy_influence_2point0_em_response }
@@ -4481,66 +4469,66 @@
 				buy_influence_2point0_em_5 = { text = buy_influence_2point0_em_response }</v>
       </c>
       <c r="AN13" s="14" t="str">
-        <f>newline &amp; space &amp; L13 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y13 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_2point0_em_1_name:0 "$buy_influence_2point0_em_name$"</v>
+        <f>newline &amp; space &amp; L13 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y13 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_1:0 "$buy_influence_2point0_em_name$"</v>
       </c>
       <c r="AO13" s="15" t="str">
-        <f>newline &amp; space &amp; M13 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y13 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_2point0_em_2_name:0 "$buy_influence_2point0_em_name$"</v>
+        <f>newline &amp; space &amp; M13 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y13 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_2:0 "$buy_influence_2point0_em_name$"</v>
       </c>
       <c r="AP13" s="15" t="str">
-        <f>newline &amp; space &amp; N13 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y13 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_2point0_em_3_name:0 "$buy_influence_2point0_em_name$"</v>
+        <f>newline &amp; space &amp; N13 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y13 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_3:0 "$buy_influence_2point0_em_name$"</v>
       </c>
       <c r="AQ13" s="15" t="str">
-        <f>newline &amp; space &amp; O13 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y13 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_2point0_em_4_name:0 "$buy_influence_2point0_em_name$"</v>
+        <f>newline &amp; space &amp; O13 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y13 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_4:0 "$buy_influence_2point0_em_name$"</v>
       </c>
       <c r="AR13" s="15" t="str">
-        <f>newline &amp; space &amp; P13 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y13 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_2point0_em_5_name:0 "$buy_influence_2point0_em_name$"</v>
+        <f>newline &amp; space &amp; P13 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y13 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_em_5:0 "$buy_influence_2point0_em_name$"</v>
       </c>
       <c r="AS13" s="18" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">
- buy_influence_2point0_em_1_name:0 "$buy_influence_2point0_em_name$"
- buy_influence_2point0_em_2_name:0 "$buy_influence_2point0_em_name$"
- buy_influence_2point0_em_3_name:0 "$buy_influence_2point0_em_name$"
- buy_influence_2point0_em_4_name:0 "$buy_influence_2point0_em_name$"
- buy_influence_2point0_em_5_name:0 "$buy_influence_2point0_em_name$"</v>
+ buy_influence_2point0_em_1:0 "$buy_influence_2point0_em_name$"
+ buy_influence_2point0_em_2:0 "$buy_influence_2point0_em_name$"
+ buy_influence_2point0_em_3:0 "$buy_influence_2point0_em_name$"
+ buy_influence_2point0_em_4:0 "$buy_influence_2point0_em_name$"
+ buy_influence_2point0_em_5:0 "$buy_influence_2point0_em_name$"</v>
       </c>
       <c r="AT13" s="14" t="str">
-        <f>newline &amp; space &amp; L13 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z13 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">
  buy_influence_2point0_em_1_desc:0 "$buy_influence_2point0_em_desc$"</v>
       </c>
       <c r="AU13" s="15" t="str">
-        <f>newline &amp; space &amp; M13 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z13 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">
  buy_influence_2point0_em_2_desc:0 "$buy_influence_2point0_em_desc$"</v>
       </c>
       <c r="AV13" s="15" t="str">
-        <f>newline &amp; space &amp; N13 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z13 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="22"/>
         <v xml:space="preserve">
  buy_influence_2point0_em_3_desc:0 "$buy_influence_2point0_em_desc$"</v>
       </c>
       <c r="AW13" s="15" t="str">
-        <f>newline &amp; space &amp; O13 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z13 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="23"/>
         <v xml:space="preserve">
  buy_influence_2point0_em_4_desc:0 "$buy_influence_2point0_em_desc$"</v>
       </c>
       <c r="AX13" s="15" t="str">
-        <f>newline &amp; space &amp; P13 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z13 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
  buy_influence_2point0_em_5_desc:0 "$buy_influence_2point0_em_desc$"</v>
       </c>
       <c r="AY13" s="16" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v xml:space="preserve">
  buy_influence_2point0_em_1_desc:0 "$buy_influence_2point0_em_desc$"
  buy_influence_2point0_em_2_desc:0 "$buy_influence_2point0_em_desc$"
@@ -4560,7 +4548,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="43">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>10</v>
       </c>
       <c r="F14" s="57"/>
@@ -4575,11 +4563,11 @@
         <v>1</v>
       </c>
       <c r="K14" s="14" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_1point0_mf</v>
       </c>
       <c r="L14" s="36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>buy_influence_1point0_mf_1</v>
       </c>
       <c r="M14" s="37" t="str">
@@ -4667,7 +4655,7 @@
 }</v>
       </c>
       <c r="X14" s="16" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">
 buy_influence_1point0_mf_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -4701,15 +4689,15 @@
 }</v>
       </c>
       <c r="Y14" s="25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>buy_influence_1point0_mf_name</v>
       </c>
       <c r="Z14" s="15" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>buy_influence_1point0_mf_desc</v>
       </c>
       <c r="AA14" s="70" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>buy_influence_1point0_mf_response</v>
       </c>
       <c r="AB14" s="14" t="str">
@@ -4861,7 +4849,7 @@
 </v>
       </c>
       <c r="AG14" s="16" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_mf_name
 		trigger = {
@@ -5017,7 +5005,7 @@
         <v xml:space="preserve">
 				buy_influence_1point0_mf_5 = { text = buy_influence_1point0_mf_response }</v>
       </c>
-      <c r="AM14" s="18" t="str">
+      <c r="AM14" s="16" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_1point0_mf_1 = { text = buy_influence_1point0_mf_response }
@@ -5027,66 +5015,66 @@
 				buy_influence_1point0_mf_5 = { text = buy_influence_1point0_mf_response }</v>
       </c>
       <c r="AN14" s="14" t="str">
-        <f>newline &amp; space &amp; L14 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y14 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point0_mf_1_name:0 "$buy_influence_1point0_mf_name$"</v>
+        <f>newline &amp; space &amp; L14 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y14 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_1:0 "$buy_influence_1point0_mf_name$"</v>
       </c>
       <c r="AO14" s="15" t="str">
-        <f>newline &amp; space &amp; M14 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y14 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point0_mf_2_name:0 "$buy_influence_1point0_mf_name$"</v>
+        <f>newline &amp; space &amp; M14 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y14 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_2:0 "$buy_influence_1point0_mf_name$"</v>
       </c>
       <c r="AP14" s="15" t="str">
-        <f>newline &amp; space &amp; N14 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y14 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point0_mf_3_name:0 "$buy_influence_1point0_mf_name$"</v>
+        <f>newline &amp; space &amp; N14 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y14 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_3:0 "$buy_influence_1point0_mf_name$"</v>
       </c>
       <c r="AQ14" s="15" t="str">
-        <f>newline &amp; space &amp; O14 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y14 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point0_mf_4_name:0 "$buy_influence_1point0_mf_name$"</v>
+        <f>newline &amp; space &amp; O14 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y14 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_4:0 "$buy_influence_1point0_mf_name$"</v>
       </c>
       <c r="AR14" s="15" t="str">
-        <f>newline &amp; space &amp; P14 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y14 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point0_mf_5_name:0 "$buy_influence_1point0_mf_name$"</v>
+        <f>newline &amp; space &amp; P14 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y14 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point0_mf_5:0 "$buy_influence_1point0_mf_name$"</v>
       </c>
       <c r="AS14" s="18" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">
- buy_influence_1point0_mf_1_name:0 "$buy_influence_1point0_mf_name$"
- buy_influence_1point0_mf_2_name:0 "$buy_influence_1point0_mf_name$"
- buy_influence_1point0_mf_3_name:0 "$buy_influence_1point0_mf_name$"
- buy_influence_1point0_mf_4_name:0 "$buy_influence_1point0_mf_name$"
- buy_influence_1point0_mf_5_name:0 "$buy_influence_1point0_mf_name$"</v>
+ buy_influence_1point0_mf_1:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point0_mf_2:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point0_mf_3:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point0_mf_4:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point0_mf_5:0 "$buy_influence_1point0_mf_name$"</v>
       </c>
       <c r="AT14" s="14" t="str">
-        <f>newline &amp; space &amp; L14 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z14 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">
  buy_influence_1point0_mf_1_desc:0 "$buy_influence_1point0_mf_desc$"</v>
       </c>
       <c r="AU14" s="15" t="str">
-        <f>newline &amp; space &amp; M14 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z14 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">
  buy_influence_1point0_mf_2_desc:0 "$buy_influence_1point0_mf_desc$"</v>
       </c>
       <c r="AV14" s="15" t="str">
-        <f>newline &amp; space &amp; N14 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z14 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="22"/>
         <v xml:space="preserve">
  buy_influence_1point0_mf_3_desc:0 "$buy_influence_1point0_mf_desc$"</v>
       </c>
       <c r="AW14" s="15" t="str">
-        <f>newline &amp; space &amp; O14 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z14 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="23"/>
         <v xml:space="preserve">
  buy_influence_1point0_mf_4_desc:0 "$buy_influence_1point0_mf_desc$"</v>
       </c>
       <c r="AX14" s="15" t="str">
-        <f>newline &amp; space &amp; P14 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z14 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
  buy_influence_1point0_mf_5_desc:0 "$buy_influence_1point0_mf_desc$"</v>
       </c>
       <c r="AY14" s="16" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v xml:space="preserve">
  buy_influence_1point0_mf_1_desc:0 "$buy_influence_1point0_mf_desc$"
  buy_influence_1point0_mf_2_desc:0 "$buy_influence_1point0_mf_desc$"
@@ -5106,7 +5094,7 @@
         <v>1.5</v>
       </c>
       <c r="E15" s="43">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>15</v>
       </c>
       <c r="F15" s="57"/>
@@ -5121,11 +5109,11 @@
         <v>1</v>
       </c>
       <c r="K15" s="14" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_1point5_mf</v>
       </c>
       <c r="L15" s="36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>buy_influence_1point5_mf_1</v>
       </c>
       <c r="M15" s="37" t="str">
@@ -5213,7 +5201,7 @@
 }</v>
       </c>
       <c r="X15" s="16" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">
 buy_influence_1point5_mf_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -5247,15 +5235,15 @@
 }</v>
       </c>
       <c r="Y15" s="25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>buy_influence_1point5_mf_name</v>
       </c>
       <c r="Z15" s="15" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>buy_influence_1point5_mf_desc</v>
       </c>
       <c r="AA15" s="70" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>buy_influence_1point5_mf_response</v>
       </c>
       <c r="AB15" s="14" t="str">
@@ -5407,7 +5395,7 @@
 </v>
       </c>
       <c r="AG15" s="16" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point5_mf_name
 		trigger = {
@@ -5563,7 +5551,7 @@
         <v xml:space="preserve">
 				buy_influence_1point5_mf_5 = { text = buy_influence_1point5_mf_response }</v>
       </c>
-      <c r="AM15" s="18" t="str">
+      <c r="AM15" s="16" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_1point5_mf_1 = { text = buy_influence_1point5_mf_response }
@@ -5573,66 +5561,66 @@
 				buy_influence_1point5_mf_5 = { text = buy_influence_1point5_mf_response }</v>
       </c>
       <c r="AN15" s="14" t="str">
-        <f>newline &amp; space &amp; L15 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y15 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point5_mf_1_name:0 "$buy_influence_1point5_mf_name$"</v>
+        <f>newline &amp; space &amp; L15 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y15 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_1:0 "$buy_influence_1point5_mf_name$"</v>
       </c>
       <c r="AO15" s="15" t="str">
-        <f>newline &amp; space &amp; M15 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y15 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point5_mf_2_name:0 "$buy_influence_1point5_mf_name$"</v>
+        <f>newline &amp; space &amp; M15 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y15 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_2:0 "$buy_influence_1point5_mf_name$"</v>
       </c>
       <c r="AP15" s="15" t="str">
-        <f>newline &amp; space &amp; N15 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y15 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point5_mf_3_name:0 "$buy_influence_1point5_mf_name$"</v>
+        <f>newline &amp; space &amp; N15 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y15 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_3:0 "$buy_influence_1point5_mf_name$"</v>
       </c>
       <c r="AQ15" s="15" t="str">
-        <f>newline &amp; space &amp; O15 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y15 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point5_mf_4_name:0 "$buy_influence_1point5_mf_name$"</v>
+        <f>newline &amp; space &amp; O15 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y15 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_4:0 "$buy_influence_1point5_mf_name$"</v>
       </c>
       <c r="AR15" s="15" t="str">
-        <f>newline &amp; space &amp; P15 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y15 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_1point5_mf_5_name:0 "$buy_influence_1point5_mf_name$"</v>
+        <f>newline &amp; space &amp; P15 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y15 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_1point5_mf_5:0 "$buy_influence_1point5_mf_name$"</v>
       </c>
       <c r="AS15" s="18" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">
- buy_influence_1point5_mf_1_name:0 "$buy_influence_1point5_mf_name$"
- buy_influence_1point5_mf_2_name:0 "$buy_influence_1point5_mf_name$"
- buy_influence_1point5_mf_3_name:0 "$buy_influence_1point5_mf_name$"
- buy_influence_1point5_mf_4_name:0 "$buy_influence_1point5_mf_name$"
- buy_influence_1point5_mf_5_name:0 "$buy_influence_1point5_mf_name$"</v>
+ buy_influence_1point5_mf_1:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_1point5_mf_2:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_1point5_mf_3:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_1point5_mf_4:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_1point5_mf_5:0 "$buy_influence_1point5_mf_name$"</v>
       </c>
       <c r="AT15" s="14" t="str">
-        <f>newline &amp; space &amp; L15 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z15 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">
  buy_influence_1point5_mf_1_desc:0 "$buy_influence_1point5_mf_desc$"</v>
       </c>
       <c r="AU15" s="15" t="str">
-        <f>newline &amp; space &amp; M15 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z15 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">
  buy_influence_1point5_mf_2_desc:0 "$buy_influence_1point5_mf_desc$"</v>
       </c>
       <c r="AV15" s="15" t="str">
-        <f>newline &amp; space &amp; N15 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z15 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="22"/>
         <v xml:space="preserve">
  buy_influence_1point5_mf_3_desc:0 "$buy_influence_1point5_mf_desc$"</v>
       </c>
       <c r="AW15" s="15" t="str">
-        <f>newline &amp; space &amp; O15 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z15 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="23"/>
         <v xml:space="preserve">
  buy_influence_1point5_mf_4_desc:0 "$buy_influence_1point5_mf_desc$"</v>
       </c>
       <c r="AX15" s="15" t="str">
-        <f>newline &amp; space &amp; P15 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z15 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
  buy_influence_1point5_mf_5_desc:0 "$buy_influence_1point5_mf_desc$"</v>
       </c>
       <c r="AY15" s="16" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v xml:space="preserve">
  buy_influence_1point5_mf_1_desc:0 "$buy_influence_1point5_mf_desc$"
  buy_influence_1point5_mf_2_desc:0 "$buy_influence_1point5_mf_desc$"
@@ -5652,7 +5640,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="43">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>20</v>
       </c>
       <c r="F16" s="57"/>
@@ -5667,11 +5655,11 @@
         <v>1</v>
       </c>
       <c r="K16" s="14" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_2point0_mf</v>
       </c>
       <c r="L16" s="36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>buy_influence_2point0_mf_1</v>
       </c>
       <c r="M16" s="37" t="str">
@@ -5759,7 +5747,7 @@
 }</v>
       </c>
       <c r="X16" s="16" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">
 buy_influence_2point0_mf_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -5793,15 +5781,15 @@
 }</v>
       </c>
       <c r="Y16" s="25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>buy_influence_2point0_mf_name</v>
       </c>
       <c r="Z16" s="15" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>buy_influence_2point0_mf_desc</v>
       </c>
       <c r="AA16" s="70" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>buy_influence_2point0_mf_response</v>
       </c>
       <c r="AB16" s="14" t="str">
@@ -5953,7 +5941,7 @@
 </v>
       </c>
       <c r="AG16" s="16" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_mf_name
 		trigger = {
@@ -6109,7 +6097,7 @@
         <v xml:space="preserve">
 				buy_influence_2point0_mf_5 = { text = buy_influence_2point0_mf_response }</v>
       </c>
-      <c r="AM16" s="18" t="str">
+      <c r="AM16" s="16" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_2point0_mf_1 = { text = buy_influence_2point0_mf_response }
@@ -6119,66 +6107,66 @@
 				buy_influence_2point0_mf_5 = { text = buy_influence_2point0_mf_response }</v>
       </c>
       <c r="AN16" s="14" t="str">
-        <f>newline &amp; space &amp; L16 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y16 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_2point0_mf_1_name:0 "$buy_influence_2point0_mf_name$"</v>
+        <f>newline &amp; space &amp; L16 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y16 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_1:0 "$buy_influence_2point0_mf_name$"</v>
       </c>
       <c r="AO16" s="15" t="str">
-        <f>newline &amp; space &amp; M16 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y16 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_2point0_mf_2_name:0 "$buy_influence_2point0_mf_name$"</v>
+        <f>newline &amp; space &amp; M16 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y16 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_2:0 "$buy_influence_2point0_mf_name$"</v>
       </c>
       <c r="AP16" s="15" t="str">
-        <f>newline &amp; space &amp; N16 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y16 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_2point0_mf_3_name:0 "$buy_influence_2point0_mf_name$"</v>
+        <f>newline &amp; space &amp; N16 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y16 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_3:0 "$buy_influence_2point0_mf_name$"</v>
       </c>
       <c r="AQ16" s="15" t="str">
-        <f>newline &amp; space &amp; O16 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y16 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_2point0_mf_4_name:0 "$buy_influence_2point0_mf_name$"</v>
+        <f>newline &amp; space &amp; O16 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y16 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_4:0 "$buy_influence_2point0_mf_name$"</v>
       </c>
       <c r="AR16" s="15" t="str">
-        <f>newline &amp; space &amp; P16 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y16 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_2point0_mf_5_name:0 "$buy_influence_2point0_mf_name$"</v>
+        <f>newline &amp; space &amp; P16 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y16 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_mf_5:0 "$buy_influence_2point0_mf_name$"</v>
       </c>
       <c r="AS16" s="18" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">
- buy_influence_2point0_mf_1_name:0 "$buy_influence_2point0_mf_name$"
- buy_influence_2point0_mf_2_name:0 "$buy_influence_2point0_mf_name$"
- buy_influence_2point0_mf_3_name:0 "$buy_influence_2point0_mf_name$"
- buy_influence_2point0_mf_4_name:0 "$buy_influence_2point0_mf_name$"
- buy_influence_2point0_mf_5_name:0 "$buy_influence_2point0_mf_name$"</v>
+ buy_influence_2point0_mf_1:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_mf_2:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_mf_3:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_mf_4:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_mf_5:0 "$buy_influence_2point0_mf_name$"</v>
       </c>
       <c r="AT16" s="14" t="str">
-        <f>newline &amp; space &amp; L16 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z16 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">
  buy_influence_2point0_mf_1_desc:0 "$buy_influence_2point0_mf_desc$"</v>
       </c>
       <c r="AU16" s="15" t="str">
-        <f>newline &amp; space &amp; M16 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z16 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">
  buy_influence_2point0_mf_2_desc:0 "$buy_influence_2point0_mf_desc$"</v>
       </c>
       <c r="AV16" s="15" t="str">
-        <f>newline &amp; space &amp; N16 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z16 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="22"/>
         <v xml:space="preserve">
  buy_influence_2point0_mf_3_desc:0 "$buy_influence_2point0_mf_desc$"</v>
       </c>
       <c r="AW16" s="15" t="str">
-        <f>newline &amp; space &amp; O16 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z16 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="23"/>
         <v xml:space="preserve">
  buy_influence_2point0_mf_4_desc:0 "$buy_influence_2point0_mf_desc$"</v>
       </c>
       <c r="AX16" s="15" t="str">
-        <f>newline &amp; space &amp; P16 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z16 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
  buy_influence_2point0_mf_5_desc:0 "$buy_influence_2point0_mf_desc$"</v>
       </c>
       <c r="AY16" s="16" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v xml:space="preserve">
  buy_influence_2point0_mf_1_desc:0 "$buy_influence_2point0_mf_desc$"
  buy_influence_2point0_mf_2_desc:0 "$buy_influence_2point0_mf_desc$"
@@ -6198,7 +6186,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="43">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>20</v>
       </c>
       <c r="F17" s="57">
@@ -6215,11 +6203,11 @@
         <v>1</v>
       </c>
       <c r="K17" s="14" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_2point0_emc</v>
       </c>
       <c r="L17" s="36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>buy_influence_2point0_emc_1</v>
       </c>
       <c r="M17" s="37" t="str">
@@ -6312,7 +6300,7 @@
 }</v>
       </c>
       <c r="X17" s="16" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">
 buy_influence_2point0_emc_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6351,15 +6339,15 @@
 }</v>
       </c>
       <c r="Y17" s="25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>buy_influence_2point0_emc_name</v>
       </c>
       <c r="Z17" s="15" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>buy_influence_2point0_emc_desc</v>
       </c>
       <c r="AA17" s="70" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>buy_influence_2point0_emc_response</v>
       </c>
       <c r="AB17" s="14" t="str">
@@ -6511,7 +6499,7 @@
 </v>
       </c>
       <c r="AG17" s="16" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_emc_name
 		trigger = {
@@ -6667,7 +6655,7 @@
         <v xml:space="preserve">
 				buy_influence_2point0_emc_5 = { text = buy_influence_2point0_emc_response }</v>
       </c>
-      <c r="AM17" s="18" t="str">
+      <c r="AM17" s="16" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_2point0_emc_1 = { text = buy_influence_2point0_emc_response }
@@ -6677,66 +6665,66 @@
 				buy_influence_2point0_emc_5 = { text = buy_influence_2point0_emc_response }</v>
       </c>
       <c r="AN17" s="14" t="str">
-        <f>newline &amp; space &amp; L17 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y17 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_2point0_emc_1_name:0 "$buy_influence_2point0_emc_name$"</v>
+        <f>newline &amp; space &amp; L17 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y17 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_1:0 "$buy_influence_2point0_emc_name$"</v>
       </c>
       <c r="AO17" s="15" t="str">
-        <f>newline &amp; space &amp; M17 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y17 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_2point0_emc_2_name:0 "$buy_influence_2point0_emc_name$"</v>
+        <f>newline &amp; space &amp; M17 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y17 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_2:0 "$buy_influence_2point0_emc_name$"</v>
       </c>
       <c r="AP17" s="15" t="str">
-        <f>newline &amp; space &amp; N17 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y17 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_2point0_emc_3_name:0 "$buy_influence_2point0_emc_name$"</v>
+        <f>newline &amp; space &amp; N17 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y17 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_3:0 "$buy_influence_2point0_emc_name$"</v>
       </c>
       <c r="AQ17" s="15" t="str">
-        <f>newline &amp; space &amp; O17 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y17 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_2point0_emc_4_name:0 "$buy_influence_2point0_emc_name$"</v>
+        <f>newline &amp; space &amp; O17 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y17 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_4:0 "$buy_influence_2point0_emc_name$"</v>
       </c>
       <c r="AR17" s="15" t="str">
-        <f>newline &amp; space &amp; P17 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y17 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_2point0_emc_5_name:0 "$buy_influence_2point0_emc_name$"</v>
+        <f>newline &amp; space &amp; P17 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y17 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_2point0_emc_5:0 "$buy_influence_2point0_emc_name$"</v>
       </c>
       <c r="AS17" s="18" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">
- buy_influence_2point0_emc_1_name:0 "$buy_influence_2point0_emc_name$"
- buy_influence_2point0_emc_2_name:0 "$buy_influence_2point0_emc_name$"
- buy_influence_2point0_emc_3_name:0 "$buy_influence_2point0_emc_name$"
- buy_influence_2point0_emc_4_name:0 "$buy_influence_2point0_emc_name$"
- buy_influence_2point0_emc_5_name:0 "$buy_influence_2point0_emc_name$"</v>
+ buy_influence_2point0_emc_1:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_2point0_emc_2:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_2point0_emc_3:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_2point0_emc_4:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_2point0_emc_5:0 "$buy_influence_2point0_emc_name$"</v>
       </c>
       <c r="AT17" s="14" t="str">
-        <f>newline &amp; space &amp; L17 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z17 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">
  buy_influence_2point0_emc_1_desc:0 "$buy_influence_2point0_emc_desc$"</v>
       </c>
       <c r="AU17" s="15" t="str">
-        <f>newline &amp; space &amp; M17 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z17 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">
  buy_influence_2point0_emc_2_desc:0 "$buy_influence_2point0_emc_desc$"</v>
       </c>
       <c r="AV17" s="15" t="str">
-        <f>newline &amp; space &amp; N17 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z17 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="22"/>
         <v xml:space="preserve">
  buy_influence_2point0_emc_3_desc:0 "$buy_influence_2point0_emc_desc$"</v>
       </c>
       <c r="AW17" s="15" t="str">
-        <f>newline &amp; space &amp; O17 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z17 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="23"/>
         <v xml:space="preserve">
  buy_influence_2point0_emc_4_desc:0 "$buy_influence_2point0_emc_desc$"</v>
       </c>
       <c r="AX17" s="15" t="str">
-        <f>newline &amp; space &amp; P17 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z17 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
  buy_influence_2point0_emc_5_desc:0 "$buy_influence_2point0_emc_desc$"</v>
       </c>
       <c r="AY17" s="16" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v xml:space="preserve">
  buy_influence_2point0_emc_1_desc:0 "$buy_influence_2point0_emc_desc$"
  buy_influence_2point0_emc_2_desc:0 "$buy_influence_2point0_emc_desc$"
@@ -6756,7 +6744,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="43">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>25</v>
       </c>
       <c r="F18" s="57">
@@ -6773,11 +6761,11 @@
         <v>1</v>
       </c>
       <c r="K18" s="14" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_3point0_emc</v>
       </c>
       <c r="L18" s="36" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>buy_influence_3point0_emc_1</v>
       </c>
       <c r="M18" s="37" t="str">
@@ -6870,7 +6858,7 @@
 }</v>
       </c>
       <c r="X18" s="16" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">
 buy_influence_3point0_emc_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6909,15 +6897,15 @@
 }</v>
       </c>
       <c r="Y18" s="25" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>buy_influence_3point0_emc_name</v>
       </c>
       <c r="Z18" s="15" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>buy_influence_3point0_emc_desc</v>
       </c>
       <c r="AA18" s="70" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>buy_influence_3point0_emc_response</v>
       </c>
       <c r="AB18" s="14" t="str">
@@ -7069,7 +7057,7 @@
 </v>
       </c>
       <c r="AG18" s="16" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_3point0_emc_name
 		trigger = {
@@ -7225,7 +7213,7 @@
         <v xml:space="preserve">
 				buy_influence_3point0_emc_5 = { text = buy_influence_3point0_emc_response }</v>
       </c>
-      <c r="AM18" s="18" t="str">
+      <c r="AM18" s="16" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_3point0_emc_1 = { text = buy_influence_3point0_emc_response }
@@ -7235,66 +7223,66 @@
 				buy_influence_3point0_emc_5 = { text = buy_influence_3point0_emc_response }</v>
       </c>
       <c r="AN18" s="14" t="str">
-        <f>newline &amp; space &amp; L18 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y18 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_3point0_emc_1_name:0 "$buy_influence_3point0_emc_name$"</v>
+        <f>newline &amp; space &amp; L18 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y18 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_1:0 "$buy_influence_3point0_emc_name$"</v>
       </c>
       <c r="AO18" s="15" t="str">
-        <f>newline &amp; space &amp; M18 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y18 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_3point0_emc_2_name:0 "$buy_influence_3point0_emc_name$"</v>
+        <f>newline &amp; space &amp; M18 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y18 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_2:0 "$buy_influence_3point0_emc_name$"</v>
       </c>
       <c r="AP18" s="15" t="str">
-        <f>newline &amp; space &amp; N18 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y18 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_3point0_emc_3_name:0 "$buy_influence_3point0_emc_name$"</v>
+        <f>newline &amp; space &amp; N18 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y18 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_3:0 "$buy_influence_3point0_emc_name$"</v>
       </c>
       <c r="AQ18" s="15" t="str">
-        <f>newline &amp; space &amp; O18 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y18 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_3point0_emc_4_name:0 "$buy_influence_3point0_emc_name$"</v>
+        <f>newline &amp; space &amp; O18 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y18 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_4:0 "$buy_influence_3point0_emc_name$"</v>
       </c>
       <c r="AR18" s="15" t="str">
-        <f>newline &amp; space &amp; P18 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y18 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_3point0_emc_5_name:0 "$buy_influence_3point0_emc_name$"</v>
+        <f>newline &amp; space &amp; P18 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y18 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_3point0_emc_5:0 "$buy_influence_3point0_emc_name$"</v>
       </c>
       <c r="AS18" s="18" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">
- buy_influence_3point0_emc_1_name:0 "$buy_influence_3point0_emc_name$"
- buy_influence_3point0_emc_2_name:0 "$buy_influence_3point0_emc_name$"
- buy_influence_3point0_emc_3_name:0 "$buy_influence_3point0_emc_name$"
- buy_influence_3point0_emc_4_name:0 "$buy_influence_3point0_emc_name$"
- buy_influence_3point0_emc_5_name:0 "$buy_influence_3point0_emc_name$"</v>
+ buy_influence_3point0_emc_1:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_3point0_emc_2:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_3point0_emc_3:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_3point0_emc_4:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_3point0_emc_5:0 "$buy_influence_3point0_emc_name$"</v>
       </c>
       <c r="AT18" s="14" t="str">
-        <f>newline &amp; space &amp; L18 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z18 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">
  buy_influence_3point0_emc_1_desc:0 "$buy_influence_3point0_emc_desc$"</v>
       </c>
       <c r="AU18" s="15" t="str">
-        <f>newline &amp; space &amp; M18 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z18 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">
  buy_influence_3point0_emc_2_desc:0 "$buy_influence_3point0_emc_desc$"</v>
       </c>
       <c r="AV18" s="15" t="str">
-        <f>newline &amp; space &amp; N18 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z18 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="22"/>
         <v xml:space="preserve">
  buy_influence_3point0_emc_3_desc:0 "$buy_influence_3point0_emc_desc$"</v>
       </c>
       <c r="AW18" s="15" t="str">
-        <f>newline &amp; space &amp; O18 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z18 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="23"/>
         <v xml:space="preserve">
  buy_influence_3point0_emc_4_desc:0 "$buy_influence_3point0_emc_desc$"</v>
       </c>
       <c r="AX18" s="15" t="str">
-        <f>newline &amp; space &amp; P18 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z18 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
  buy_influence_3point0_emc_5_desc:0 "$buy_influence_3point0_emc_desc$"</v>
       </c>
       <c r="AY18" s="16" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v xml:space="preserve">
  buy_influence_3point0_emc_1_desc:0 "$buy_influence_3point0_emc_desc$"
  buy_influence_3point0_emc_2_desc:0 "$buy_influence_3point0_emc_desc$"
@@ -7314,7 +7302,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="44">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>25</v>
       </c>
       <c r="F19" s="61">
@@ -7331,11 +7319,11 @@
         <v>1</v>
       </c>
       <c r="K19" s="19" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>buy_influence_4point0_emc</v>
       </c>
       <c r="L19" s="39" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>buy_influence_4point0_emc_1</v>
       </c>
       <c r="M19" s="40" t="str">
@@ -7428,7 +7416,7 @@
 }</v>
       </c>
       <c r="X19" s="21" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v xml:space="preserve">
 buy_influence_4point0_emc_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -7467,15 +7455,15 @@
 }</v>
       </c>
       <c r="Y19" s="26" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>buy_influence_4point0_emc_name</v>
       </c>
       <c r="Z19" s="20" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>buy_influence_4point0_emc_desc</v>
       </c>
       <c r="AA19" s="71" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>buy_influence_4point0_emc_response</v>
       </c>
       <c r="AB19" s="19" t="str">
@@ -7627,7 +7615,7 @@
 </v>
       </c>
       <c r="AG19" s="21" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_4point0_emc_name
 		trigger = {
@@ -7783,7 +7771,7 @@
         <v xml:space="preserve">
 				buy_influence_4point0_emc_5 = { text = buy_influence_4point0_emc_response }</v>
       </c>
-      <c r="AM19" s="23" t="str">
+      <c r="AM19" s="21" t="str">
         <f t="shared" si="18"/>
         <v xml:space="preserve">
 				buy_influence_4point0_emc_1 = { text = buy_influence_4point0_emc_response }
@@ -7793,66 +7781,66 @@
 				buy_influence_4point0_emc_5 = { text = buy_influence_4point0_emc_response }</v>
       </c>
       <c r="AN19" s="19" t="str">
-        <f>newline &amp; space &amp; L19 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y19 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_4point0_emc_1_name:0 "$buy_influence_4point0_emc_name$"</v>
+        <f>newline &amp; space &amp; L19 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y19 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_1:0 "$buy_influence_4point0_emc_name$"</v>
       </c>
       <c r="AO19" s="20" t="str">
-        <f>newline &amp; space &amp; M19 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y19 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_4point0_emc_2_name:0 "$buy_influence_4point0_emc_name$"</v>
+        <f>newline &amp; space &amp; M19 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y19 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_2:0 "$buy_influence_4point0_emc_name$"</v>
       </c>
       <c r="AP19" s="20" t="str">
-        <f>newline &amp; space &amp; N19 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y19 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_4point0_emc_3_name:0 "$buy_influence_4point0_emc_name$"</v>
+        <f>newline &amp; space &amp; N19 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y19 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_3:0 "$buy_influence_4point0_emc_name$"</v>
       </c>
       <c r="AQ19" s="20" t="str">
-        <f>newline &amp; space &amp; O19 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y19 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_4point0_emc_4_name:0 "$buy_influence_4point0_emc_name$"</v>
+        <f>newline &amp; space &amp; O19 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y19 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_4:0 "$buy_influence_4point0_emc_name$"</v>
       </c>
       <c r="AR19" s="20" t="str">
-        <f>newline &amp; space &amp; P19 &amp; "_name:0 " &amp; doublequote &amp; "$" &amp; $Y19 &amp; "$" &amp; doublequote</f>
-        <v xml:space="preserve">
- buy_influence_4point0_emc_5_name:0 "$buy_influence_4point0_emc_name$"</v>
+        <f>newline &amp; space &amp; P19 &amp; ":0 " &amp; doublequote &amp; "$" &amp; $Y19 &amp; "$" &amp; doublequote</f>
+        <v xml:space="preserve">
+ buy_influence_4point0_emc_5:0 "$buy_influence_4point0_emc_name$"</v>
       </c>
       <c r="AS19" s="23" t="str">
         <f t="shared" si="19"/>
         <v xml:space="preserve">
- buy_influence_4point0_emc_1_name:0 "$buy_influence_4point0_emc_name$"
- buy_influence_4point0_emc_2_name:0 "$buy_influence_4point0_emc_name$"
- buy_influence_4point0_emc_3_name:0 "$buy_influence_4point0_emc_name$"
- buy_influence_4point0_emc_4_name:0 "$buy_influence_4point0_emc_name$"
- buy_influence_4point0_emc_5_name:0 "$buy_influence_4point0_emc_name$"</v>
+ buy_influence_4point0_emc_1:0 "$buy_influence_4point0_emc_name$"
+ buy_influence_4point0_emc_2:0 "$buy_influence_4point0_emc_name$"
+ buy_influence_4point0_emc_3:0 "$buy_influence_4point0_emc_name$"
+ buy_influence_4point0_emc_4:0 "$buy_influence_4point0_emc_name$"
+ buy_influence_4point0_emc_5:0 "$buy_influence_4point0_emc_name$"</v>
       </c>
       <c r="AT19" s="19" t="str">
-        <f>newline &amp; space &amp; L19 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z19 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">
  buy_influence_4point0_emc_1_desc:0 "$buy_influence_4point0_emc_desc$"</v>
       </c>
       <c r="AU19" s="20" t="str">
-        <f>newline &amp; space &amp; M19 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z19 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="21"/>
         <v xml:space="preserve">
  buy_influence_4point0_emc_2_desc:0 "$buy_influence_4point0_emc_desc$"</v>
       </c>
       <c r="AV19" s="20" t="str">
-        <f>newline &amp; space &amp; N19 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z19 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="22"/>
         <v xml:space="preserve">
  buy_influence_4point0_emc_3_desc:0 "$buy_influence_4point0_emc_desc$"</v>
       </c>
       <c r="AW19" s="20" t="str">
-        <f>newline &amp; space &amp; O19 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z19 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="23"/>
         <v xml:space="preserve">
  buy_influence_4point0_emc_4_desc:0 "$buy_influence_4point0_emc_desc$"</v>
       </c>
       <c r="AX19" s="20" t="str">
-        <f>newline &amp; space &amp; P19 &amp; "_desc:0 " &amp; doublequote &amp; "$" &amp; $Z19 &amp; "$" &amp; doublequote</f>
+        <f t="shared" si="24"/>
         <v xml:space="preserve">
  buy_influence_4point0_emc_5_desc:0 "$buy_influence_4point0_emc_desc$"</v>
       </c>
       <c r="AY19" s="21" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v xml:space="preserve">
  buy_influence_4point0_emc_1_desc:0 "$buy_influence_4point0_emc_desc$"
  buy_influence_4point0_emc_2_desc:0 "$buy_influence_4point0_emc_desc$"
@@ -9820,61 +9808,61 @@
         <f>space &amp; "#Generated code: Set modifier names equal to the generic (non-pop-dependent) name for each modifier" &amp;
 CONCATENATE(AS9,AS10,AS11,AS12,AS13,AS14,AS15,AS16,AS17,AS18,AS19)</f>
         <v xml:space="preserve"> #Generated code: Set modifier names equal to the generic (non-pop-dependent) name for each modifier
- buy_influence_0point5_e_1_name:0 "$buy_influence_0point5_e_name$"
- buy_influence_0point5_e_2_name:0 "$buy_influence_0point5_e_name$"
- buy_influence_0point5_e_3_name:0 "$buy_influence_0point5_e_name$"
- buy_influence_0point5_e_4_name:0 "$buy_influence_0point5_e_name$"
- buy_influence_0point5_e_5_name:0 "$buy_influence_0point5_e_name$"
- buy_influence_1point0_e_1_name:0 "$buy_influence_1point0_e_name$"
- buy_influence_1point0_e_2_name:0 "$buy_influence_1point0_e_name$"
- buy_influence_1point0_e_3_name:0 "$buy_influence_1point0_e_name$"
- buy_influence_1point0_e_4_name:0 "$buy_influence_1point0_e_name$"
- buy_influence_1point0_e_5_name:0 "$buy_influence_1point0_e_name$"
- buy_influence_1point0_em_1_name:0 "$buy_influence_1point0_em_name$"
- buy_influence_1point0_em_2_name:0 "$buy_influence_1point0_em_name$"
- buy_influence_1point0_em_3_name:0 "$buy_influence_1point0_em_name$"
- buy_influence_1point0_em_4_name:0 "$buy_influence_1point0_em_name$"
- buy_influence_1point0_em_5_name:0 "$buy_influence_1point0_em_name$"
- buy_influence_1point5_em_1_name:0 "$buy_influence_1point5_em_name$"
- buy_influence_1point5_em_2_name:0 "$buy_influence_1point5_em_name$"
- buy_influence_1point5_em_3_name:0 "$buy_influence_1point5_em_name$"
- buy_influence_1point5_em_4_name:0 "$buy_influence_1point5_em_name$"
- buy_influence_1point5_em_5_name:0 "$buy_influence_1point5_em_name$"
- buy_influence_2point0_em_1_name:0 "$buy_influence_2point0_em_name$"
- buy_influence_2point0_em_2_name:0 "$buy_influence_2point0_em_name$"
- buy_influence_2point0_em_3_name:0 "$buy_influence_2point0_em_name$"
- buy_influence_2point0_em_4_name:0 "$buy_influence_2point0_em_name$"
- buy_influence_2point0_em_5_name:0 "$buy_influence_2point0_em_name$"
- buy_influence_1point0_mf_1_name:0 "$buy_influence_1point0_mf_name$"
- buy_influence_1point0_mf_2_name:0 "$buy_influence_1point0_mf_name$"
- buy_influence_1point0_mf_3_name:0 "$buy_influence_1point0_mf_name$"
- buy_influence_1point0_mf_4_name:0 "$buy_influence_1point0_mf_name$"
- buy_influence_1point0_mf_5_name:0 "$buy_influence_1point0_mf_name$"
- buy_influence_1point5_mf_1_name:0 "$buy_influence_1point5_mf_name$"
- buy_influence_1point5_mf_2_name:0 "$buy_influence_1point5_mf_name$"
- buy_influence_1point5_mf_3_name:0 "$buy_influence_1point5_mf_name$"
- buy_influence_1point5_mf_4_name:0 "$buy_influence_1point5_mf_name$"
- buy_influence_1point5_mf_5_name:0 "$buy_influence_1point5_mf_name$"
- buy_influence_2point0_mf_1_name:0 "$buy_influence_2point0_mf_name$"
- buy_influence_2point0_mf_2_name:0 "$buy_influence_2point0_mf_name$"
- buy_influence_2point0_mf_3_name:0 "$buy_influence_2point0_mf_name$"
- buy_influence_2point0_mf_4_name:0 "$buy_influence_2point0_mf_name$"
- buy_influence_2point0_mf_5_name:0 "$buy_influence_2point0_mf_name$"
- buy_influence_2point0_emc_1_name:0 "$buy_influence_2point0_emc_name$"
- buy_influence_2point0_emc_2_name:0 "$buy_influence_2point0_emc_name$"
- buy_influence_2point0_emc_3_name:0 "$buy_influence_2point0_emc_name$"
- buy_influence_2point0_emc_4_name:0 "$buy_influence_2point0_emc_name$"
- buy_influence_2point0_emc_5_name:0 "$buy_influence_2point0_emc_name$"
- buy_influence_3point0_emc_1_name:0 "$buy_influence_3point0_emc_name$"
- buy_influence_3point0_emc_2_name:0 "$buy_influence_3point0_emc_name$"
- buy_influence_3point0_emc_3_name:0 "$buy_influence_3point0_emc_name$"
- buy_influence_3point0_emc_4_name:0 "$buy_influence_3point0_emc_name$"
- buy_influence_3point0_emc_5_name:0 "$buy_influence_3point0_emc_name$"
- buy_influence_4point0_emc_1_name:0 "$buy_influence_4point0_emc_name$"
- buy_influence_4point0_emc_2_name:0 "$buy_influence_4point0_emc_name$"
- buy_influence_4point0_emc_3_name:0 "$buy_influence_4point0_emc_name$"
- buy_influence_4point0_emc_4_name:0 "$buy_influence_4point0_emc_name$"
- buy_influence_4point0_emc_5_name:0 "$buy_influence_4point0_emc_name$"</v>
+ buy_influence_0point5_e_1:0 "$buy_influence_0point5_e_name$"
+ buy_influence_0point5_e_2:0 "$buy_influence_0point5_e_name$"
+ buy_influence_0point5_e_3:0 "$buy_influence_0point5_e_name$"
+ buy_influence_0point5_e_4:0 "$buy_influence_0point5_e_name$"
+ buy_influence_0point5_e_5:0 "$buy_influence_0point5_e_name$"
+ buy_influence_1point0_e_1:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_e_2:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_e_3:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_e_4:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_e_5:0 "$buy_influence_1point0_e_name$"
+ buy_influence_1point0_em_1:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point0_em_2:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point0_em_3:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point0_em_4:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point0_em_5:0 "$buy_influence_1point0_em_name$"
+ buy_influence_1point5_em_1:0 "$buy_influence_1point5_em_name$"
+ buy_influence_1point5_em_2:0 "$buy_influence_1point5_em_name$"
+ buy_influence_1point5_em_3:0 "$buy_influence_1point5_em_name$"
+ buy_influence_1point5_em_4:0 "$buy_influence_1point5_em_name$"
+ buy_influence_1point5_em_5:0 "$buy_influence_1point5_em_name$"
+ buy_influence_2point0_em_1:0 "$buy_influence_2point0_em_name$"
+ buy_influence_2point0_em_2:0 "$buy_influence_2point0_em_name$"
+ buy_influence_2point0_em_3:0 "$buy_influence_2point0_em_name$"
+ buy_influence_2point0_em_4:0 "$buy_influence_2point0_em_name$"
+ buy_influence_2point0_em_5:0 "$buy_influence_2point0_em_name$"
+ buy_influence_1point0_mf_1:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point0_mf_2:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point0_mf_3:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point0_mf_4:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point0_mf_5:0 "$buy_influence_1point0_mf_name$"
+ buy_influence_1point5_mf_1:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_1point5_mf_2:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_1point5_mf_3:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_1point5_mf_4:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_1point5_mf_5:0 "$buy_influence_1point5_mf_name$"
+ buy_influence_2point0_mf_1:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_mf_2:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_mf_3:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_mf_4:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_mf_5:0 "$buy_influence_2point0_mf_name$"
+ buy_influence_2point0_emc_1:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_2point0_emc_2:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_2point0_emc_3:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_2point0_emc_4:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_2point0_emc_5:0 "$buy_influence_2point0_emc_name$"
+ buy_influence_3point0_emc_1:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_3point0_emc_2:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_3point0_emc_3:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_3point0_emc_4:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_3point0_emc_5:0 "$buy_influence_3point0_emc_name$"
+ buy_influence_4point0_emc_1:0 "$buy_influence_4point0_emc_name$"
+ buy_influence_4point0_emc_2:0 "$buy_influence_4point0_emc_name$"
+ buy_influence_4point0_emc_3:0 "$buy_influence_4point0_emc_name$"
+ buy_influence_4point0_emc_4:0 "$buy_influence_4point0_emc_name$"
+ buy_influence_4point0_emc_5:0 "$buy_influence_4point0_emc_name$"</v>
       </c>
       <c r="AY20" s="30" t="str">
         <f>space &amp; "#Generated code: Set modifier descriptions equal to the generic (non-pop-dependent) description for each modifier" &amp;

</xml_diff>

<commit_message>
Buy Influence: Final bugfixes & tweaks before workshop upload
Bugfix: Trust with artisan enclave is increased every year that a propaganda campaign is active, as desired.

Renewal screen shows a reminder of which campaign has just expired.

Custom tooltip explaining trust gain is now embedded in the modifier. (Previously, it was only present in the event.) This means you can view the expected trust gain from the empire screen at any time.
</commit_message>
<xml_diff>
--- a/buy_influence/CodeGen.xlsx
+++ b/buy_influence/CodeGen.xlsx
@@ -13,8 +13,8 @@
     <definedName name="doublequote">CodeGen!$C$4</definedName>
     <definedName name="event_option_add_static_modifier_raw">CodeGen!$AD$4</definedName>
     <definedName name="event_option_add_static_modifier_subst_text">CodeGen!$AD$3</definedName>
-    <definedName name="event_option_opinion_gain_raw">CodeGen!$AE$4</definedName>
-    <definedName name="event_option_opinion_gain_subst_text">CodeGen!$AE$3</definedName>
+    <definedName name="event_option_opinion_gain_raw">CodeGen!$U$4</definedName>
+    <definedName name="event_option_opinion_gain_subst_text">CodeGen!$U$3</definedName>
     <definedName name="event_option_trigger_renewal_event">CodeGen!$AF$4</definedName>
     <definedName name="newline">CodeGen!$C$1</definedName>
     <definedName name="space">CodeGen!$C$3</definedName>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>Theme</t>
   </si>
@@ -212,12 +212,36 @@
   <si>
     <t>Modif type main event</t>
   </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>Remove</t>
+  </si>
+  <si>
+    <t>Renewal flags</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Event desc</t>
+  </si>
+  <si>
+    <t>Localisation</t>
+  </si>
+  <si>
+    <t>Localisation string</t>
+  </si>
+  <si>
+    <t>Renewal localisation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -817,7 +841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -989,13 +1013,40 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1007,19 +1058,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1377,20 +1419,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:BD20"/>
+  <dimension ref="B1:BJ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI20" sqref="AI20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" outlineLevelCol="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="3.1328125" style="1" customWidth="1"/>
     <col min="2" max="3" width="9.06640625" style="27"/>
     <col min="4" max="5" width="10" style="27" customWidth="1"/>
     <col min="6" max="10" width="9.06640625" style="27"/>
-    <col min="11" max="17" width="9.06640625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="20" width="9.06640625" style="1"/>
+    <col min="11" max="17" width="9.06640625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="9.06640625" style="1" collapsed="1"/>
+    <col min="19" max="20" width="9.06640625" style="1"/>
     <col min="21" max="25" width="9.06640625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="26" max="26" width="9.06640625" style="1" collapsed="1"/>
     <col min="27" max="29" width="9.06640625" style="1"/>
@@ -1404,10 +1447,14 @@
     <col min="54" max="54" width="13.33203125" style="1" customWidth="1"/>
     <col min="55" max="55" width="10.53125" style="1" customWidth="1"/>
     <col min="56" max="56" width="10.3984375" style="1" customWidth="1"/>
-    <col min="57" max="16384" width="9.06640625" style="1"/>
+    <col min="57" max="59" width="9.06640625" style="1"/>
+    <col min="60" max="60" width="10.265625" style="1" customWidth="1"/>
+    <col min="61" max="61" width="10.9296875" style="1" customWidth="1"/>
+    <col min="62" max="62" width="10.73046875" style="1" customWidth="1"/>
+    <col min="63" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:56" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:62">
       <c r="B1" s="45" t="s">
         <v>19</v>
       </c>
@@ -1451,7 +1498,7 @@
 		}</v>
       </c>
     </row>
-    <row r="2" spans="2:56" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:62">
       <c r="B2" s="47" t="s">
         <v>20</v>
       </c>
@@ -1463,7 +1510,7 @@
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
     </row>
-    <row r="3" spans="2:56" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:62">
       <c r="B3" s="47" t="s">
         <v>23</v>
       </c>
@@ -1471,20 +1518,24 @@
         <f>" "</f>
         <v xml:space="preserve"> </v>
       </c>
+      <c r="U3" s="63" t="s">
+        <v>30</v>
+      </c>
       <c r="AD3" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="AE3" s="63" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="4" spans="2:56" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:62" ht="14.65" thickBot="1">
       <c r="B4" s="49" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="50" t="str">
         <f>CHAR(34)</f>
         <v>"</v>
+      </c>
+      <c r="U4" s="63" t="str">
+        <f>"custom_tooltip = buy_influence_opinion_gain_" &amp; $U$3</f>
+        <v>custom_tooltip = buy_influence_opinion_gain_$OPINION_GAIN_SIZE$</v>
       </c>
       <c r="AD4" s="63" t="str">
         <f>tab &amp; tab &amp; "add_modifier = {" &amp; newline &amp;
@@ -1495,10 +1546,6 @@
 			modifier = $STATIC_MODIFIER_NAME$
 			days = @buy_influence_buff_duration
 		}</v>
-      </c>
-      <c r="AE4" s="63" t="str">
-        <f>tab &amp; tab &amp; "custom_tooltip = buy_influence_opinion_gain_" &amp; $AE$3</f>
-        <v xml:space="preserve">		custom_tooltip = buy_influence_opinion_gain_$OPINION_GAIN_SIZE$</v>
       </c>
       <c r="AF4" s="63" t="str">
         <f>tab &amp; tab &amp; "hidden_effect = {" &amp; newline &amp;
@@ -1515,166 +1562,194 @@
 		}</v>
       </c>
     </row>
-    <row r="5" spans="2:56" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="6" spans="2:56" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="92" t="s">
+    <row r="5" spans="2:62" ht="14.65" thickBot="1"/>
+    <row r="6" spans="2:62" ht="14.25" customHeight="1">
+      <c r="B6" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="92" t="s">
+      <c r="C6" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="92" t="s">
+      <c r="D6" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="92" t="s">
+      <c r="E6" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="96" t="s">
+      <c r="F6" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="97"/>
-      <c r="J6" s="92" t="s">
+      <c r="G6" s="102"/>
+      <c r="H6" s="102"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="95" t="s">
+      <c r="K6" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="96"/>
-      <c r="M6" s="96"/>
-      <c r="N6" s="96"/>
-      <c r="O6" s="96"/>
-      <c r="P6" s="96"/>
-      <c r="Q6" s="97"/>
-      <c r="R6" s="92" t="s">
+      <c r="L6" s="102"/>
+      <c r="M6" s="102"/>
+      <c r="N6" s="102"/>
+      <c r="O6" s="102"/>
+      <c r="P6" s="102"/>
+      <c r="Q6" s="103"/>
+      <c r="R6" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="S6" s="92" t="s">
+      <c r="S6" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="T6" s="92" t="s">
+      <c r="T6" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="U6" s="95" t="s">
+      <c r="U6" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="V6" s="96"/>
-      <c r="W6" s="96"/>
-      <c r="X6" s="96"/>
-      <c r="Y6" s="96"/>
-      <c r="Z6" s="97"/>
-      <c r="AA6" s="95" t="s">
+      <c r="V6" s="102"/>
+      <c r="W6" s="102"/>
+      <c r="X6" s="102"/>
+      <c r="Y6" s="102"/>
+      <c r="Z6" s="103"/>
+      <c r="AA6" s="101" t="s">
         <v>26</v>
       </c>
-      <c r="AB6" s="96"/>
-      <c r="AC6" s="97"/>
-      <c r="AD6" s="101" t="s">
+      <c r="AB6" s="102"/>
+      <c r="AC6" s="103"/>
+      <c r="AD6" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="AE6" s="102"/>
-      <c r="AF6" s="102"/>
-      <c r="AG6" s="102"/>
-      <c r="AH6" s="102"/>
-      <c r="AI6" s="103"/>
-      <c r="AJ6" s="95" t="s">
+      <c r="AE6" s="108"/>
+      <c r="AF6" s="108"/>
+      <c r="AG6" s="108"/>
+      <c r="AH6" s="108"/>
+      <c r="AI6" s="109"/>
+      <c r="AJ6" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="AK6" s="96"/>
-      <c r="AL6" s="96"/>
-      <c r="AM6" s="96"/>
-      <c r="AN6" s="96"/>
-      <c r="AO6" s="97"/>
-      <c r="AP6" s="87" t="s">
+      <c r="AK6" s="102"/>
+      <c r="AL6" s="102"/>
+      <c r="AM6" s="102"/>
+      <c r="AN6" s="102"/>
+      <c r="AO6" s="103"/>
+      <c r="AP6" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="AQ6" s="88"/>
-      <c r="AR6" s="88"/>
-      <c r="AS6" s="88"/>
-      <c r="AT6" s="88"/>
-      <c r="AU6" s="89"/>
-      <c r="AV6" s="87" t="s">
+      <c r="AQ6" s="85"/>
+      <c r="AR6" s="85"/>
+      <c r="AS6" s="85"/>
+      <c r="AT6" s="85"/>
+      <c r="AU6" s="96"/>
+      <c r="AV6" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="AW6" s="88"/>
-      <c r="AX6" s="88"/>
-      <c r="AY6" s="88"/>
-      <c r="AZ6" s="88"/>
-      <c r="BA6" s="91"/>
-      <c r="BB6" s="84" t="s">
+      <c r="AW6" s="85"/>
+      <c r="AX6" s="85"/>
+      <c r="AY6" s="85"/>
+      <c r="AZ6" s="85"/>
+      <c r="BA6" s="86"/>
+      <c r="BB6" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="BC6" s="85"/>
-      <c r="BD6" s="86"/>
+      <c r="BC6" s="94"/>
+      <c r="BD6" s="95"/>
+      <c r="BE6" s="84" t="s">
+        <v>46</v>
+      </c>
+      <c r="BF6" s="85"/>
+      <c r="BG6" s="86"/>
+      <c r="BH6" s="81" t="s">
+        <v>51</v>
+      </c>
+      <c r="BI6" s="82"/>
+      <c r="BJ6" s="83"/>
     </row>
-    <row r="7" spans="2:56" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="93"/>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="99"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="99"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="107"/>
-      <c r="L7" s="108"/>
-      <c r="M7" s="108"/>
-      <c r="N7" s="108"/>
-      <c r="O7" s="108"/>
-      <c r="P7" s="108"/>
-      <c r="Q7" s="109"/>
-      <c r="R7" s="93"/>
-      <c r="S7" s="93"/>
-      <c r="T7" s="93"/>
-      <c r="U7" s="98"/>
-      <c r="V7" s="99"/>
-      <c r="W7" s="99"/>
-      <c r="X7" s="99"/>
-      <c r="Y7" s="99"/>
-      <c r="Z7" s="100"/>
-      <c r="AA7" s="98"/>
-      <c r="AB7" s="99"/>
-      <c r="AC7" s="100"/>
-      <c r="AD7" s="104"/>
-      <c r="AE7" s="105"/>
-      <c r="AF7" s="105"/>
-      <c r="AG7" s="105"/>
-      <c r="AH7" s="105"/>
-      <c r="AI7" s="106"/>
-      <c r="AJ7" s="98"/>
-      <c r="AK7" s="99"/>
-      <c r="AL7" s="99"/>
-      <c r="AM7" s="99"/>
-      <c r="AN7" s="99"/>
-      <c r="AO7" s="100"/>
-      <c r="AP7" s="82"/>
-      <c r="AQ7" s="81"/>
-      <c r="AR7" s="81"/>
-      <c r="AS7" s="81"/>
-      <c r="AT7" s="81"/>
-      <c r="AU7" s="90"/>
-      <c r="AV7" s="82"/>
-      <c r="AW7" s="81"/>
-      <c r="AX7" s="81"/>
-      <c r="AY7" s="81"/>
-      <c r="AZ7" s="81"/>
-      <c r="BA7" s="83"/>
-      <c r="BB7" s="82" t="s">
+    <row r="7" spans="2:62" s="3" customFormat="1" ht="14.25" customHeight="1">
+      <c r="B7" s="99"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="105"/>
+      <c r="H7" s="105"/>
+      <c r="I7" s="106"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="113"/>
+      <c r="L7" s="114"/>
+      <c r="M7" s="114"/>
+      <c r="N7" s="114"/>
+      <c r="O7" s="114"/>
+      <c r="P7" s="114"/>
+      <c r="Q7" s="115"/>
+      <c r="R7" s="99"/>
+      <c r="S7" s="99"/>
+      <c r="T7" s="99"/>
+      <c r="U7" s="104"/>
+      <c r="V7" s="105"/>
+      <c r="W7" s="105"/>
+      <c r="X7" s="105"/>
+      <c r="Y7" s="105"/>
+      <c r="Z7" s="106"/>
+      <c r="AA7" s="104"/>
+      <c r="AB7" s="105"/>
+      <c r="AC7" s="106"/>
+      <c r="AD7" s="110"/>
+      <c r="AE7" s="111"/>
+      <c r="AF7" s="111"/>
+      <c r="AG7" s="111"/>
+      <c r="AH7" s="111"/>
+      <c r="AI7" s="112"/>
+      <c r="AJ7" s="104"/>
+      <c r="AK7" s="105"/>
+      <c r="AL7" s="105"/>
+      <c r="AM7" s="105"/>
+      <c r="AN7" s="105"/>
+      <c r="AO7" s="106"/>
+      <c r="AP7" s="91"/>
+      <c r="AQ7" s="89"/>
+      <c r="AR7" s="89"/>
+      <c r="AS7" s="89"/>
+      <c r="AT7" s="89"/>
+      <c r="AU7" s="97"/>
+      <c r="AV7" s="91"/>
+      <c r="AW7" s="89"/>
+      <c r="AX7" s="89"/>
+      <c r="AY7" s="89"/>
+      <c r="AZ7" s="89"/>
+      <c r="BA7" s="87"/>
+      <c r="BB7" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="BC7" s="81" t="s">
+      <c r="BC7" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="BD7" s="83" t="s">
+      <c r="BD7" s="87" t="s">
         <v>43</v>
       </c>
+      <c r="BE7" s="91" t="s">
+        <v>47</v>
+      </c>
+      <c r="BF7" s="89" t="s">
+        <v>44</v>
+      </c>
+      <c r="BG7" s="87" t="s">
+        <v>45</v>
+      </c>
+      <c r="BH7" s="91" t="s">
+        <v>50</v>
+      </c>
+      <c r="BI7" s="89" t="s">
+        <v>48</v>
+      </c>
+      <c r="BJ7" s="87" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="8" spans="2:56" s="3" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
+    <row r="8" spans="2:62" s="3" customFormat="1" ht="14.65" thickBot="1">
+      <c r="B8" s="100"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
       <c r="F8" s="31" t="s">
         <v>4</v>
       </c>
@@ -1687,7 +1762,7 @@
       <c r="I8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="94"/>
+      <c r="J8" s="100"/>
       <c r="K8" s="9" t="s">
         <v>29</v>
       </c>
@@ -1709,9 +1784,9 @@
       <c r="Q8" s="7">
         <v>5</v>
       </c>
-      <c r="R8" s="94"/>
-      <c r="S8" s="94"/>
-      <c r="T8" s="94"/>
+      <c r="R8" s="100"/>
+      <c r="S8" s="100"/>
+      <c r="T8" s="100"/>
       <c r="U8" s="9">
         <f>M8</f>
         <v>1</v>
@@ -1816,11 +1891,17 @@
       <c r="BA8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="BB8" s="82"/>
-      <c r="BC8" s="81"/>
-      <c r="BD8" s="83"/>
+      <c r="BB8" s="91"/>
+      <c r="BC8" s="89"/>
+      <c r="BD8" s="87"/>
+      <c r="BE8" s="92"/>
+      <c r="BF8" s="90"/>
+      <c r="BG8" s="88"/>
+      <c r="BH8" s="92"/>
+      <c r="BI8" s="90"/>
+      <c r="BJ8" s="88"/>
     </row>
-    <row r="9" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:62" s="2" customFormat="1">
       <c r="B9" s="51" t="s">
         <v>1</v>
       </c>
@@ -1874,7 +1955,6 @@
       <c r="R9" s="24" t="str">
         <f t="shared" ref="R9:R19" si="1">newline
 &amp; $L9 &amp; " = {" &amp; newline
-&amp; tab &amp; "exists = from" &amp; newline
 &amp; tab &amp; "OR = {" &amp; newline
 &amp; tab &amp; tab &amp; "has_modifier = " &amp; $M9 &amp; newline
 &amp; tab &amp; tab &amp; "has_modifier = " &amp; $N9 &amp; newline
@@ -1885,7 +1965,6 @@
 &amp; "}" &amp; newline</f>
         <v xml:space="preserve">
 buy_influence_has_modifier_0point5_e = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_0point5_e_1
 		has_modifier = buy_influence_0point5_e_2
@@ -1897,9 +1976,9 @@
 </v>
       </c>
       <c r="S9" s="13" t="str">
-        <f t="shared" ref="S9:S19" si="2">newline &amp; tab &amp; tab &amp; tab &amp; $L9 &amp; " = yes"</f>
-        <v xml:space="preserve">
-			buy_influence_has_modifier_0point5_e = yes</v>
+        <f t="shared" ref="S9:S19" si="2">newline &amp; tab &amp; tab &amp; $L9 &amp; " = yes"</f>
+        <v xml:space="preserve">
+		buy_influence_has_modifier_0point5_e = yes</v>
       </c>
       <c r="T9" s="24" t="str">
         <f t="shared" ref="T9:T19" si="3" xml:space="preserve">
@@ -1923,12 +2002,16 @@
 &amp;IF($G9&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G9*$J9*M$8,"")
 &amp;IF($H9&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H9*$J9*M$8,"")
 &amp;IF($I9&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I9*$J9*M$8,"")
+&amp;newline&amp;tab&amp;"show_only_custom_tooltip = no"
+&amp;newline&amp;tab&amp;SUBSTITUTE(event_option_opinion_gain_raw,event_option_opinion_gain_subst_text,$E9)
 &amp;newline&amp;"}"</f>
         <v xml:space="preserve">
 buy_influence_0point5_e_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 0.5
 	country_base_energy_produces_add = -10
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="V9" s="65" t="str">
@@ -1939,12 +2022,16 @@
 &amp;IF($G9&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G9*$J9*N$8,"")
 &amp;IF($H9&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H9*$J9*N$8,"")
 &amp;IF($I9&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I9*$J9*N$8,"")
+&amp;newline&amp;tab&amp;"show_only_custom_tooltip = no"
+&amp;newline&amp;tab&amp;SUBSTITUTE(event_option_opinion_gain_raw,event_option_opinion_gain_subst_text,$E9)
 &amp;newline&amp;"}"</f>
         <v xml:space="preserve">
 buy_influence_0point5_e_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 0.5
 	country_base_energy_produces_add = -20
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="W9" s="65" t="str">
@@ -1955,12 +2042,16 @@
 &amp;IF($G9&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G9*$J9*O$8,"")
 &amp;IF($H9&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H9*$J9*O$8,"")
 &amp;IF($I9&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I9*$J9*O$8,"")
+&amp;newline&amp;tab&amp;"show_only_custom_tooltip = no"
+&amp;newline&amp;tab&amp;SUBSTITUTE(event_option_opinion_gain_raw,event_option_opinion_gain_subst_text,$E9)
 &amp;newline&amp;"}"</f>
         <v xml:space="preserve">
 buy_influence_0point5_e_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 0.5
 	country_base_energy_produces_add = -30
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="X9" s="65" t="str">
@@ -1971,12 +2062,16 @@
 &amp;IF($G9&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G9*$J9*P$8,"")
 &amp;IF($H9&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H9*$J9*P$8,"")
 &amp;IF($I9&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I9*$J9*P$8,"")
+&amp;newline&amp;tab&amp;"show_only_custom_tooltip = no"
+&amp;newline&amp;tab&amp;SUBSTITUTE(event_option_opinion_gain_raw,event_option_opinion_gain_subst_text,$E9)
 &amp;newline&amp;"}"</f>
         <v xml:space="preserve">
 buy_influence_0point5_e_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 0.5
 	country_base_energy_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="Y9" s="67" t="str">
@@ -1987,12 +2082,16 @@
 &amp;IF($G9&gt;0,newline&amp;tab&amp;"country_base_minerals_produces_add = -"&amp;$G9*$J9*Q$8,"")
 &amp;IF($H9&gt;0,newline&amp;tab&amp;"country_base_food_produces_add = -"&amp;$H9*$J9*Q$8,"")
 &amp;IF($I9&gt;0,newline&amp;tab&amp;"country_base_consumer_goods_produces_add = -"&amp;$I9*$J9*Q$8,"")
+&amp;newline&amp;tab&amp;"show_only_custom_tooltip = no"
+&amp;newline&amp;tab&amp;SUBSTITUTE(event_option_opinion_gain_raw,event_option_opinion_gain_subst_text,$E9)
 &amp;newline&amp;"}"</f>
         <v xml:space="preserve">
 buy_influence_0point5_e_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 0.5
 	country_base_energy_produces_add = -50
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="Z9" s="66" t="str">
@@ -2002,26 +2101,36 @@
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 0.5
 	country_base_energy_produces_add = -10
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_0point5_e_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 0.5
 	country_base_energy_produces_add = -20
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_0point5_e_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 0.5
 	country_base_energy_produces_add = -30
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_0point5_e_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 0.5
 	country_base_energy_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_0point5_e_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 0.5
 	country_base_energy_produces_add = -50
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="AA9" s="68" t="str">
@@ -2041,7 +2150,6 @@
 tab &amp; tab &amp; "name = " &amp; $AA9 &amp; newline &amp;
 AD$1 &amp; newline &amp;
 SUBSTITUTE(event_option_add_static_modifier_raw,event_option_add_static_modifier_subst_text,M9) &amp; newline &amp;
-SUBSTITUTE(event_option_opinion_gain_raw,event_option_opinion_gain_subst_text,$E9) &amp; newline &amp;
 event_option_trigger_renewal_event &amp; newline &amp;
 tab &amp; "}" &amp; newline</f>
         <v xml:space="preserve">	option = {
@@ -2053,7 +2161,6 @@
 			modifier = buy_influence_0point5_e_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2068,7 +2175,6 @@
 tab &amp; tab &amp; "name = " &amp; $AA9 &amp; newline &amp;
 AE$1 &amp; newline &amp;
 SUBSTITUTE(event_option_add_static_modifier_raw,event_option_add_static_modifier_subst_text,N9) &amp; newline &amp;
-SUBSTITUTE(event_option_opinion_gain_raw,event_option_opinion_gain_subst_text,$E9) &amp; newline &amp;
 event_option_trigger_renewal_event &amp; newline &amp;
 tab &amp; "}" &amp; newline</f>
         <v xml:space="preserve">	option = {
@@ -2081,7 +2187,6 @@
 			modifier = buy_influence_0point5_e_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2096,7 +2201,6 @@
 tab &amp; tab &amp; "name = " &amp; $AA9 &amp; newline &amp;
 AF$1 &amp; newline &amp;
 SUBSTITUTE(event_option_add_static_modifier_raw,event_option_add_static_modifier_subst_text,O9) &amp; newline &amp;
-SUBSTITUTE(event_option_opinion_gain_raw,event_option_opinion_gain_subst_text,$E9) &amp; newline &amp;
 event_option_trigger_renewal_event &amp; newline &amp;
 tab &amp; "}" &amp; newline</f>
         <v xml:space="preserve">	option = {
@@ -2109,7 +2213,6 @@
 			modifier = buy_influence_0point5_e_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2124,7 +2227,6 @@
 tab &amp; tab &amp; "name = " &amp; $AA9 &amp; newline &amp;
 AG$1 &amp; newline &amp;
 SUBSTITUTE(event_option_add_static_modifier_raw,event_option_add_static_modifier_subst_text,P9) &amp; newline &amp;
-SUBSTITUTE(event_option_opinion_gain_raw,event_option_opinion_gain_subst_text,$E9) &amp; newline &amp;
 event_option_trigger_renewal_event &amp; newline &amp;
 tab &amp; "}" &amp; newline</f>
         <v xml:space="preserve">	option = {
@@ -2137,7 +2239,6 @@
 			modifier = buy_influence_0point5_e_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2152,7 +2253,6 @@
 tab &amp; tab &amp; "name = " &amp; $AA9 &amp; newline &amp;
 AH$1 &amp; newline &amp;
 SUBSTITUTE(event_option_add_static_modifier_raw,event_option_add_static_modifier_subst_text,Q9) &amp; newline &amp;
-SUBSTITUTE(event_option_opinion_gain_raw,event_option_opinion_gain_subst_text,$E9) &amp; newline &amp;
 event_option_trigger_renewal_event &amp; newline &amp;
 tab &amp; "}" &amp; newline</f>
         <v xml:space="preserve">	option = {
@@ -2164,7 +2264,6 @@
 			modifier = buy_influence_0point5_e_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2185,7 +2284,6 @@
 			modifier = buy_influence_0point5_e_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2203,7 +2301,6 @@
 			modifier = buy_influence_0point5_e_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2221,7 +2318,6 @@
 			modifier = buy_influence_0point5_e_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2239,7 +2335,6 @@
 			modifier = buy_influence_0point5_e_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2256,7 +2351,6 @@
 			modifier = buy_influence_0point5_e_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2414,8 +2508,43 @@
 	}
 }</v>
       </c>
+      <c r="BE9" s="12" t="str">
+        <f>SUBSTITUTE($K9,"buy_influence","buy_influence_renewal")</f>
+        <v>buy_influence_renewal_0point5_e</v>
+      </c>
+      <c r="BF9" s="72" t="str">
+        <f t="shared" ref="BF9:BF19" si="33" xml:space="preserve">
+tab &amp; tab &amp; IF(ROW()=ROW($A$9),"","else_") &amp; "if = {" &amp; newline &amp;
+tab &amp; tab &amp; tab &amp; "limit = { " &amp; $L9 &amp; " = yes }" &amp; newline &amp;
+tab &amp; tab &amp; tab &amp; "set_country_flag = " &amp; $BE9 &amp; newline &amp;
+tab &amp; tab &amp; "}" &amp; newline</f>
+        <v xml:space="preserve">		if = {
+			limit = { buy_influence_has_modifier_0point5_e = yes }
+			set_country_flag = buy_influence_renewal_0point5_e
+		}
+</v>
+      </c>
+      <c r="BG9" s="74" t="str">
+        <f t="shared" ref="BG9:BG19" si="34">newline &amp; tab &amp; tab &amp; "remove_country_flag = " &amp; $BE9</f>
+        <v xml:space="preserve">
+		remove_country_flag = buy_influence_renewal_0point5_e</v>
+      </c>
+      <c r="BH9" s="64" t="str">
+        <f>SUBSTITUTE($BE9,"buy_influence_renewal","buy_influence.101.renewal")</f>
+        <v>buy_influence.101.renewal_0point5_e</v>
+      </c>
+      <c r="BI9" s="65" t="str">
+        <f t="shared" ref="BI9:BI19" si="35">tab &amp; tab &amp; tab &amp; tab &amp; $BE9 &amp; " = { text = " &amp; $BH9 &amp; " }" &amp; newline</f>
+        <v xml:space="preserve">				buy_influence_renewal_0point5_e = { text = buy_influence.101.renewal_0point5_e }
+</v>
+      </c>
+      <c r="BJ9" s="66" t="str">
+        <f t="shared" ref="BJ9:BJ19" si="36">space &amp; $BH9 &amp; ":0 ""Expired campaign: §Y$" &amp; $AA9 &amp; "$§!\n\n$buy_influence.101.renewal$""" &amp; newline</f>
+        <v xml:space="preserve"> buy_influence.101.renewal_0point5_e:0 "Expired campaign: §Y$buy_influence_0point5_e_name$§!\n\n$buy_influence.101.renewal$"
+</v>
+      </c>
     </row>
-    <row r="10" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:62" s="2" customFormat="1">
       <c r="B10" s="55" t="s">
         <v>1</v>
       </c>
@@ -2426,7 +2555,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="43">
-        <f t="shared" ref="E10:E19" si="33">MAX(1,ROUNDUP(D10,0))</f>
+        <f t="shared" ref="E10:E19" si="37">MAX(1,ROUNDUP(D10,0))</f>
         <v>1</v>
       </c>
       <c r="F10" s="57">
@@ -2439,15 +2568,15 @@
         <v>1</v>
       </c>
       <c r="K10" s="14" t="str">
-        <f t="shared" ref="K10:K19" si="34">"buy_influence_"&amp;ROUNDDOWN($D10,0)&amp;"point"&amp;(ROUNDDOWN($D10*10,0)-(ROUNDDOWN($D10,0)*10))&amp;"_"&amp;$C10</f>
+        <f t="shared" ref="K10:K19" si="38">"buy_influence_"&amp;ROUNDDOWN($D10,0)&amp;"point"&amp;(ROUNDDOWN($D10*10,0)-(ROUNDDOWN($D10,0)*10))&amp;"_"&amp;$C10</f>
         <v>buy_influence_1point0_e</v>
       </c>
       <c r="L10" s="76" t="str">
-        <f t="shared" ref="L10:L19" si="35">SUBSTITUTE($K10,"buy_influence_","buy_influence_has_modifier_")</f>
+        <f t="shared" ref="L10:L19" si="39">SUBSTITUTE($K10,"buy_influence_","buy_influence_has_modifier_")</f>
         <v>buy_influence_has_modifier_1point0_e</v>
       </c>
       <c r="M10" s="36" t="str">
-        <f t="shared" ref="M10:M19" si="36">$K10&amp;"_"&amp;M$8</f>
+        <f t="shared" ref="M10:M19" si="40">$K10&amp;"_"&amp;M$8</f>
         <v>buy_influence_1point0_e_1</v>
       </c>
       <c r="N10" s="37" t="str">
@@ -2470,7 +2599,6 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">
 buy_influence_has_modifier_1point0_e = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_1point0_e_1
 		has_modifier = buy_influence_1point0_e_2
@@ -2484,7 +2612,7 @@
       <c r="S10" s="17" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">
-			buy_influence_has_modifier_1point0_e = yes</v>
+		buy_influence_has_modifier_1point0_e = yes</v>
       </c>
       <c r="T10" s="25" t="str">
         <f t="shared" si="3"/>
@@ -2502,6 +2630,8 @@
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -30
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="V10" s="15" t="str">
@@ -2511,6 +2641,8 @@
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -60
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="W10" s="15" t="str">
@@ -2520,6 +2652,8 @@
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -90
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="X10" s="15" t="str">
@@ -2529,6 +2663,8 @@
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="Y10" s="18" t="str">
@@ -2538,47 +2674,59 @@
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -150
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="Z10" s="16" t="str">
-        <f t="shared" ref="Z10:Z19" si="37">CONCATENATE(U10,V10,W10,X10,Y10)</f>
+        <f t="shared" ref="Z10:Z19" si="41">CONCATENATE(U10,V10,W10,X10,Y10)</f>
         <v xml:space="preserve">
 buy_influence_1point0_e_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -30
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_e_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -60
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_e_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -90
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_e_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_e_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -150
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="AA10" s="25" t="str">
-        <f t="shared" ref="AA10:AA19" si="38">$K10&amp;"_name"</f>
+        <f t="shared" ref="AA10:AA19" si="42">$K10&amp;"_name"</f>
         <v>buy_influence_1point0_e_name</v>
       </c>
       <c r="AB10" s="15" t="str">
-        <f t="shared" ref="AB10:AB19" si="39">$K10&amp;"_desc"</f>
+        <f t="shared" ref="AB10:AB19" si="43">$K10&amp;"_desc"</f>
         <v>buy_influence_1point0_e_desc</v>
       </c>
       <c r="AC10" s="70" t="str">
-        <f t="shared" ref="AC10:AC19" si="40">$K10&amp;"_response"</f>
+        <f t="shared" ref="AC10:AC19" si="44">$K10&amp;"_response"</f>
         <v>buy_influence_1point0_e_response</v>
       </c>
       <c r="AD10" s="14" t="str">
@@ -2592,7 +2740,6 @@
 			modifier = buy_influence_1point0_e_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2614,7 +2761,6 @@
 			modifier = buy_influence_1point0_e_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2636,7 +2782,6 @@
 			modifier = buy_influence_1point0_e_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2658,7 +2803,6 @@
 			modifier = buy_influence_1point0_e_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2679,7 +2823,6 @@
 			modifier = buy_influence_1point0_e_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2690,7 +2833,7 @@
 </v>
       </c>
       <c r="AI10" s="16" t="str">
-        <f t="shared" ref="AI10:AI19" si="41">CONCATENATE(AD10,AE10,AF10,AG10,AH10)</f>
+        <f t="shared" ref="AI10:AI19" si="45">CONCATENATE(AD10,AE10,AF10,AG10,AH10)</f>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_e_name
 		trigger = {
@@ -2700,7 +2843,6 @@
 			modifier = buy_influence_1point0_e_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2718,7 +2860,6 @@
 			modifier = buy_influence_1point0_e_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2736,7 +2877,6 @@
 			modifier = buy_influence_1point0_e_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2754,7 +2894,6 @@
 			modifier = buy_influence_1point0_e_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2771,7 +2910,6 @@
 			modifier = buy_influence_1point0_e_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -2884,11 +3022,11 @@
  buy_influence_1point0_e_5_desc:0 "$buy_influence_1point0_e_desc$"</v>
       </c>
       <c r="BB10" s="79">
-        <f t="shared" ref="BB10:BB19" si="42">(200 + ((ROW()-ROW($B$9)+1)*10))</f>
+        <f t="shared" ref="BB10:BB19" si="46">(200 + ((ROW()-ROW($B$9)+1)*10))</f>
         <v>220</v>
       </c>
       <c r="BC10" s="15" t="str">
-        <f t="shared" ref="BC10:BC19" si="43">newline &amp;
+        <f t="shared" ref="BC10:BC19" si="47">newline &amp;
 tab &amp; tab &amp; IF(ROW()=ROW($B$9),"","else_") &amp; "if = {" &amp; newline &amp;
 tab &amp; tab &amp; tab &amp; "limit = { " &amp; $L10 &amp; " = yes }" &amp; newline &amp;
 tab &amp; tab &amp; tab &amp; "country_event = { id = buy_influence." &amp; (200 + ((ROW()-ROW($B$9)+1)*10)) &amp; " }" &amp; newline &amp;
@@ -2916,8 +3054,39 @@
 	}
 }</v>
       </c>
+      <c r="BE10" s="14" t="str">
+        <f t="shared" ref="BE10:BE19" si="48">SUBSTITUTE($K10,"buy_influence","buy_influence_renewal")</f>
+        <v>buy_influence_renewal_1point0_e</v>
+      </c>
+      <c r="BF10" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v xml:space="preserve">		else_if = {
+			limit = { buy_influence_has_modifier_1point0_e = yes }
+			set_country_flag = buy_influence_renewal_1point0_e
+		}
+</v>
+      </c>
+      <c r="BG10" s="16" t="str">
+        <f t="shared" si="34"/>
+        <v xml:space="preserve">
+		remove_country_flag = buy_influence_renewal_1point0_e</v>
+      </c>
+      <c r="BH10" s="14" t="str">
+        <f t="shared" ref="BH10:BH19" si="49">SUBSTITUTE($BE10,"buy_influence_renewal","buy_influence.101.renewal")</f>
+        <v>buy_influence.101.renewal_1point0_e</v>
+      </c>
+      <c r="BI10" s="15" t="str">
+        <f t="shared" si="35"/>
+        <v xml:space="preserve">				buy_influence_renewal_1point0_e = { text = buy_influence.101.renewal_1point0_e }
+</v>
+      </c>
+      <c r="BJ10" s="16" t="str">
+        <f t="shared" si="36"/>
+        <v xml:space="preserve"> buy_influence.101.renewal_1point0_e:0 "Expired campaign: §Y$buy_influence_1point0_e_name$§!\n\n$buy_influence.101.renewal$"
+</v>
+      </c>
     </row>
-    <row r="11" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:62" s="2" customFormat="1">
       <c r="B11" s="55" t="s">
         <v>8</v>
       </c>
@@ -2928,7 +3097,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="43">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="F11" s="57">
@@ -2943,15 +3112,15 @@
         <v>1</v>
       </c>
       <c r="K11" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>buy_influence_1point0_em</v>
       </c>
       <c r="L11" s="76" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>buy_influence_has_modifier_1point0_em</v>
       </c>
       <c r="M11" s="36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>buy_influence_1point0_em_1</v>
       </c>
       <c r="N11" s="37" t="str">
@@ -2974,7 +3143,6 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">
 buy_influence_has_modifier_1point0_em = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_1point0_em_1
 		has_modifier = buy_influence_1point0_em_2
@@ -2988,7 +3156,7 @@
       <c r="S11" s="17" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">
-			buy_influence_has_modifier_1point0_em = yes</v>
+		buy_influence_has_modifier_1point0_em = yes</v>
       </c>
       <c r="T11" s="25" t="str">
         <f t="shared" si="3"/>
@@ -3007,6 +3175,8 @@
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -20
 	country_base_minerals_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="V11" s="15" t="str">
@@ -3017,6 +3187,8 @@
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -40
 	country_base_minerals_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="W11" s="15" t="str">
@@ -3027,6 +3199,8 @@
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -60
 	country_base_minerals_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="X11" s="15" t="str">
@@ -3037,6 +3211,8 @@
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -80
 	country_base_minerals_produces_add = -160
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="Y11" s="18" t="str">
@@ -3047,52 +3223,64 @@
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -100
 	country_base_minerals_produces_add = -200
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="Z11" s="16" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v xml:space="preserve">
 buy_influence_1point0_em_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -20
 	country_base_minerals_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_em_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -40
 	country_base_minerals_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_em_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -60
 	country_base_minerals_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_em_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -80
 	country_base_minerals_produces_add = -160
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_em_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -100
 	country_base_minerals_produces_add = -200
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="AA11" s="25" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>buy_influence_1point0_em_name</v>
       </c>
       <c r="AB11" s="15" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>buy_influence_1point0_em_desc</v>
       </c>
       <c r="AC11" s="70" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>buy_influence_1point0_em_response</v>
       </c>
       <c r="AD11" s="14" t="str">
@@ -3106,7 +3294,6 @@
 			modifier = buy_influence_1point0_em_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3128,7 +3315,6 @@
 			modifier = buy_influence_1point0_em_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3150,7 +3336,6 @@
 			modifier = buy_influence_1point0_em_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3172,7 +3357,6 @@
 			modifier = buy_influence_1point0_em_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3193,7 +3377,6 @@
 			modifier = buy_influence_1point0_em_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3204,7 +3387,7 @@
 </v>
       </c>
       <c r="AI11" s="16" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_em_name
 		trigger = {
@@ -3214,7 +3397,6 @@
 			modifier = buy_influence_1point0_em_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3232,7 +3414,6 @@
 			modifier = buy_influence_1point0_em_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3250,7 +3431,6 @@
 			modifier = buy_influence_1point0_em_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3268,7 +3448,6 @@
 			modifier = buy_influence_1point0_em_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3285,7 +3464,6 @@
 			modifier = buy_influence_1point0_em_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3398,11 +3576,11 @@
  buy_influence_1point0_em_5_desc:0 "$buy_influence_1point0_em_desc$"</v>
       </c>
       <c r="BB11" s="79">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>230</v>
       </c>
       <c r="BC11" s="15" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v xml:space="preserve">
 		else_if = {
 			limit = { buy_influence_has_modifier_1point0_em = yes }
@@ -3426,8 +3604,39 @@
 	}
 }</v>
       </c>
+      <c r="BE11" s="14" t="str">
+        <f t="shared" si="48"/>
+        <v>buy_influence_renewal_1point0_em</v>
+      </c>
+      <c r="BF11" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v xml:space="preserve">		else_if = {
+			limit = { buy_influence_has_modifier_1point0_em = yes }
+			set_country_flag = buy_influence_renewal_1point0_em
+		}
+</v>
+      </c>
+      <c r="BG11" s="16" t="str">
+        <f t="shared" si="34"/>
+        <v xml:space="preserve">
+		remove_country_flag = buy_influence_renewal_1point0_em</v>
+      </c>
+      <c r="BH11" s="14" t="str">
+        <f t="shared" si="49"/>
+        <v>buy_influence.101.renewal_1point0_em</v>
+      </c>
+      <c r="BI11" s="15" t="str">
+        <f t="shared" si="35"/>
+        <v xml:space="preserve">				buy_influence_renewal_1point0_em = { text = buy_influence.101.renewal_1point0_em }
+</v>
+      </c>
+      <c r="BJ11" s="16" t="str">
+        <f t="shared" si="36"/>
+        <v xml:space="preserve"> buy_influence.101.renewal_1point0_em:0 "Expired campaign: §Y$buy_influence_1point0_em_name$§!\n\n$buy_influence.101.renewal$"
+</v>
+      </c>
     </row>
-    <row r="12" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:62" s="2" customFormat="1">
       <c r="B12" s="55" t="s">
         <v>8</v>
       </c>
@@ -3438,7 +3647,7 @@
         <v>1.5</v>
       </c>
       <c r="E12" s="43">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>2</v>
       </c>
       <c r="F12" s="57">
@@ -3453,15 +3662,15 @@
         <v>1</v>
       </c>
       <c r="K12" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>buy_influence_1point5_em</v>
       </c>
       <c r="L12" s="76" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>buy_influence_has_modifier_1point5_em</v>
       </c>
       <c r="M12" s="36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>buy_influence_1point5_em_1</v>
       </c>
       <c r="N12" s="37" t="str">
@@ -3484,7 +3693,6 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">
 buy_influence_has_modifier_1point5_em = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_1point5_em_1
 		has_modifier = buy_influence_1point5_em_2
@@ -3498,7 +3706,7 @@
       <c r="S12" s="17" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">
-			buy_influence_has_modifier_1point5_em = yes</v>
+		buy_influence_has_modifier_1point5_em = yes</v>
       </c>
       <c r="T12" s="25" t="str">
         <f t="shared" si="3"/>
@@ -3517,6 +3725,8 @@
 	country_base_influence_produces_add = 1.5
 	country_base_energy_produces_add = -40
 	country_base_minerals_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="V12" s="15" t="str">
@@ -3527,6 +3737,8 @@
 	country_base_influence_produces_add = 1.5
 	country_base_energy_produces_add = -80
 	country_base_minerals_produces_add = -160
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="W12" s="15" t="str">
@@ -3537,6 +3749,8 @@
 	country_base_influence_produces_add = 1.5
 	country_base_energy_produces_add = -120
 	country_base_minerals_produces_add = -240
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="X12" s="15" t="str">
@@ -3547,6 +3761,8 @@
 	country_base_influence_produces_add = 1.5
 	country_base_energy_produces_add = -160
 	country_base_minerals_produces_add = -320
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="Y12" s="18" t="str">
@@ -3557,52 +3773,64 @@
 	country_base_influence_produces_add = 1.5
 	country_base_energy_produces_add = -200
 	country_base_minerals_produces_add = -400
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="Z12" s="16" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v xml:space="preserve">
 buy_influence_1point5_em_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_energy_produces_add = -40
 	country_base_minerals_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point5_em_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_energy_produces_add = -80
 	country_base_minerals_produces_add = -160
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point5_em_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_energy_produces_add = -120
 	country_base_minerals_produces_add = -240
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point5_em_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_energy_produces_add = -160
 	country_base_minerals_produces_add = -320
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point5_em_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_energy_produces_add = -200
 	country_base_minerals_produces_add = -400
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="AA12" s="25" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>buy_influence_1point5_em_name</v>
       </c>
       <c r="AB12" s="15" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>buy_influence_1point5_em_desc</v>
       </c>
       <c r="AC12" s="70" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>buy_influence_1point5_em_response</v>
       </c>
       <c r="AD12" s="14" t="str">
@@ -3616,7 +3844,6 @@
 			modifier = buy_influence_1point5_em_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3638,7 +3865,6 @@
 			modifier = buy_influence_1point5_em_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3660,7 +3886,6 @@
 			modifier = buy_influence_1point5_em_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3682,7 +3907,6 @@
 			modifier = buy_influence_1point5_em_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3703,7 +3927,6 @@
 			modifier = buy_influence_1point5_em_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3714,7 +3937,7 @@
 </v>
       </c>
       <c r="AI12" s="16" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point5_em_name
 		trigger = {
@@ -3724,7 +3947,6 @@
 			modifier = buy_influence_1point5_em_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3742,7 +3964,6 @@
 			modifier = buy_influence_1point5_em_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3760,7 +3981,6 @@
 			modifier = buy_influence_1point5_em_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3778,7 +3998,6 @@
 			modifier = buy_influence_1point5_em_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3795,7 +4014,6 @@
 			modifier = buy_influence_1point5_em_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -3908,11 +4126,11 @@
  buy_influence_1point5_em_5_desc:0 "$buy_influence_1point5_em_desc$"</v>
       </c>
       <c r="BB12" s="79">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>240</v>
       </c>
       <c r="BC12" s="15" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v xml:space="preserve">
 		else_if = {
 			limit = { buy_influence_has_modifier_1point5_em = yes }
@@ -3936,8 +4154,39 @@
 	}
 }</v>
       </c>
+      <c r="BE12" s="14" t="str">
+        <f t="shared" si="48"/>
+        <v>buy_influence_renewal_1point5_em</v>
+      </c>
+      <c r="BF12" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v xml:space="preserve">		else_if = {
+			limit = { buy_influence_has_modifier_1point5_em = yes }
+			set_country_flag = buy_influence_renewal_1point5_em
+		}
+</v>
+      </c>
+      <c r="BG12" s="16" t="str">
+        <f t="shared" si="34"/>
+        <v xml:space="preserve">
+		remove_country_flag = buy_influence_renewal_1point5_em</v>
+      </c>
+      <c r="BH12" s="14" t="str">
+        <f t="shared" si="49"/>
+        <v>buy_influence.101.renewal_1point5_em</v>
+      </c>
+      <c r="BI12" s="15" t="str">
+        <f t="shared" si="35"/>
+        <v xml:space="preserve">				buy_influence_renewal_1point5_em = { text = buy_influence.101.renewal_1point5_em }
+</v>
+      </c>
+      <c r="BJ12" s="16" t="str">
+        <f t="shared" si="36"/>
+        <v xml:space="preserve"> buy_influence.101.renewal_1point5_em:0 "Expired campaign: §Y$buy_influence_1point5_em_name$§!\n\n$buy_influence.101.renewal$"
+</v>
+      </c>
     </row>
-    <row r="13" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:62" s="2" customFormat="1">
       <c r="B13" s="55" t="s">
         <v>8</v>
       </c>
@@ -3948,7 +4197,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="43">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>2</v>
       </c>
       <c r="F13" s="57">
@@ -3963,15 +4212,15 @@
         <v>1</v>
       </c>
       <c r="K13" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>buy_influence_2point0_em</v>
       </c>
       <c r="L13" s="76" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>buy_influence_has_modifier_2point0_em</v>
       </c>
       <c r="M13" s="36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>buy_influence_2point0_em_1</v>
       </c>
       <c r="N13" s="37" t="str">
@@ -3994,7 +4243,6 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">
 buy_influence_has_modifier_2point0_em = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_2point0_em_1
 		has_modifier = buy_influence_2point0_em_2
@@ -4008,7 +4256,7 @@
       <c r="S13" s="17" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">
-			buy_influence_has_modifier_2point0_em = yes</v>
+		buy_influence_has_modifier_2point0_em = yes</v>
       </c>
       <c r="T13" s="25" t="str">
         <f t="shared" si="3"/>
@@ -4027,6 +4275,8 @@
 	country_base_influence_produces_add = 2
 	country_base_energy_produces_add = -60
 	country_base_minerals_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="V13" s="15" t="str">
@@ -4037,6 +4287,8 @@
 	country_base_influence_produces_add = 2
 	country_base_energy_produces_add = -120
 	country_base_minerals_produces_add = -240
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="W13" s="15" t="str">
@@ -4047,6 +4299,8 @@
 	country_base_influence_produces_add = 2
 	country_base_energy_produces_add = -180
 	country_base_minerals_produces_add = -360
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="X13" s="15" t="str">
@@ -4057,6 +4311,8 @@
 	country_base_influence_produces_add = 2
 	country_base_energy_produces_add = -240
 	country_base_minerals_produces_add = -480
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="Y13" s="18" t="str">
@@ -4067,52 +4323,64 @@
 	country_base_influence_produces_add = 2
 	country_base_energy_produces_add = -300
 	country_base_minerals_produces_add = -600
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="Z13" s="16" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v xml:space="preserve">
 buy_influence_2point0_em_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_energy_produces_add = -60
 	country_base_minerals_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_em_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_energy_produces_add = -120
 	country_base_minerals_produces_add = -240
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_em_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_energy_produces_add = -180
 	country_base_minerals_produces_add = -360
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_em_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_energy_produces_add = -240
 	country_base_minerals_produces_add = -480
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_em_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_energy_produces_add = -300
 	country_base_minerals_produces_add = -600
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="AA13" s="25" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>buy_influence_2point0_em_name</v>
       </c>
       <c r="AB13" s="15" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>buy_influence_2point0_em_desc</v>
       </c>
       <c r="AC13" s="70" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>buy_influence_2point0_em_response</v>
       </c>
       <c r="AD13" s="14" t="str">
@@ -4126,7 +4394,6 @@
 			modifier = buy_influence_2point0_em_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4148,7 +4415,6 @@
 			modifier = buy_influence_2point0_em_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4170,7 +4436,6 @@
 			modifier = buy_influence_2point0_em_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4192,7 +4457,6 @@
 			modifier = buy_influence_2point0_em_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4213,7 +4477,6 @@
 			modifier = buy_influence_2point0_em_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4224,7 +4487,7 @@
 </v>
       </c>
       <c r="AI13" s="16" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_em_name
 		trigger = {
@@ -4234,7 +4497,6 @@
 			modifier = buy_influence_2point0_em_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4252,7 +4514,6 @@
 			modifier = buy_influence_2point0_em_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4270,7 +4531,6 @@
 			modifier = buy_influence_2point0_em_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4288,7 +4548,6 @@
 			modifier = buy_influence_2point0_em_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4305,7 +4564,6 @@
 			modifier = buy_influence_2point0_em_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4418,11 +4676,11 @@
  buy_influence_2point0_em_5_desc:0 "$buy_influence_2point0_em_desc$"</v>
       </c>
       <c r="BB13" s="79">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>250</v>
       </c>
       <c r="BC13" s="15" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v xml:space="preserve">
 		else_if = {
 			limit = { buy_influence_has_modifier_2point0_em = yes }
@@ -4446,8 +4704,39 @@
 	}
 }</v>
       </c>
+      <c r="BE13" s="14" t="str">
+        <f t="shared" si="48"/>
+        <v>buy_influence_renewal_2point0_em</v>
+      </c>
+      <c r="BF13" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v xml:space="preserve">		else_if = {
+			limit = { buy_influence_has_modifier_2point0_em = yes }
+			set_country_flag = buy_influence_renewal_2point0_em
+		}
+</v>
+      </c>
+      <c r="BG13" s="16" t="str">
+        <f t="shared" si="34"/>
+        <v xml:space="preserve">
+		remove_country_flag = buy_influence_renewal_2point0_em</v>
+      </c>
+      <c r="BH13" s="14" t="str">
+        <f t="shared" si="49"/>
+        <v>buy_influence.101.renewal_2point0_em</v>
+      </c>
+      <c r="BI13" s="15" t="str">
+        <f t="shared" si="35"/>
+        <v xml:space="preserve">				buy_influence_renewal_2point0_em = { text = buy_influence.101.renewal_2point0_em }
+</v>
+      </c>
+      <c r="BJ13" s="16" t="str">
+        <f t="shared" si="36"/>
+        <v xml:space="preserve"> buy_influence.101.renewal_2point0_em:0 "Expired campaign: §Y$buy_influence_2point0_em_name$§!\n\n$buy_influence.101.renewal$"
+</v>
+      </c>
     </row>
-    <row r="14" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:62" s="2" customFormat="1">
       <c r="B14" s="55" t="s">
         <v>12</v>
       </c>
@@ -4458,7 +4747,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="43">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="F14" s="57"/>
@@ -4473,15 +4762,15 @@
         <v>1</v>
       </c>
       <c r="K14" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>buy_influence_1point0_mf</v>
       </c>
       <c r="L14" s="76" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>buy_influence_has_modifier_1point0_mf</v>
       </c>
       <c r="M14" s="36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>buy_influence_1point0_mf_1</v>
       </c>
       <c r="N14" s="37" t="str">
@@ -4504,7 +4793,6 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">
 buy_influence_has_modifier_1point0_mf = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_1point0_mf_1
 		has_modifier = buy_influence_1point0_mf_2
@@ -4518,7 +4806,7 @@
       <c r="S14" s="17" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">
-			buy_influence_has_modifier_1point0_mf = yes</v>
+		buy_influence_has_modifier_1point0_mf = yes</v>
       </c>
       <c r="T14" s="25" t="str">
         <f t="shared" si="3"/>
@@ -4537,6 +4825,8 @@
 	country_base_influence_produces_add = 1
 	country_base_minerals_produces_add = -40
 	country_base_food_produces_add = -20
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="V14" s="15" t="str">
@@ -4547,6 +4837,8 @@
 	country_base_influence_produces_add = 1
 	country_base_minerals_produces_add = -80
 	country_base_food_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="W14" s="15" t="str">
@@ -4557,6 +4849,8 @@
 	country_base_influence_produces_add = 1
 	country_base_minerals_produces_add = -120
 	country_base_food_produces_add = -60
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="X14" s="15" t="str">
@@ -4567,6 +4861,8 @@
 	country_base_influence_produces_add = 1
 	country_base_minerals_produces_add = -160
 	country_base_food_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="Y14" s="18" t="str">
@@ -4577,52 +4873,64 @@
 	country_base_influence_produces_add = 1
 	country_base_minerals_produces_add = -200
 	country_base_food_produces_add = -100
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="Z14" s="16" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v xml:space="preserve">
 buy_influence_1point0_mf_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_minerals_produces_add = -40
 	country_base_food_produces_add = -20
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_mf_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_minerals_produces_add = -80
 	country_base_food_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_mf_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_minerals_produces_add = -120
 	country_base_food_produces_add = -60
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_mf_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_minerals_produces_add = -160
 	country_base_food_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_mf_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_minerals_produces_add = -200
 	country_base_food_produces_add = -100
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }</v>
       </c>
       <c r="AA14" s="25" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>buy_influence_1point0_mf_name</v>
       </c>
       <c r="AB14" s="15" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>buy_influence_1point0_mf_desc</v>
       </c>
       <c r="AC14" s="70" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>buy_influence_1point0_mf_response</v>
       </c>
       <c r="AD14" s="14" t="str">
@@ -4636,7 +4944,6 @@
 			modifier = buy_influence_1point0_mf_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4658,7 +4965,6 @@
 			modifier = buy_influence_1point0_mf_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4680,7 +4986,6 @@
 			modifier = buy_influence_1point0_mf_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4702,7 +5007,6 @@
 			modifier = buy_influence_1point0_mf_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4723,7 +5027,6 @@
 			modifier = buy_influence_1point0_mf_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4734,7 +5037,7 @@
 </v>
       </c>
       <c r="AI14" s="16" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point0_mf_name
 		trigger = {
@@ -4744,7 +5047,6 @@
 			modifier = buy_influence_1point0_mf_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4762,7 +5064,6 @@
 			modifier = buy_influence_1point0_mf_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4780,7 +5081,6 @@
 			modifier = buy_influence_1point0_mf_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4798,7 +5098,6 @@
 			modifier = buy_influence_1point0_mf_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4815,7 +5114,6 @@
 			modifier = buy_influence_1point0_mf_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -4928,11 +5226,11 @@
  buy_influence_1point0_mf_5_desc:0 "$buy_influence_1point0_mf_desc$"</v>
       </c>
       <c r="BB14" s="79">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>260</v>
       </c>
       <c r="BC14" s="15" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v xml:space="preserve">
 		else_if = {
 			limit = { buy_influence_has_modifier_1point0_mf = yes }
@@ -4956,8 +5254,39 @@
 	}
 }</v>
       </c>
+      <c r="BE14" s="14" t="str">
+        <f t="shared" si="48"/>
+        <v>buy_influence_renewal_1point0_mf</v>
+      </c>
+      <c r="BF14" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v xml:space="preserve">		else_if = {
+			limit = { buy_influence_has_modifier_1point0_mf = yes }
+			set_country_flag = buy_influence_renewal_1point0_mf
+		}
+</v>
+      </c>
+      <c r="BG14" s="16" t="str">
+        <f t="shared" si="34"/>
+        <v xml:space="preserve">
+		remove_country_flag = buy_influence_renewal_1point0_mf</v>
+      </c>
+      <c r="BH14" s="14" t="str">
+        <f t="shared" si="49"/>
+        <v>buy_influence.101.renewal_1point0_mf</v>
+      </c>
+      <c r="BI14" s="15" t="str">
+        <f t="shared" si="35"/>
+        <v xml:space="preserve">				buy_influence_renewal_1point0_mf = { text = buy_influence.101.renewal_1point0_mf }
+</v>
+      </c>
+      <c r="BJ14" s="16" t="str">
+        <f t="shared" si="36"/>
+        <v xml:space="preserve"> buy_influence.101.renewal_1point0_mf:0 "Expired campaign: §Y$buy_influence_1point0_mf_name$§!\n\n$buy_influence.101.renewal$"
+</v>
+      </c>
     </row>
-    <row r="15" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:62" s="2" customFormat="1">
       <c r="B15" s="55" t="s">
         <v>12</v>
       </c>
@@ -4968,7 +5297,7 @@
         <v>1.5</v>
       </c>
       <c r="E15" s="43">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>2</v>
       </c>
       <c r="F15" s="57"/>
@@ -4983,15 +5312,15 @@
         <v>1</v>
       </c>
       <c r="K15" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>buy_influence_1point5_mf</v>
       </c>
       <c r="L15" s="76" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>buy_influence_has_modifier_1point5_mf</v>
       </c>
       <c r="M15" s="36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>buy_influence_1point5_mf_1</v>
       </c>
       <c r="N15" s="37" t="str">
@@ -5014,7 +5343,6 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">
 buy_influence_has_modifier_1point5_mf = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_1point5_mf_1
 		has_modifier = buy_influence_1point5_mf_2
@@ -5028,7 +5356,7 @@
       <c r="S15" s="17" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">
-			buy_influence_has_modifier_1point5_mf = yes</v>
+		buy_influence_has_modifier_1point5_mf = yes</v>
       </c>
       <c r="T15" s="25" t="str">
         <f t="shared" si="3"/>
@@ -5047,6 +5375,8 @@
 	country_base_influence_produces_add = 1.5
 	country_base_minerals_produces_add = -80
 	country_base_food_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="V15" s="15" t="str">
@@ -5057,6 +5387,8 @@
 	country_base_influence_produces_add = 1.5
 	country_base_minerals_produces_add = -160
 	country_base_food_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="W15" s="15" t="str">
@@ -5067,6 +5399,8 @@
 	country_base_influence_produces_add = 1.5
 	country_base_minerals_produces_add = -240
 	country_base_food_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="X15" s="15" t="str">
@@ -5077,6 +5411,8 @@
 	country_base_influence_produces_add = 1.5
 	country_base_minerals_produces_add = -320
 	country_base_food_produces_add = -160
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="Y15" s="18" t="str">
@@ -5087,52 +5423,64 @@
 	country_base_influence_produces_add = 1.5
 	country_base_minerals_produces_add = -400
 	country_base_food_produces_add = -200
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="Z15" s="16" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v xml:space="preserve">
 buy_influence_1point5_mf_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_minerals_produces_add = -80
 	country_base_food_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point5_mf_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_minerals_produces_add = -160
 	country_base_food_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point5_mf_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_minerals_produces_add = -240
 	country_base_food_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point5_mf_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_minerals_produces_add = -320
 	country_base_food_produces_add = -160
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point5_mf_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_minerals_produces_add = -400
 	country_base_food_produces_add = -200
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="AA15" s="25" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>buy_influence_1point5_mf_name</v>
       </c>
       <c r="AB15" s="15" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>buy_influence_1point5_mf_desc</v>
       </c>
       <c r="AC15" s="70" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>buy_influence_1point5_mf_response</v>
       </c>
       <c r="AD15" s="14" t="str">
@@ -5146,7 +5494,6 @@
 			modifier = buy_influence_1point5_mf_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5168,7 +5515,6 @@
 			modifier = buy_influence_1point5_mf_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5190,7 +5536,6 @@
 			modifier = buy_influence_1point5_mf_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5212,7 +5557,6 @@
 			modifier = buy_influence_1point5_mf_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5233,7 +5577,6 @@
 			modifier = buy_influence_1point5_mf_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5244,7 +5587,7 @@
 </v>
       </c>
       <c r="AI15" s="16" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_1point5_mf_name
 		trigger = {
@@ -5254,7 +5597,6 @@
 			modifier = buy_influence_1point5_mf_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5272,7 +5614,6 @@
 			modifier = buy_influence_1point5_mf_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5290,7 +5631,6 @@
 			modifier = buy_influence_1point5_mf_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5308,7 +5648,6 @@
 			modifier = buy_influence_1point5_mf_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5325,7 +5664,6 @@
 			modifier = buy_influence_1point5_mf_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5438,11 +5776,11 @@
  buy_influence_1point5_mf_5_desc:0 "$buy_influence_1point5_mf_desc$"</v>
       </c>
       <c r="BB15" s="79">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>270</v>
       </c>
       <c r="BC15" s="15" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v xml:space="preserve">
 		else_if = {
 			limit = { buy_influence_has_modifier_1point5_mf = yes }
@@ -5466,8 +5804,39 @@
 	}
 }</v>
       </c>
+      <c r="BE15" s="14" t="str">
+        <f t="shared" si="48"/>
+        <v>buy_influence_renewal_1point5_mf</v>
+      </c>
+      <c r="BF15" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v xml:space="preserve">		else_if = {
+			limit = { buy_influence_has_modifier_1point5_mf = yes }
+			set_country_flag = buy_influence_renewal_1point5_mf
+		}
+</v>
+      </c>
+      <c r="BG15" s="16" t="str">
+        <f t="shared" si="34"/>
+        <v xml:space="preserve">
+		remove_country_flag = buy_influence_renewal_1point5_mf</v>
+      </c>
+      <c r="BH15" s="14" t="str">
+        <f t="shared" si="49"/>
+        <v>buy_influence.101.renewal_1point5_mf</v>
+      </c>
+      <c r="BI15" s="15" t="str">
+        <f t="shared" si="35"/>
+        <v xml:space="preserve">				buy_influence_renewal_1point5_mf = { text = buy_influence.101.renewal_1point5_mf }
+</v>
+      </c>
+      <c r="BJ15" s="16" t="str">
+        <f t="shared" si="36"/>
+        <v xml:space="preserve"> buy_influence.101.renewal_1point5_mf:0 "Expired campaign: §Y$buy_influence_1point5_mf_name$§!\n\n$buy_influence.101.renewal$"
+</v>
+      </c>
     </row>
-    <row r="16" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:62" s="2" customFormat="1">
       <c r="B16" s="55" t="s">
         <v>12</v>
       </c>
@@ -5478,7 +5847,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="43">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>2</v>
       </c>
       <c r="F16" s="57"/>
@@ -5493,15 +5862,15 @@
         <v>1</v>
       </c>
       <c r="K16" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>buy_influence_2point0_mf</v>
       </c>
       <c r="L16" s="76" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>buy_influence_has_modifier_2point0_mf</v>
       </c>
       <c r="M16" s="36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>buy_influence_2point0_mf_1</v>
       </c>
       <c r="N16" s="37" t="str">
@@ -5524,7 +5893,6 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">
 buy_influence_has_modifier_2point0_mf = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_2point0_mf_1
 		has_modifier = buy_influence_2point0_mf_2
@@ -5538,7 +5906,7 @@
       <c r="S16" s="17" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">
-			buy_influence_has_modifier_2point0_mf = yes</v>
+		buy_influence_has_modifier_2point0_mf = yes</v>
       </c>
       <c r="T16" s="25" t="str">
         <f t="shared" si="3"/>
@@ -5557,6 +5925,8 @@
 	country_base_influence_produces_add = 2
 	country_base_minerals_produces_add = -120
 	country_base_food_produces_add = -60
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="V16" s="15" t="str">
@@ -5567,6 +5937,8 @@
 	country_base_influence_produces_add = 2
 	country_base_minerals_produces_add = -240
 	country_base_food_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="W16" s="15" t="str">
@@ -5577,6 +5949,8 @@
 	country_base_influence_produces_add = 2
 	country_base_minerals_produces_add = -360
 	country_base_food_produces_add = -180
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="X16" s="15" t="str">
@@ -5587,6 +5961,8 @@
 	country_base_influence_produces_add = 2
 	country_base_minerals_produces_add = -480
 	country_base_food_produces_add = -240
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="Y16" s="18" t="str">
@@ -5597,52 +5973,64 @@
 	country_base_influence_produces_add = 2
 	country_base_minerals_produces_add = -600
 	country_base_food_produces_add = -300
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="Z16" s="16" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v xml:space="preserve">
 buy_influence_2point0_mf_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_minerals_produces_add = -120
 	country_base_food_produces_add = -60
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_mf_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_minerals_produces_add = -240
 	country_base_food_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_mf_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_minerals_produces_add = -360
 	country_base_food_produces_add = -180
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_mf_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_minerals_produces_add = -480
 	country_base_food_produces_add = -240
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_mf_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_minerals_produces_add = -600
 	country_base_food_produces_add = -300
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="AA16" s="25" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>buy_influence_2point0_mf_name</v>
       </c>
       <c r="AB16" s="15" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>buy_influence_2point0_mf_desc</v>
       </c>
       <c r="AC16" s="70" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>buy_influence_2point0_mf_response</v>
       </c>
       <c r="AD16" s="14" t="str">
@@ -5656,7 +6044,6 @@
 			modifier = buy_influence_2point0_mf_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5678,7 +6065,6 @@
 			modifier = buy_influence_2point0_mf_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5700,7 +6086,6 @@
 			modifier = buy_influence_2point0_mf_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5722,7 +6107,6 @@
 			modifier = buy_influence_2point0_mf_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5743,7 +6127,6 @@
 			modifier = buy_influence_2point0_mf_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5754,7 +6137,7 @@
 </v>
       </c>
       <c r="AI16" s="16" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_mf_name
 		trigger = {
@@ -5764,7 +6147,6 @@
 			modifier = buy_influence_2point0_mf_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5782,7 +6164,6 @@
 			modifier = buy_influence_2point0_mf_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5800,7 +6181,6 @@
 			modifier = buy_influence_2point0_mf_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5818,7 +6198,6 @@
 			modifier = buy_influence_2point0_mf_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5835,7 +6214,6 @@
 			modifier = buy_influence_2point0_mf_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -5948,11 +6326,11 @@
  buy_influence_2point0_mf_5_desc:0 "$buy_influence_2point0_mf_desc$"</v>
       </c>
       <c r="BB16" s="79">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>280</v>
       </c>
       <c r="BC16" s="15" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v xml:space="preserve">
 		else_if = {
 			limit = { buy_influence_has_modifier_2point0_mf = yes }
@@ -5976,8 +6354,39 @@
 	}
 }</v>
       </c>
+      <c r="BE16" s="14" t="str">
+        <f t="shared" si="48"/>
+        <v>buy_influence_renewal_2point0_mf</v>
+      </c>
+      <c r="BF16" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v xml:space="preserve">		else_if = {
+			limit = { buy_influence_has_modifier_2point0_mf = yes }
+			set_country_flag = buy_influence_renewal_2point0_mf
+		}
+</v>
+      </c>
+      <c r="BG16" s="16" t="str">
+        <f t="shared" si="34"/>
+        <v xml:space="preserve">
+		remove_country_flag = buy_influence_renewal_2point0_mf</v>
+      </c>
+      <c r="BH16" s="14" t="str">
+        <f t="shared" si="49"/>
+        <v>buy_influence.101.renewal_2point0_mf</v>
+      </c>
+      <c r="BI16" s="15" t="str">
+        <f t="shared" si="35"/>
+        <v xml:space="preserve">				buy_influence_renewal_2point0_mf = { text = buy_influence.101.renewal_2point0_mf }
+</v>
+      </c>
+      <c r="BJ16" s="16" t="str">
+        <f t="shared" si="36"/>
+        <v xml:space="preserve"> buy_influence.101.renewal_2point0_mf:0 "Expired campaign: §Y$buy_influence_2point0_mf_name$§!\n\n$buy_influence.101.renewal$"
+</v>
+      </c>
     </row>
-    <row r="17" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:62" s="2" customFormat="1">
       <c r="B17" s="55" t="s">
         <v>14</v>
       </c>
@@ -5988,7 +6397,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="43">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>2</v>
       </c>
       <c r="F17" s="57">
@@ -6005,15 +6414,15 @@
         <v>1</v>
       </c>
       <c r="K17" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>buy_influence_2point0_emc</v>
       </c>
       <c r="L17" s="76" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>buy_influence_has_modifier_2point0_emc</v>
       </c>
       <c r="M17" s="36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>buy_influence_2point0_emc_1</v>
       </c>
       <c r="N17" s="37" t="str">
@@ -6036,7 +6445,6 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">
 buy_influence_has_modifier_2point0_emc = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_2point0_emc_1
 		has_modifier = buy_influence_2point0_emc_2
@@ -6050,7 +6458,7 @@
       <c r="S17" s="17" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">
-			buy_influence_has_modifier_2point0_emc = yes</v>
+		buy_influence_has_modifier_2point0_emc = yes</v>
       </c>
       <c r="T17" s="25" t="str">
         <f t="shared" si="3"/>
@@ -6070,6 +6478,8 @@
 	country_base_energy_produces_add = -40
 	country_base_minerals_produces_add = -80
 	country_base_consumer_goods_produces_add = -20
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="V17" s="15" t="str">
@@ -6081,6 +6491,8 @@
 	country_base_energy_produces_add = -80
 	country_base_minerals_produces_add = -160
 	country_base_consumer_goods_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="W17" s="15" t="str">
@@ -6092,6 +6504,8 @@
 	country_base_energy_produces_add = -120
 	country_base_minerals_produces_add = -240
 	country_base_consumer_goods_produces_add = -60
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="X17" s="15" t="str">
@@ -6103,6 +6517,8 @@
 	country_base_energy_produces_add = -160
 	country_base_minerals_produces_add = -320
 	country_base_consumer_goods_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="Y17" s="18" t="str">
@@ -6114,10 +6530,12 @@
 	country_base_energy_produces_add = -200
 	country_base_minerals_produces_add = -400
 	country_base_consumer_goods_produces_add = -100
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="Z17" s="16" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v xml:space="preserve">
 buy_influence_2point0_emc_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6125,6 +6543,8 @@
 	country_base_energy_produces_add = -40
 	country_base_minerals_produces_add = -80
 	country_base_consumer_goods_produces_add = -20
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_emc_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6132,6 +6552,8 @@
 	country_base_energy_produces_add = -80
 	country_base_minerals_produces_add = -160
 	country_base_consumer_goods_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_emc_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6139,6 +6561,8 @@
 	country_base_energy_produces_add = -120
 	country_base_minerals_produces_add = -240
 	country_base_consumer_goods_produces_add = -60
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_emc_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6146,6 +6570,8 @@
 	country_base_energy_produces_add = -160
 	country_base_minerals_produces_add = -320
 	country_base_consumer_goods_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_emc_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6153,18 +6579,20 @@
 	country_base_energy_produces_add = -200
 	country_base_minerals_produces_add = -400
 	country_base_consumer_goods_produces_add = -100
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }</v>
       </c>
       <c r="AA17" s="25" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>buy_influence_2point0_emc_name</v>
       </c>
       <c r="AB17" s="15" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>buy_influence_2point0_emc_desc</v>
       </c>
       <c r="AC17" s="70" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>buy_influence_2point0_emc_response</v>
       </c>
       <c r="AD17" s="14" t="str">
@@ -6178,7 +6606,6 @@
 			modifier = buy_influence_2point0_emc_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6200,7 +6627,6 @@
 			modifier = buy_influence_2point0_emc_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6222,7 +6648,6 @@
 			modifier = buy_influence_2point0_emc_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6244,7 +6669,6 @@
 			modifier = buy_influence_2point0_emc_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6265,7 +6689,6 @@
 			modifier = buy_influence_2point0_emc_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6276,7 +6699,7 @@
 </v>
       </c>
       <c r="AI17" s="16" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_2point0_emc_name
 		trigger = {
@@ -6286,7 +6709,6 @@
 			modifier = buy_influence_2point0_emc_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6304,7 +6726,6 @@
 			modifier = buy_influence_2point0_emc_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6322,7 +6743,6 @@
 			modifier = buy_influence_2point0_emc_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6340,7 +6760,6 @@
 			modifier = buy_influence_2point0_emc_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6357,7 +6776,6 @@
 			modifier = buy_influence_2point0_emc_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6470,11 +6888,11 @@
  buy_influence_2point0_emc_5_desc:0 "$buy_influence_2point0_emc_desc$"</v>
       </c>
       <c r="BB17" s="79">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>290</v>
       </c>
       <c r="BC17" s="15" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v xml:space="preserve">
 		else_if = {
 			limit = { buy_influence_has_modifier_2point0_emc = yes }
@@ -6498,8 +6916,39 @@
 	}
 }</v>
       </c>
+      <c r="BE17" s="14" t="str">
+        <f t="shared" si="48"/>
+        <v>buy_influence_renewal_2point0_emc</v>
+      </c>
+      <c r="BF17" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v xml:space="preserve">		else_if = {
+			limit = { buy_influence_has_modifier_2point0_emc = yes }
+			set_country_flag = buy_influence_renewal_2point0_emc
+		}
+</v>
+      </c>
+      <c r="BG17" s="16" t="str">
+        <f t="shared" si="34"/>
+        <v xml:space="preserve">
+		remove_country_flag = buy_influence_renewal_2point0_emc</v>
+      </c>
+      <c r="BH17" s="14" t="str">
+        <f t="shared" si="49"/>
+        <v>buy_influence.101.renewal_2point0_emc</v>
+      </c>
+      <c r="BI17" s="15" t="str">
+        <f t="shared" si="35"/>
+        <v xml:space="preserve">				buy_influence_renewal_2point0_emc = { text = buy_influence.101.renewal_2point0_emc }
+</v>
+      </c>
+      <c r="BJ17" s="16" t="str">
+        <f t="shared" si="36"/>
+        <v xml:space="preserve"> buy_influence.101.renewal_2point0_emc:0 "Expired campaign: §Y$buy_influence_2point0_emc_name$§!\n\n$buy_influence.101.renewal$"
+</v>
+      </c>
     </row>
-    <row r="18" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:62" s="2" customFormat="1">
       <c r="B18" s="55" t="s">
         <v>14</v>
       </c>
@@ -6510,7 +6959,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="43">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>3</v>
       </c>
       <c r="F18" s="57">
@@ -6527,15 +6976,15 @@
         <v>1</v>
       </c>
       <c r="K18" s="14" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>buy_influence_3point0_emc</v>
       </c>
       <c r="L18" s="76" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>buy_influence_has_modifier_3point0_emc</v>
       </c>
       <c r="M18" s="36" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>buy_influence_3point0_emc_1</v>
       </c>
       <c r="N18" s="37" t="str">
@@ -6558,7 +7007,6 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">
 buy_influence_has_modifier_3point0_emc = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_3point0_emc_1
 		has_modifier = buy_influence_3point0_emc_2
@@ -6572,7 +7020,7 @@
       <c r="S18" s="17" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">
-			buy_influence_has_modifier_3point0_emc = yes</v>
+		buy_influence_has_modifier_3point0_emc = yes</v>
       </c>
       <c r="T18" s="25" t="str">
         <f t="shared" si="3"/>
@@ -6592,6 +7040,8 @@
 	country_base_energy_produces_add = -80
 	country_base_minerals_produces_add = -160
 	country_base_consumer_goods_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_3
 }</v>
       </c>
       <c r="V18" s="15" t="str">
@@ -6603,6 +7053,8 @@
 	country_base_energy_produces_add = -160
 	country_base_minerals_produces_add = -320
 	country_base_consumer_goods_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_3
 }</v>
       </c>
       <c r="W18" s="15" t="str">
@@ -6614,6 +7066,8 @@
 	country_base_energy_produces_add = -240
 	country_base_minerals_produces_add = -480
 	country_base_consumer_goods_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_3
 }</v>
       </c>
       <c r="X18" s="15" t="str">
@@ -6625,6 +7079,8 @@
 	country_base_energy_produces_add = -320
 	country_base_minerals_produces_add = -640
 	country_base_consumer_goods_produces_add = -160
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_3
 }</v>
       </c>
       <c r="Y18" s="18" t="str">
@@ -6636,10 +7092,12 @@
 	country_base_energy_produces_add = -400
 	country_base_minerals_produces_add = -800
 	country_base_consumer_goods_produces_add = -200
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_3
 }</v>
       </c>
       <c r="Z18" s="16" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v xml:space="preserve">
 buy_influence_3point0_emc_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6647,6 +7105,8 @@
 	country_base_energy_produces_add = -80
 	country_base_minerals_produces_add = -160
 	country_base_consumer_goods_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_3
 }
 buy_influence_3point0_emc_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6654,6 +7114,8 @@
 	country_base_energy_produces_add = -160
 	country_base_minerals_produces_add = -320
 	country_base_consumer_goods_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_3
 }
 buy_influence_3point0_emc_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6661,6 +7123,8 @@
 	country_base_energy_produces_add = -240
 	country_base_minerals_produces_add = -480
 	country_base_consumer_goods_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_3
 }
 buy_influence_3point0_emc_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6668,6 +7132,8 @@
 	country_base_energy_produces_add = -320
 	country_base_minerals_produces_add = -640
 	country_base_consumer_goods_produces_add = -160
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_3
 }
 buy_influence_3point0_emc_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -6675,18 +7141,20 @@
 	country_base_energy_produces_add = -400
 	country_base_minerals_produces_add = -800
 	country_base_consumer_goods_produces_add = -200
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_3
 }</v>
       </c>
       <c r="AA18" s="25" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>buy_influence_3point0_emc_name</v>
       </c>
       <c r="AB18" s="15" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>buy_influence_3point0_emc_desc</v>
       </c>
       <c r="AC18" s="70" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>buy_influence_3point0_emc_response</v>
       </c>
       <c r="AD18" s="14" t="str">
@@ -6700,7 +7168,6 @@
 			modifier = buy_influence_3point0_emc_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_3
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6722,7 +7189,6 @@
 			modifier = buy_influence_3point0_emc_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_3
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6744,7 +7210,6 @@
 			modifier = buy_influence_3point0_emc_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_3
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6766,7 +7231,6 @@
 			modifier = buy_influence_3point0_emc_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_3
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6787,7 +7251,6 @@
 			modifier = buy_influence_3point0_emc_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_3
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6798,7 +7261,7 @@
 </v>
       </c>
       <c r="AI18" s="16" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_3point0_emc_name
 		trigger = {
@@ -6808,7 +7271,6 @@
 			modifier = buy_influence_3point0_emc_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_3
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6826,7 +7288,6 @@
 			modifier = buy_influence_3point0_emc_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_3
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6844,7 +7305,6 @@
 			modifier = buy_influence_3point0_emc_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_3
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6862,7 +7322,6 @@
 			modifier = buy_influence_3point0_emc_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_3
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6879,7 +7338,6 @@
 			modifier = buy_influence_3point0_emc_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_3
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -6992,11 +7450,11 @@
  buy_influence_3point0_emc_5_desc:0 "$buy_influence_3point0_emc_desc$"</v>
       </c>
       <c r="BB18" s="79">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>300</v>
       </c>
       <c r="BC18" s="15" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v xml:space="preserve">
 		else_if = {
 			limit = { buy_influence_has_modifier_3point0_emc = yes }
@@ -7020,8 +7478,39 @@
 	}
 }</v>
       </c>
+      <c r="BE18" s="14" t="str">
+        <f t="shared" si="48"/>
+        <v>buy_influence_renewal_3point0_emc</v>
+      </c>
+      <c r="BF18" s="15" t="str">
+        <f t="shared" si="33"/>
+        <v xml:space="preserve">		else_if = {
+			limit = { buy_influence_has_modifier_3point0_emc = yes }
+			set_country_flag = buy_influence_renewal_3point0_emc
+		}
+</v>
+      </c>
+      <c r="BG18" s="16" t="str">
+        <f t="shared" si="34"/>
+        <v xml:space="preserve">
+		remove_country_flag = buy_influence_renewal_3point0_emc</v>
+      </c>
+      <c r="BH18" s="14" t="str">
+        <f t="shared" si="49"/>
+        <v>buy_influence.101.renewal_3point0_emc</v>
+      </c>
+      <c r="BI18" s="15" t="str">
+        <f t="shared" si="35"/>
+        <v xml:space="preserve">				buy_influence_renewal_3point0_emc = { text = buy_influence.101.renewal_3point0_emc }
+</v>
+      </c>
+      <c r="BJ18" s="16" t="str">
+        <f t="shared" si="36"/>
+        <v xml:space="preserve"> buy_influence.101.renewal_3point0_emc:0 "Expired campaign: §Y$buy_influence_3point0_emc_name$§!\n\n$buy_influence.101.renewal$"
+</v>
+      </c>
     </row>
-    <row r="19" spans="2:56" s="2" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:62" s="2" customFormat="1" ht="14.65" thickBot="1">
       <c r="B19" s="59" t="s">
         <v>14</v>
       </c>
@@ -7032,7 +7521,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="44">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="F19" s="61">
@@ -7049,15 +7538,15 @@
         <v>1</v>
       </c>
       <c r="K19" s="19" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>buy_influence_4point0_emc</v>
       </c>
       <c r="L19" s="77" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>buy_influence_has_modifier_4point0_emc</v>
       </c>
       <c r="M19" s="39" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>buy_influence_4point0_emc_1</v>
       </c>
       <c r="N19" s="40" t="str">
@@ -7080,7 +7569,6 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve">
 buy_influence_has_modifier_4point0_emc = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_4point0_emc_1
 		has_modifier = buy_influence_4point0_emc_2
@@ -7094,7 +7582,7 @@
       <c r="S19" s="22" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">
-			buy_influence_has_modifier_4point0_emc = yes</v>
+		buy_influence_has_modifier_4point0_emc = yes</v>
       </c>
       <c r="T19" s="26" t="str">
         <f t="shared" si="3"/>
@@ -7114,6 +7602,8 @@
 	country_base_energy_produces_add = -120
 	country_base_minerals_produces_add = -240
 	country_base_consumer_goods_produces_add = -60
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_4
 }</v>
       </c>
       <c r="V19" s="20" t="str">
@@ -7125,6 +7615,8 @@
 	country_base_energy_produces_add = -240
 	country_base_minerals_produces_add = -480
 	country_base_consumer_goods_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_4
 }</v>
       </c>
       <c r="W19" s="20" t="str">
@@ -7136,6 +7628,8 @@
 	country_base_energy_produces_add = -360
 	country_base_minerals_produces_add = -720
 	country_base_consumer_goods_produces_add = -180
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_4
 }</v>
       </c>
       <c r="X19" s="20" t="str">
@@ -7147,6 +7641,8 @@
 	country_base_energy_produces_add = -480
 	country_base_minerals_produces_add = -960
 	country_base_consumer_goods_produces_add = -240
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_4
 }</v>
       </c>
       <c r="Y19" s="23" t="str">
@@ -7158,10 +7654,12 @@
 	country_base_energy_produces_add = -600
 	country_base_minerals_produces_add = -1200
 	country_base_consumer_goods_produces_add = -300
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_4
 }</v>
       </c>
       <c r="Z19" s="21" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v xml:space="preserve">
 buy_influence_4point0_emc_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -7169,6 +7667,8 @@
 	country_base_energy_produces_add = -120
 	country_base_minerals_produces_add = -240
 	country_base_consumer_goods_produces_add = -60
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_4
 }
 buy_influence_4point0_emc_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -7176,6 +7676,8 @@
 	country_base_energy_produces_add = -240
 	country_base_minerals_produces_add = -480
 	country_base_consumer_goods_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_4
 }
 buy_influence_4point0_emc_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -7183,6 +7685,8 @@
 	country_base_energy_produces_add = -360
 	country_base_minerals_produces_add = -720
 	country_base_consumer_goods_produces_add = -180
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_4
 }
 buy_influence_4point0_emc_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -7190,6 +7694,8 @@
 	country_base_energy_produces_add = -480
 	country_base_minerals_produces_add = -960
 	country_base_consumer_goods_produces_add = -240
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_4
 }
 buy_influence_4point0_emc_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -7197,18 +7703,20 @@
 	country_base_energy_produces_add = -600
 	country_base_minerals_produces_add = -1200
 	country_base_consumer_goods_produces_add = -300
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_4
 }</v>
       </c>
       <c r="AA19" s="26" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v>buy_influence_4point0_emc_name</v>
       </c>
       <c r="AB19" s="20" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>buy_influence_4point0_emc_desc</v>
       </c>
       <c r="AC19" s="71" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>buy_influence_4point0_emc_response</v>
       </c>
       <c r="AD19" s="19" t="str">
@@ -7222,7 +7730,6 @@
 			modifier = buy_influence_4point0_emc_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_4
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -7244,7 +7751,6 @@
 			modifier = buy_influence_4point0_emc_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_4
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -7266,7 +7772,6 @@
 			modifier = buy_influence_4point0_emc_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_4
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -7288,7 +7793,6 @@
 			modifier = buy_influence_4point0_emc_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_4
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -7309,7 +7813,6 @@
 			modifier = buy_influence_4point0_emc_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_4
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -7320,7 +7823,7 @@
 </v>
       </c>
       <c r="AI19" s="21" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v xml:space="preserve">	option = {
 		name = buy_influence_4point0_emc_name
 		trigger = {
@@ -7330,7 +7833,6 @@
 			modifier = buy_influence_4point0_emc_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_4
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -7348,7 +7850,6 @@
 			modifier = buy_influence_4point0_emc_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_4
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -7366,7 +7867,6 @@
 			modifier = buy_influence_4point0_emc_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_4
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -7384,7 +7884,6 @@
 			modifier = buy_influence_4point0_emc_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_4
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -7401,7 +7900,6 @@
 			modifier = buy_influence_4point0_emc_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_4
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -7514,11 +8012,11 @@
  buy_influence_4point0_emc_5_desc:0 "$buy_influence_4point0_emc_desc$"</v>
       </c>
       <c r="BB19" s="80">
-        <f t="shared" si="42"/>
+        <f t="shared" si="46"/>
         <v>310</v>
       </c>
       <c r="BC19" s="20" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="47"/>
         <v xml:space="preserve">
 		else_if = {
 			limit = { buy_influence_has_modifier_4point0_emc = yes }
@@ -7542,8 +8040,39 @@
 	}
 }</v>
       </c>
+      <c r="BE19" s="19" t="str">
+        <f t="shared" si="48"/>
+        <v>buy_influence_renewal_4point0_emc</v>
+      </c>
+      <c r="BF19" s="20" t="str">
+        <f t="shared" si="33"/>
+        <v xml:space="preserve">		else_if = {
+			limit = { buy_influence_has_modifier_4point0_emc = yes }
+			set_country_flag = buy_influence_renewal_4point0_emc
+		}
+</v>
+      </c>
+      <c r="BG19" s="21" t="str">
+        <f t="shared" si="34"/>
+        <v xml:space="preserve">
+		remove_country_flag = buy_influence_renewal_4point0_emc</v>
+      </c>
+      <c r="BH19" s="19" t="str">
+        <f t="shared" si="49"/>
+        <v>buy_influence.101.renewal_4point0_emc</v>
+      </c>
+      <c r="BI19" s="20" t="str">
+        <f t="shared" si="35"/>
+        <v xml:space="preserve">				buy_influence_renewal_4point0_emc = { text = buy_influence.101.renewal_4point0_emc }
+</v>
+      </c>
+      <c r="BJ19" s="21" t="str">
+        <f t="shared" si="36"/>
+        <v xml:space="preserve"> buy_influence.101.renewal_4point0_emc:0 "Expired campaign: §Y$buy_influence_4point0_emc_name$§!\n\n$buy_influence.101.renewal$"
+</v>
+      </c>
     </row>
-    <row r="20" spans="2:56" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:62" ht="14.65" thickBot="1">
       <c r="R20" s="11" t="str">
         <f>"#################################################################"&amp;newline&amp;
 "#Begin generated code: Does the current (country) scope have one particular type of modifier added by this mod?"&amp;newline&amp;
@@ -7556,7 +8085,6 @@
 #Begin generated code: Does the current (country) scope have one particular type of modifier added by this mod?
 #################################################################
 buy_influence_has_modifier_0point5_e = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_0point5_e_1
 		has_modifier = buy_influence_0point5_e_2
@@ -7566,7 +8094,6 @@
 	}
 }
 buy_influence_has_modifier_1point0_e = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_1point0_e_1
 		has_modifier = buy_influence_1point0_e_2
@@ -7576,7 +8103,6 @@
 	}
 }
 buy_influence_has_modifier_1point0_em = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_1point0_em_1
 		has_modifier = buy_influence_1point0_em_2
@@ -7586,7 +8112,6 @@
 	}
 }
 buy_influence_has_modifier_1point5_em = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_1point5_em_1
 		has_modifier = buy_influence_1point5_em_2
@@ -7596,7 +8121,6 @@
 	}
 }
 buy_influence_has_modifier_2point0_em = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_2point0_em_1
 		has_modifier = buy_influence_2point0_em_2
@@ -7606,7 +8130,6 @@
 	}
 }
 buy_influence_has_modifier_1point0_mf = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_1point0_mf_1
 		has_modifier = buy_influence_1point0_mf_2
@@ -7616,7 +8139,6 @@
 	}
 }
 buy_influence_has_modifier_1point5_mf = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_1point5_mf_1
 		has_modifier = buy_influence_1point5_mf_2
@@ -7626,7 +8148,6 @@
 	}
 }
 buy_influence_has_modifier_2point0_mf = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_2point0_mf_1
 		has_modifier = buy_influence_2point0_mf_2
@@ -7636,7 +8157,6 @@
 	}
 }
 buy_influence_has_modifier_2point0_emc = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_2point0_emc_1
 		has_modifier = buy_influence_2point0_emc_2
@@ -7646,7 +8166,6 @@
 	}
 }
 buy_influence_has_modifier_3point0_emc = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_3point0_emc_1
 		has_modifier = buy_influence_3point0_emc_2
@@ -7656,7 +8175,6 @@
 	}
 }
 buy_influence_has_modifier_4point0_emc = {
-	exists = from
 	OR = {
 		has_modifier = buy_influence_4point0_emc_1
 		has_modifier = buy_influence_4point0_emc_2
@@ -7678,17 +8196,17 @@
 newline &amp; tab &amp; tab &amp; "}"</f>
         <v xml:space="preserve">		#Generated code: Does the current (country) scope have any of the modifiers added by this mod?
 		OR = {
-			buy_influence_has_modifier_0point5_e = yes
-			buy_influence_has_modifier_1point0_e = yes
-			buy_influence_has_modifier_1point0_em = yes
-			buy_influence_has_modifier_1point5_em = yes
-			buy_influence_has_modifier_2point0_em = yes
-			buy_influence_has_modifier_1point0_mf = yes
-			buy_influence_has_modifier_1point5_mf = yes
-			buy_influence_has_modifier_2point0_mf = yes
-			buy_influence_has_modifier_2point0_emc = yes
-			buy_influence_has_modifier_3point0_emc = yes
-			buy_influence_has_modifier_4point0_emc = yes
+		buy_influence_has_modifier_0point5_e = yes
+		buy_influence_has_modifier_1point0_e = yes
+		buy_influence_has_modifier_1point0_em = yes
+		buy_influence_has_modifier_1point5_em = yes
+		buy_influence_has_modifier_2point0_em = yes
+		buy_influence_has_modifier_1point0_mf = yes
+		buy_influence_has_modifier_1point5_mf = yes
+		buy_influence_has_modifier_2point0_mf = yes
+		buy_influence_has_modifier_2point0_emc = yes
+		buy_influence_has_modifier_3point0_emc = yes
+		buy_influence_has_modifier_4point0_emc = yes
 		}</v>
       </c>
       <c r="T20" s="11" t="str">
@@ -7757,231 +8275,311 @@
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 0.5
 	country_base_energy_produces_add = -10
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_0point5_e_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 0.5
 	country_base_energy_produces_add = -20
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_0point5_e_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 0.5
 	country_base_energy_produces_add = -30
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_0point5_e_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 0.5
 	country_base_energy_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_0point5_e_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 0.5
 	country_base_energy_produces_add = -50
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_e_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -30
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_e_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -60
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_e_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -90
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_e_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_e_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -150
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_em_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -20
 	country_base_minerals_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_em_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -40
 	country_base_minerals_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_em_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -60
 	country_base_minerals_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_em_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -80
 	country_base_minerals_produces_add = -160
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_em_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_energy_produces_add = -100
 	country_base_minerals_produces_add = -200
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point5_em_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_energy_produces_add = -40
 	country_base_minerals_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point5_em_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_energy_produces_add = -80
 	country_base_minerals_produces_add = -160
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point5_em_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_energy_produces_add = -120
 	country_base_minerals_produces_add = -240
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point5_em_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_energy_produces_add = -160
 	country_base_minerals_produces_add = -320
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point5_em_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_energy_produces_add = -200
 	country_base_minerals_produces_add = -400
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_em_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_energy_produces_add = -60
 	country_base_minerals_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_em_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_energy_produces_add = -120
 	country_base_minerals_produces_add = -240
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_em_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_energy_produces_add = -180
 	country_base_minerals_produces_add = -360
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_em_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_energy_produces_add = -240
 	country_base_minerals_produces_add = -480
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_em_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_energy_produces_add = -300
 	country_base_minerals_produces_add = -600
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point0_mf_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_minerals_produces_add = -40
 	country_base_food_produces_add = -20
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_mf_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_minerals_produces_add = -80
 	country_base_food_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_mf_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_minerals_produces_add = -120
 	country_base_food_produces_add = -60
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_mf_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_minerals_produces_add = -160
 	country_base_food_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point0_mf_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1
 	country_base_minerals_produces_add = -200
 	country_base_food_produces_add = -100
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_1
 }
 buy_influence_1point5_mf_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_minerals_produces_add = -80
 	country_base_food_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point5_mf_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_minerals_produces_add = -160
 	country_base_food_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point5_mf_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_minerals_produces_add = -240
 	country_base_food_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point5_mf_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_minerals_produces_add = -320
 	country_base_food_produces_add = -160
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_1point5_mf_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 1.5
 	country_base_minerals_produces_add = -400
 	country_base_food_produces_add = -200
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_mf_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_minerals_produces_add = -120
 	country_base_food_produces_add = -60
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_mf_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_minerals_produces_add = -240
 	country_base_food_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_mf_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_minerals_produces_add = -360
 	country_base_food_produces_add = -180
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_mf_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_minerals_produces_add = -480
 	country_base_food_produces_add = -240
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_mf_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
 	country_base_influence_produces_add = 2
 	country_base_minerals_produces_add = -600
 	country_base_food_produces_add = -300
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_emc_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -7989,6 +8587,8 @@
 	country_base_energy_produces_add = -40
 	country_base_minerals_produces_add = -80
 	country_base_consumer_goods_produces_add = -20
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_emc_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -7996,6 +8596,8 @@
 	country_base_energy_produces_add = -80
 	country_base_minerals_produces_add = -160
 	country_base_consumer_goods_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_emc_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -8003,6 +8605,8 @@
 	country_base_energy_produces_add = -120
 	country_base_minerals_produces_add = -240
 	country_base_consumer_goods_produces_add = -60
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_emc_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -8010,6 +8614,8 @@
 	country_base_energy_produces_add = -160
 	country_base_minerals_produces_add = -320
 	country_base_consumer_goods_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_2point0_emc_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -8017,6 +8623,8 @@
 	country_base_energy_produces_add = -200
 	country_base_minerals_produces_add = -400
 	country_base_consumer_goods_produces_add = -100
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_2
 }
 buy_influence_3point0_emc_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -8024,6 +8632,8 @@
 	country_base_energy_produces_add = -80
 	country_base_minerals_produces_add = -160
 	country_base_consumer_goods_produces_add = -40
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_3
 }
 buy_influence_3point0_emc_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -8031,6 +8641,8 @@
 	country_base_energy_produces_add = -160
 	country_base_minerals_produces_add = -320
 	country_base_consumer_goods_produces_add = -80
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_3
 }
 buy_influence_3point0_emc_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -8038,6 +8650,8 @@
 	country_base_energy_produces_add = -240
 	country_base_minerals_produces_add = -480
 	country_base_consumer_goods_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_3
 }
 buy_influence_3point0_emc_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -8045,6 +8659,8 @@
 	country_base_energy_produces_add = -320
 	country_base_minerals_produces_add = -640
 	country_base_consumer_goods_produces_add = -160
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_3
 }
 buy_influence_3point0_emc_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -8052,6 +8668,8 @@
 	country_base_energy_produces_add = -400
 	country_base_minerals_produces_add = -800
 	country_base_consumer_goods_produces_add = -200
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_3
 }
 buy_influence_4point0_emc_1 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -8059,6 +8677,8 @@
 	country_base_energy_produces_add = -120
 	country_base_minerals_produces_add = -240
 	country_base_consumer_goods_produces_add = -60
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_4
 }
 buy_influence_4point0_emc_2 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -8066,6 +8686,8 @@
 	country_base_energy_produces_add = -240
 	country_base_minerals_produces_add = -480
 	country_base_consumer_goods_produces_add = -120
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_4
 }
 buy_influence_4point0_emc_3 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -8073,6 +8695,8 @@
 	country_base_energy_produces_add = -360
 	country_base_minerals_produces_add = -720
 	country_base_consumer_goods_produces_add = -180
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_4
 }
 buy_influence_4point0_emc_4 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -8080,6 +8704,8 @@
 	country_base_energy_produces_add = -480
 	country_base_minerals_produces_add = -960
 	country_base_consumer_goods_produces_add = -240
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_4
 }
 buy_influence_4point0_emc_5 = {
 	icon = "gfx/interface/icons/modifiers/mod_country_previous_deals.dds"
@@ -8087,6 +8713,8 @@
 	country_base_energy_produces_add = -600
 	country_base_minerals_produces_add = -1200
 	country_base_consumer_goods_produces_add = -300
+	show_only_custom_tooltip = no
+	custom_tooltip = buy_influence_opinion_gain_4
 }</v>
       </c>
       <c r="AD20" s="73"/>
@@ -8114,7 +8742,6 @@
 			modifier = buy_influence_0point5_e_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8132,7 +8759,6 @@
 			modifier = buy_influence_0point5_e_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8150,7 +8776,6 @@
 			modifier = buy_influence_0point5_e_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8168,7 +8793,6 @@
 			modifier = buy_influence_0point5_e_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8185,7 +8809,6 @@
 			modifier = buy_influence_0point5_e_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8202,7 +8825,6 @@
 			modifier = buy_influence_1point0_e_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8220,7 +8842,6 @@
 			modifier = buy_influence_1point0_e_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8238,7 +8859,6 @@
 			modifier = buy_influence_1point0_e_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8256,7 +8876,6 @@
 			modifier = buy_influence_1point0_e_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8273,7 +8892,6 @@
 			modifier = buy_influence_1point0_e_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8290,7 +8908,6 @@
 			modifier = buy_influence_1point0_em_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8308,7 +8925,6 @@
 			modifier = buy_influence_1point0_em_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8326,7 +8942,6 @@
 			modifier = buy_influence_1point0_em_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8344,7 +8959,6 @@
 			modifier = buy_influence_1point0_em_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8361,7 +8975,6 @@
 			modifier = buy_influence_1point0_em_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8378,7 +8991,6 @@
 			modifier = buy_influence_1point5_em_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8396,7 +9008,6 @@
 			modifier = buy_influence_1point5_em_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8414,7 +9025,6 @@
 			modifier = buy_influence_1point5_em_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8432,7 +9042,6 @@
 			modifier = buy_influence_1point5_em_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8449,7 +9058,6 @@
 			modifier = buy_influence_1point5_em_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8466,7 +9074,6 @@
 			modifier = buy_influence_2point0_em_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8484,7 +9091,6 @@
 			modifier = buy_influence_2point0_em_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8502,7 +9108,6 @@
 			modifier = buy_influence_2point0_em_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8520,7 +9125,6 @@
 			modifier = buy_influence_2point0_em_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8537,7 +9141,6 @@
 			modifier = buy_influence_2point0_em_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8554,7 +9157,6 @@
 			modifier = buy_influence_1point0_mf_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8572,7 +9174,6 @@
 			modifier = buy_influence_1point0_mf_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8590,7 +9191,6 @@
 			modifier = buy_influence_1point0_mf_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8608,7 +9208,6 @@
 			modifier = buy_influence_1point0_mf_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8625,7 +9224,6 @@
 			modifier = buy_influence_1point0_mf_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_1
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8642,7 +9240,6 @@
 			modifier = buy_influence_1point5_mf_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8660,7 +9257,6 @@
 			modifier = buy_influence_1point5_mf_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8678,7 +9274,6 @@
 			modifier = buy_influence_1point5_mf_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8696,7 +9291,6 @@
 			modifier = buy_influence_1point5_mf_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8713,7 +9307,6 @@
 			modifier = buy_influence_1point5_mf_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8730,7 +9323,6 @@
 			modifier = buy_influence_2point0_mf_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8748,7 +9340,6 @@
 			modifier = buy_influence_2point0_mf_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8766,7 +9357,6 @@
 			modifier = buy_influence_2point0_mf_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8784,7 +9374,6 @@
 			modifier = buy_influence_2point0_mf_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8801,7 +9390,6 @@
 			modifier = buy_influence_2point0_mf_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8818,7 +9406,6 @@
 			modifier = buy_influence_2point0_emc_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8836,7 +9423,6 @@
 			modifier = buy_influence_2point0_emc_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8854,7 +9440,6 @@
 			modifier = buy_influence_2point0_emc_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8872,7 +9457,6 @@
 			modifier = buy_influence_2point0_emc_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8889,7 +9473,6 @@
 			modifier = buy_influence_2point0_emc_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_2
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8906,7 +9489,6 @@
 			modifier = buy_influence_3point0_emc_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_3
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8924,7 +9506,6 @@
 			modifier = buy_influence_3point0_emc_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_3
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8942,7 +9523,6 @@
 			modifier = buy_influence_3point0_emc_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_3
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8960,7 +9540,6 @@
 			modifier = buy_influence_3point0_emc_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_3
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8977,7 +9556,6 @@
 			modifier = buy_influence_3point0_emc_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_3
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -8994,7 +9572,6 @@
 			modifier = buy_influence_4point0_emc_1
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_4
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -9012,7 +9589,6 @@
 			modifier = buy_influence_4point0_emc_2
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_4
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -9030,7 +9606,6 @@
 			modifier = buy_influence_4point0_emc_3
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_4
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -9048,7 +9623,6 @@
 			modifier = buy_influence_4point0_emc_4
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_4
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -9065,7 +9639,6 @@
 			modifier = buy_influence_4point0_emc_5
 			days = @buy_influence_buff_duration
 		}
-		custom_tooltip = buy_influence_opinion_gain_4
 		hidden_effect = {
 			country_event = {
 				id = buy_influence.110
@@ -9468,9 +10041,113 @@
 #################################################################
 </v>
       </c>
+      <c r="BF20" s="30" t="str">
+        <f>tab &amp; tab &amp; "#Generated code: Set renewal flag depending on currently-active campaign" &amp; newline &amp;
+CONCATENATE(BF9,BF10,BF11,BF12,BF13,BF14,BF15,BF16,BF17,BF18,BF19) &amp; newline &amp;
+tab &amp; tab &amp; "#End of generated code"</f>
+        <v xml:space="preserve">		#Generated code: Set renewal flag depending on currently-active campaign
+		if = {
+			limit = { buy_influence_has_modifier_0point5_e = yes }
+			set_country_flag = buy_influence_renewal_0point5_e
+		}
+		else_if = {
+			limit = { buy_influence_has_modifier_1point0_e = yes }
+			set_country_flag = buy_influence_renewal_1point0_e
+		}
+		else_if = {
+			limit = { buy_influence_has_modifier_1point0_em = yes }
+			set_country_flag = buy_influence_renewal_1point0_em
+		}
+		else_if = {
+			limit = { buy_influence_has_modifier_1point5_em = yes }
+			set_country_flag = buy_influence_renewal_1point5_em
+		}
+		else_if = {
+			limit = { buy_influence_has_modifier_2point0_em = yes }
+			set_country_flag = buy_influence_renewal_2point0_em
+		}
+		else_if = {
+			limit = { buy_influence_has_modifier_1point0_mf = yes }
+			set_country_flag = buy_influence_renewal_1point0_mf
+		}
+		else_if = {
+			limit = { buy_influence_has_modifier_1point5_mf = yes }
+			set_country_flag = buy_influence_renewal_1point5_mf
+		}
+		else_if = {
+			limit = { buy_influence_has_modifier_2point0_mf = yes }
+			set_country_flag = buy_influence_renewal_2point0_mf
+		}
+		else_if = {
+			limit = { buy_influence_has_modifier_2point0_emc = yes }
+			set_country_flag = buy_influence_renewal_2point0_emc
+		}
+		else_if = {
+			limit = { buy_influence_has_modifier_3point0_emc = yes }
+			set_country_flag = buy_influence_renewal_3point0_emc
+		}
+		else_if = {
+			limit = { buy_influence_has_modifier_4point0_emc = yes }
+			set_country_flag = buy_influence_renewal_4point0_emc
+		}
+		#End of generated code</v>
+      </c>
+      <c r="BG20" s="30" t="str">
+        <f>tab &amp; tab &amp; "#Generated code: Remove all renewal flags" &amp; newline &amp;
+CONCATENATE(BG9,BG10,BG11,BG12,BG13,BG14,BG15,BG16,BG17,BG18,BG19) &amp; newline &amp; newline &amp;
+tab &amp; tab &amp; "#End of generated code"</f>
+        <v xml:space="preserve">		#Generated code: Remove all renewal flags
+		remove_country_flag = buy_influence_renewal_0point5_e
+		remove_country_flag = buy_influence_renewal_1point0_e
+		remove_country_flag = buy_influence_renewal_1point0_em
+		remove_country_flag = buy_influence_renewal_1point5_em
+		remove_country_flag = buy_influence_renewal_2point0_em
+		remove_country_flag = buy_influence_renewal_1point0_mf
+		remove_country_flag = buy_influence_renewal_1point5_mf
+		remove_country_flag = buy_influence_renewal_2point0_mf
+		remove_country_flag = buy_influence_renewal_2point0_emc
+		remove_country_flag = buy_influence_renewal_3point0_emc
+		remove_country_flag = buy_influence_renewal_4point0_emc
+		#End of generated code</v>
+      </c>
+      <c r="BI20" s="30" t="str">
+        <f>tab &amp; tab &amp; tab &amp; tab &amp; "#Generated code: Different renewal text depending on which buff has expired" &amp; newline &amp;
+CONCATENATE(BI9,BI10,BI11,BI12,BI13,BI14,BI15,BI16,BI17,BI18,BI19) &amp; newline &amp;
+tab &amp; tab &amp; tab &amp; tab &amp; "#End of generated code"</f>
+        <v xml:space="preserve">				#Generated code: Different renewal text depending on which buff has expired
+				buy_influence_renewal_0point5_e = { text = buy_influence.101.renewal_0point5_e }
+				buy_influence_renewal_1point0_e = { text = buy_influence.101.renewal_1point0_e }
+				buy_influence_renewal_1point0_em = { text = buy_influence.101.renewal_1point0_em }
+				buy_influence_renewal_1point5_em = { text = buy_influence.101.renewal_1point5_em }
+				buy_influence_renewal_2point0_em = { text = buy_influence.101.renewal_2point0_em }
+				buy_influence_renewal_1point0_mf = { text = buy_influence.101.renewal_1point0_mf }
+				buy_influence_renewal_1point5_mf = { text = buy_influence.101.renewal_1point5_mf }
+				buy_influence_renewal_2point0_mf = { text = buy_influence.101.renewal_2point0_mf }
+				buy_influence_renewal_2point0_emc = { text = buy_influence.101.renewal_2point0_emc }
+				buy_influence_renewal_3point0_emc = { text = buy_influence.101.renewal_3point0_emc }
+				buy_influence_renewal_4point0_emc = { text = buy_influence.101.renewal_4point0_emc }
+				#End of generated code</v>
+      </c>
+      <c r="BJ20" s="30" t="str">
+        <f>space &amp; "#Generated code: Renewal text contains a reminder of which buff has expired" &amp; newline &amp;
+CONCATENATE(BJ9,BJ10,BJ11,BJ12,BJ13,BJ14,BJ15,BJ16,BJ17,BJ18,BJ19)</f>
+        <v xml:space="preserve"> #Generated code: Renewal text contains a reminder of which buff has expired
+ buy_influence.101.renewal_0point5_e:0 "Expired campaign: §Y$buy_influence_0point5_e_name$§!\n\n$buy_influence.101.renewal$"
+ buy_influence.101.renewal_1point0_e:0 "Expired campaign: §Y$buy_influence_1point0_e_name$§!\n\n$buy_influence.101.renewal$"
+ buy_influence.101.renewal_1point0_em:0 "Expired campaign: §Y$buy_influence_1point0_em_name$§!\n\n$buy_influence.101.renewal$"
+ buy_influence.101.renewal_1point5_em:0 "Expired campaign: §Y$buy_influence_1point5_em_name$§!\n\n$buy_influence.101.renewal$"
+ buy_influence.101.renewal_2point0_em:0 "Expired campaign: §Y$buy_influence_2point0_em_name$§!\n\n$buy_influence.101.renewal$"
+ buy_influence.101.renewal_1point0_mf:0 "Expired campaign: §Y$buy_influence_1point0_mf_name$§!\n\n$buy_influence.101.renewal$"
+ buy_influence.101.renewal_1point5_mf:0 "Expired campaign: §Y$buy_influence_1point5_mf_name$§!\n\n$buy_influence.101.renewal$"
+ buy_influence.101.renewal_2point0_mf:0 "Expired campaign: §Y$buy_influence_2point0_mf_name$§!\n\n$buy_influence.101.renewal$"
+ buy_influence.101.renewal_2point0_emc:0 "Expired campaign: §Y$buy_influence_2point0_emc_name$§!\n\n$buy_influence.101.renewal$"
+ buy_influence.101.renewal_3point0_emc:0 "Expired campaign: §Y$buy_influence_3point0_emc_name$§!\n\n$buy_influence.101.renewal$"
+ buy_influence.101.renewal_4point0_emc:0 "Expired campaign: §Y$buy_influence_4point0_emc_name$§!\n\n$buy_influence.101.renewal$"
+</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="28">
     <mergeCell ref="AJ6:AO7"/>
     <mergeCell ref="AD6:AI7"/>
     <mergeCell ref="AA6:AC7"/>
@@ -9491,6 +10168,14 @@
     <mergeCell ref="BB6:BD6"/>
     <mergeCell ref="AP6:AU7"/>
     <mergeCell ref="AV6:BA7"/>
+    <mergeCell ref="BH6:BJ6"/>
+    <mergeCell ref="BE6:BG6"/>
+    <mergeCell ref="BG7:BG8"/>
+    <mergeCell ref="BF7:BF8"/>
+    <mergeCell ref="BE7:BE8"/>
+    <mergeCell ref="BH7:BH8"/>
+    <mergeCell ref="BI7:BI8"/>
+    <mergeCell ref="BJ7:BJ8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>